<commit_message>
add correct tolerance to ChemEcho queries
</commit_message>
<xml_diff>
--- a/assets/compendium.xlsx
+++ b/assets/compendium.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tharwood\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tharwood\Desktop\ChemEcho\fixed_queries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21F025B4-5E5C-4C3B-B345-AA1116A57B49}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{513BAA34-3A2F-4A0B-BC4D-A8EB3E7AA72D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="16125" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -575,162 +575,9 @@
     <t>Macrolides from NP-Classifier (ML-generated using ChemEcho) [Ionization mode: positive]</t>
   </si>
   <si>
-    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C2H3O2):TOLERANCEPPM=6:INTENSITYPERCENT=0.0:EXCLUDED AND MS2PROD=formula(O3P):INTENSITYPERCENT=0.00019:EXCLUDED AND MS2PROD=formula(C8H6N):INTENSITYPERCENT=0.000046:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C2H3O2):TOLERANCEPPM=6:INTENSITYPERCENT=0.0:EXCLUDED AND MS2PROD=formula(O3P):INTENSITYPERCENT=0.00019:EXCLUDED AND MS2PROD=formula(C8H6N):INTENSITYPERCENT=0.000046 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C2H3O2):TOLERANCEPPM=6:INTENSITYPERCENT=0.0:EXCLUDED AND MS2PROD=formula(O3P):INTENSITYPERCENT=0.00019 AND MS2PROD=formula(C6H5O):INTENSITYPERCENT=0.000727 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C2H3O2):TOLERANCEPPM=6:INTENSITYPERCENT=0.0 AND MS2PROD=formula(C8H5O):INTENSITYPERCENT=0.00002:EXCLUDED AND MS2PROD=formula(C7H5O2):INTENSITYPERCENT=0.000566 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C2H3O2):TOLERANCEPPM=6:INTENSITYPERCENT=0.0 AND MS2PROD=formula(C8H5O):INTENSITYPERCENT=0.00002 AND MS2PROD=formula(CHO2):INTENSITYPERCENT=0.026492:EXCLUDED</t>
-  </si>
-  <si>
-    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(O3S):TOLERANCEPPM=6:INTENSITYPERCENT=0.0:EXCLUDED AND MS2PROD=formula(HO4S):INTENSITYPERCENT=0.00163:EXCLUDED AND MS2NL=formula(O3S):INTENSITYPERCENT=0.002914 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(O3S):TOLERANCEPPM=6:INTENSITYPERCENT=0.0:EXCLUDED AND MS2PROD=formula(HO4S):INTENSITYPERCENT=0.00163 AND MS2PROD=formula(C7H11NO6S):INTENSITYPERCENT=0.001570:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(O3S):TOLERANCEPPM=6:INTENSITYPERCENT=0.0 AND MS2PROD=formula(NO2S):INTENSITYPERCENT=0.00286:EXCLUDED AND MS2PROD=formula(C6H5NO2S):INTENSITYPERCENT=0.000320:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(O3S):TOLERANCEPPM=6:INTENSITYPERCENT=0.0 AND MS2PROD=formula(NO2S):INTENSITYPERCENT=0.00286 AND MS2PROD=formula(C15H3N2O3):INTENSITYPERCENT=0.002061</t>
-  </si>
-  <si>
-    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C6H10O8P):TOLERANCEPPM=6:INTENSITYPERCENT=0.0:EXCLUDED AND MS2PROD=formula(C9O11P):INTENSITYPERCENT=0.00351:EXCLUDED AND MS2PROD=formula(C39H18O4P):INTENSITYPERCENT=0.115346 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C6H10O8P):TOLERANCEPPM=6:INTENSITYPERCENT=0.0:EXCLUDED AND MS2PROD=formula(C9O11P):INTENSITYPERCENT=0.00351 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C6H10O8P):TOLERANCEPPM=6:INTENSITYPERCENT=0.0 AND MS2PROD=formula(H2O4P):INTENSITYPERCENT=0.03440:EXCLUDED AND MS2PROD=formula(C6H11O11P2):INTENSITYPERCENT=0.000636:EXCLUDED</t>
-  </si>
-  <si>
-    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C24H33):TOLERANCEPPM=6:INTENSITYPERCENT=0.0:EXCLUDED AND MS2PROD=formula(C24H33O):INTENSITYPERCENT=0.01452:EXCLUDED AND MS2NL=formula(C23H39N2P):INTENSITYPERCENT=0.184262 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C24H33):TOLERANCEPPM=6:INTENSITYPERCENT=0.0:EXCLUDED AND MS2PROD=formula(C24H33O):INTENSITYPERCENT=0.01452 AND MS2NL=formula(C20H42N2OS2):INTENSITYPERCENT=0.008663 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C24H33):TOLERANCEPPM=6:INTENSITYPERCENT=0.0 AND MS2NL=formula(C12H22O3):INTENSITYPERCENT=0.00192:EXCLUDED AND MS2PROD=formula(C16H21O2):INTENSITYPERCENT=0.001793:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C24H33):TOLERANCEPPM=6:INTENSITYPERCENT=0.0 AND MS2NL=formula(C12H22O3):INTENSITYPERCENT=0.00192 AND MS2PROD=formula(C18H27O2):INTENSITYPERCENT=0.010528</t>
-  </si>
-  <si>
-    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C6H10NO2S):TOLERANCEPPM=6:INTENSITYPERCENT=0.0:EXCLUDED AND MS2PROD=formula(H5N5O4):INTENSITYPERCENT=0.00125:EXCLUDED AND MS2PROD=formula(C7H7N4OS2):INTENSITYPERCENT=0.000602 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C6H10NO2S):TOLERANCEPPM=6:INTENSITYPERCENT=0.0:EXCLUDED AND MS2PROD=formula(H5N5O4):INTENSITYPERCENT=0.00125 AND MS2PROD=formula(C5H6NS):INTENSITYPERCENT=0.002949 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C6H10NO2S):TOLERANCEPPM=6:INTENSITYPERCENT=0.0 AND MS2PROD=formula(C3H6N):INTENSITYPERCENT=0.00099:EXCLUDED AND MS2PROD=formula(C14H6N2):INTENSITYPERCENT=0.006564:EXCLUDED</t>
-  </si>
-  <si>
-    <t>QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(C24H38O3):TOLERANCEPPM=6:INTENSITYPERCENT=0.0:EXCLUDED AND MS2PROD=formula(C23H35O2):INTENSITYPERCENT=0.00007:EXCLUDED AND MS2NL=formula(C25H34N4):INTENSITYPERCENT=0.000982 ||| QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(C24H38O3):TOLERANCEPPM=6:INTENSITYPERCENT=0.0:EXCLUDED AND MS2PROD=formula(C23H35O2):INTENSITYPERCENT=0.00007 AND MS2PROD=formula(C22H31O3):INTENSITYPERCENT=0.000077:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(C24H38O3):TOLERANCEPPM=6:INTENSITYPERCENT=0.0 AND MS2NL=formula(C15H41N7O7):INTENSITYPERCENT=0.00051:EXCLUDED AND MS2PROD=formula(C6H13N2O2):INTENSITYPERCENT=0.880451:EXCLUDED</t>
-  </si>
-  <si>
-    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C3H6O5P):TOLERANCEPPM=6:INTENSITYPERCENT=0.0:EXCLUDED AND MS2PROD=formula(C5H11NO5P):INTENSITYPERCENT=0.00046:EXCLUDED AND MS2PROD=formula(C18H33O2):INTENSITYPERCENT=0.045027 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C3H6O5P):TOLERANCEPPM=6:INTENSITYPERCENT=0.0:EXCLUDED AND MS2PROD=formula(C5H11NO5P):INTENSITYPERCENT=0.00046 AND MS2NL=formula(C8H3N7):INTENSITYPERCENT=0.952171:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C3H6O5P):TOLERANCEPPM=6:INTENSITYPERCENT=0.0 AND MS2PROD=formula(O3P):INTENSITYPERCENT=0.46254:EXCLUDED AND MS2NL=formula(H5O5P):INTENSITYPERCENT=0.030577:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C3H6O5P):TOLERANCEPPM=6:INTENSITYPERCENT=0.0 AND MS2PROD=formula(O3P):INTENSITYPERCENT=0.46254 AND MS2PROD=formula(C6H9O10P2):INTENSITYPERCENT=0.002631</t>
-  </si>
-  <si>
-    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C7H3O4):TOLERANCEPPM=6:INTENSITYPERCENT=0.0:EXCLUDED AND MS2PROD=formula(C15H9O6):INTENSITYPERCENT=0.00831:EXCLUDED AND MS2PROD=formula(C15H8O7):INTENSITYPERCENT=0.016601 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C7H3O4):TOLERANCEPPM=6:INTENSITYPERCENT=0.0:EXCLUDED AND MS2PROD=formula(C15H9O6):INTENSITYPERCENT=0.00831 AND MS2PROD=formula(C15H9O6):INTENSITYPERCENT=0.122768:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C7H3O4):TOLERANCEPPM=6:INTENSITYPERCENT=0.0:EXCLUDED AND MS2PROD=formula(C15H9O6):INTENSITYPERCENT=0.00831 AND MS2PROD=formula(C15H9O6):INTENSITYPERCENT=0.122768 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C7H3O4):TOLERANCEPPM=6:INTENSITYPERCENT=0.0 AND MS2PROD=formula(C6H3O4):INTENSITYPERCENT=0.00099:EXCLUDED AND MS2PROD=formula(C8H6O4):INTENSITYPERCENT=0.000394:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C7H3O4):TOLERANCEPPM=6:INTENSITYPERCENT=0.0 AND MS2PROD=formula(C6H3O4):INTENSITYPERCENT=0.00099 AND MS2PROD=formula(C12H7O3):INTENSITYPERCENT=0.004171</t>
-  </si>
-  <si>
-    <t>QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(C5H8O4):TOLERANCEPPM=6:INTENSITYPERCENT=0.3:EXCLUDED AND MS2PROD=formula(C5H6N5):INTENSITYPERCENT=0.73700:EXCLUDED AND MS2NL=formula(C8H8N2OS2):INTENSITYPERCENT=0.127969 ||| QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(C5H8O4):TOLERANCEPPM=6:INTENSITYPERCENT=0.3:EXCLUDED AND MS2PROD=formula(C5H6N5):INTENSITYPERCENT=0.73700 AND MS2PROD=formula(C6H6N5):INTENSITYPERCENT=0.005699:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(C5H8O4):TOLERANCEPPM=6:INTENSITYPERCENT=0.3 AND MS2NL=formula(C5H11NO4):INTENSITYPERCENT=0.00010:EXCLUDED AND MS2NL=formula(C5H8O4):INTENSITYPERCENT=0.919773 ||| QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(C5H8O4):TOLERANCEPPM=6:INTENSITYPERCENT=0.3 AND MS2NL=formula(C5H11NO4):INTENSITYPERCENT=0.00010 AND MS2PROD=formula(C7H5N4O):INTENSITYPERCENT=0.013940:EXCLUDED</t>
-  </si>
-  <si>
-    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C6H9O5):TOLERANCEPPM=6:INTENSITYPERCENT=0.0:EXCLUDED AND MS2NL=formula(C7H14S2):INTENSITYPERCENT=0.09230:EXCLUDED AND MS2NL=formula(C13H24O4S2):INTENSITYPERCENT=0.056189 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C6H9O5):TOLERANCEPPM=6:INTENSITYPERCENT=0.0:EXCLUDED AND MS2NL=formula(C7H14S2):INTENSITYPERCENT=0.09230 AND MS2NL=formula(C3H6O3):INTENSITYPERCENT=0.008776:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C6H9O5):TOLERANCEPPM=6:INTENSITYPERCENT=0.0 AND MS2PROD=formula(C6H7O4):INTENSITYPERCENT=0.00283:EXCLUDED AND MS2PROD=formula(C9H7NO2):INTENSITYPERCENT=0.000115:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C6H9O5):TOLERANCEPPM=6:INTENSITYPERCENT=0.0 AND MS2PROD=formula(C6H7O4):INTENSITYPERCENT=0.00283 AND MS2NL=formula(C3H8O3):INTENSITYPERCENT=0.018492:EXCLUDED</t>
-  </si>
-  <si>
-    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C5H10N6O):TOLERANCEPPM=6:INTENSITYPERCENT=0.0:EXCLUDED AND MS2PROD=formula(C7H11N5O):INTENSITYPERCENT=0.00064:EXCLUDED AND MS2PROD=formula(C2H6N6O):INTENSITYPERCENT=0.004135 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C5H10N6O):TOLERANCEPPM=6:INTENSITYPERCENT=0.0:EXCLUDED AND MS2PROD=formula(C7H11N5O):INTENSITYPERCENT=0.00064 AND MS2PROD=formula(C9H13N5O2):INTENSITYPERCENT=0.001688:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C5H10N6O):TOLERANCEPPM=6:INTENSITYPERCENT=0.0 AND MS2NL=formula(C24H43N3O6P2):INTENSITYPERCENT=0.00116:EXCLUDED AND MS2PROD=formula(C8H14N5O2):INTENSITYPERCENT=0.000451:EXCLUDED</t>
-  </si>
-  <si>
-    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C3H8O5P):TOLERANCEPPM=6:INTENSITYPERCENT=0.0:EXCLUDED AND MS2PROD=formula(C3H7NaO5P):INTENSITYPERCENT=0.00039:EXCLUDED AND MS2NL=formula(C3H4N5P):INTENSITYPERCENT=0.338294 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C3H8O5P):TOLERANCEPPM=6:INTENSITYPERCENT=0.0:EXCLUDED AND MS2PROD=formula(C3H7NaO5P):INTENSITYPERCENT=0.00039 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C3H8O5P):TOLERANCEPPM=6:INTENSITYPERCENT=0.0 AND MS2NL=formula(C16H18N2O2S3):INTENSITYPERCENT=0.00453:EXCLUDED</t>
-  </si>
-  <si>
-    <t>QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(C5H8O4):TOLERANCEPPM=6:INTENSITYPERCENT=0.2:EXCLUDED AND MS2PROD=formula(C3H6N3O6P):INTENSITYPERCENT=0.01006:EXCLUDED AND MS2NL=formula(C4H7NO4):INTENSITYPERCENT=0.029269 ||| QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(C5H8O4):TOLERANCEPPM=6:INTENSITYPERCENT=0.2:EXCLUDED AND MS2PROD=formula(C3H6N3O6P):INTENSITYPERCENT=0.01006 AND MS2PROD=formula(C19H2N7O5):INTENSITYPERCENT=0.007694:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(C5H8O4):TOLERANCEPPM=6:INTENSITYPERCENT=0.2 AND MS2NL=formula(C6H9NO5):INTENSITYPERCENT=0.00124:EXCLUDED AND MS2NL=formula(C5H8O4):INTENSITYPERCENT=0.858722 ||| QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(C5H8O4):TOLERANCEPPM=6:INTENSITYPERCENT=0.2 AND MS2NL=formula(C6H9NO5):INTENSITYPERCENT=0.00124 AND MS2PROD=formula(C7H3N4O):INTENSITYPERCENT=0.196133:EXCLUDED</t>
-  </si>
-  <si>
-    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C24H35O):TOLERANCEPPM=6:INTENSITYPERCENT=0.0:EXCLUDED AND MS2PROD=formula(C24H33O):INTENSITYPERCENT=0.00958 AND MS2PROD=formula(C16H17):INTENSITYPERCENT=0.012364 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C24H35O):TOLERANCEPPM=6:INTENSITYPERCENT=0.0 AND MS2PROD=formula(C16H23):INTENSITYPERCENT=0.01395:EXCLUDED AND MS2PROD=formula(C28H42NO3):INTENSITYPERCENT=0.000191 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C24H35O):TOLERANCEPPM=6:INTENSITYPERCENT=0.0 AND MS2PROD=formula(C16H23):INTENSITYPERCENT=0.01395 AND MS2NL=formula(C22H37NO3):INTENSITYPERCENT=0.004929:EXCLUDED</t>
-  </si>
-  <si>
-    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C9H13):TOLERANCEPPM=6:INTENSITYPERCENT=0.0:EXCLUDED AND MS2PROD=formula(C7H7):INTENSITYPERCENT=0.00021:EXCLUDED AND MS2PROD=formula(C6H5):INTENSITYPERCENT=0.000258 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C9H13):TOLERANCEPPM=6:INTENSITYPERCENT=0.0:EXCLUDED AND MS2PROD=formula(C7H7):INTENSITYPERCENT=0.00021 AND MS2PROD=formula(C6H9):INTENSITYPERCENT=0.001077:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C9H13):TOLERANCEPPM=6:INTENSITYPERCENT=0.0 AND MS2PROD=formula(C9H7O2):INTENSITYPERCENT=0.00093 AND MS2PROD=formula(C12H13):INTENSITYPERCENT=0.003782:EXCLUDED</t>
-  </si>
-  <si>
-    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C9H13):TOLERANCEPPM=6:INTENSITYPERCENT=0.0:EXCLUDED AND MS2PROD=formula(C7H7):INTENSITYPERCENT=0.00008:EXCLUDED AND MS2PROD=formula(C9H8N):INTENSITYPERCENT=0.000181 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C9H13):TOLERANCEPPM=6:INTENSITYPERCENT=0.0:EXCLUDED AND MS2PROD=formula(C7H7):INTENSITYPERCENT=0.00008 AND MS2PROD=formula(C6H9):INTENSITYPERCENT=0.001348:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C9H13):TOLERANCEPPM=6:INTENSITYPERCENT=0.0 AND MS2PROD=formula(C9H7O3):INTENSITYPERCENT=0.00015:EXCLUDED AND MS2PROD=formula(C9H8N):INTENSITYPERCENT=0.001364 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C9H13):TOLERANCEPPM=6:INTENSITYPERCENT=0.0 AND MS2PROD=formula(C9H7O3):INTENSITYPERCENT=0.00015 AND MS2PROD=formula(C12H13):INTENSITYPERCENT=0.002894:EXCLUDED</t>
-  </si>
-  <si>
-    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C6H9O4):TOLERANCEPPM=6:INTENSITYPERCENT=0.1:EXCLUDED AND MS2PROD=formula(C13H22NO7):INTENSITYPERCENT=0.07694:EXCLUDED AND MS2NL=formula(C2H10O4):INTENSITYPERCENT=0.060764 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C6H9O4):TOLERANCEPPM=6:INTENSITYPERCENT=0.1:EXCLUDED AND MS2PROD=formula(C13H22NO7):INTENSITYPERCENT=0.07694 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C6H9O4):TOLERANCEPPM=6:INTENSITYPERCENT=0.1 AND MS2NL=formula(C7H16OS2):INTENSITYPERCENT=0.00063:EXCLUDED AND MS2PROD=formula(C6H7O3):INTENSITYPERCENT=0.131305 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C6H9O4):TOLERANCEPPM=6:INTENSITYPERCENT=0.1 AND MS2NL=formula(C7H16OS2):INTENSITYPERCENT=0.00063 AND MS2PROD=formula(C6H11O5):INTENSITYPERCENT=0.004699</t>
-  </si>
-  <si>
-    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C19H29O):TOLERANCEPPM=6:INTENSITYPERCENT=0.0:EXCLUDED AND MS2PROD=formula(C14H17O3):INTENSITYPERCENT=0.02106:EXCLUDED AND MS2PROD=formula(C19H29):INTENSITYPERCENT=0.050000 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C19H29O):TOLERANCEPPM=6:INTENSITYPERCENT=0.0:EXCLUDED AND MS2PROD=formula(C14H17O3):INTENSITYPERCENT=0.02106 AND MS2PROD=formula(C7H9O):INTENSITYPERCENT=0.001107 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C19H29O):TOLERANCEPPM=6:INTENSITYPERCENT=0.0 AND MS2PROD=formula(C2H3O2):INTENSITYPERCENT=0.00033:EXCLUDED AND MS2PROD=formula(C14H19O3):INTENSITYPERCENT=0.004220 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C19H29O):TOLERANCEPPM=6:INTENSITYPERCENT=0.0 AND MS2PROD=formula(C2H3O2):INTENSITYPERCENT=0.00033 AND MS2NL=formula(C4N4):INTENSITYPERCENT=0.007086:EXCLUDED</t>
-  </si>
-  <si>
-    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C30H47O3):TOLERANCEPPM=6:INTENSITYPERCENT=0.0:EXCLUDED AND MS2PROD=formula(C28H41O):INTENSITYPERCENT=0.00026:EXCLUDED AND MS2PROD=formula(C35H55O7):INTENSITYPERCENT=0.008906 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C30H47O3):TOLERANCEPPM=6:INTENSITYPERCENT=0.0:EXCLUDED AND MS2PROD=formula(C28H41O):INTENSITYPERCENT=0.00026 AND MS2PROD=formula(C28H43O):INTENSITYPERCENT=0.004046:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C30H47O3):TOLERANCEPPM=6:INTENSITYPERCENT=0.0 AND MS2NL=formula(C39H39O6PS):INTENSITYPERCENT=0.00009:EXCLUDED AND MS2PROD=formula(C30H47O3):INTENSITYPERCENT=0.996306:EXCLUDED</t>
-  </si>
-  <si>
-    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C23H24O7):TOLERANCEPPM=6:INTENSITYPERCENT=0.1:EXCLUDED AND MS2PROD=formula(C13H5Cl2O4):INTENSITYPERCENT=0.01738:EXCLUDED AND MS2PROD=formula(C13H6O5):INTENSITYPERCENT=0.385088 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C23H24O7):TOLERANCEPPM=6:INTENSITYPERCENT=0.1:EXCLUDED AND MS2PROD=formula(C13H5Cl2O4):INTENSITYPERCENT=0.01738 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C23H24O7):TOLERANCEPPM=6:INTENSITYPERCENT=0.1</t>
-  </si>
-  <si>
-    <t>QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(C2H8O3):TOLERANCEPPM=6:INTENSITYPERCENT=0.1:EXCLUDED AND MS2PROD=formula(C12H21O11):INTENSITYPERCENT=0.02284:EXCLUDED AND MS2NL=formula(CH17N4O7P):INTENSITYPERCENT=0.019822 ||| QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(C2H8O3):TOLERANCEPPM=6:INTENSITYPERCENT=0.1:EXCLUDED AND MS2PROD=formula(C12H21O11):INTENSITYPERCENT=0.02284 AND MS2PROD=formula(C12H19O10):INTENSITYPERCENT=0.023576:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(C2H8O3):TOLERANCEPPM=6:INTENSITYPERCENT=0.1 AND MS2PROD=formula(C3H5O3):INTENSITYPERCENT=0.04271:EXCLUDED AND MS2PROD=formula(C4H5O3):INTENSITYPERCENT=0.135896 ||| QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(C2H8O3):TOLERANCEPPM=6:INTENSITYPERCENT=0.1 AND MS2PROD=formula(C3H5O3):INTENSITYPERCENT=0.04271 AND MS2PROD=formula(C4H6NO):INTENSITYPERCENT=0.001751:EXCLUDED</t>
-  </si>
-  <si>
-    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C9H8N):TOLERANCEPPM=6:INTENSITYPERCENT=0.7:EXCLUDED AND MS2PROD=formula(C10H11N2):INTENSITYPERCENT=0.01843 AND MS2PROD=formula(C11H10NO2):INTENSITYPERCENT=0.001119 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C9H8N):TOLERANCEPPM=6:INTENSITYPERCENT=0.7 AND MS2NL=formula(C2H7N):INTENSITYPERCENT=0.41267:EXCLUDED AND MS2PROD=formula(C8H7):INTENSITYPERCENT=0.015723 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C9H8N):TOLERANCEPPM=6:INTENSITYPERCENT=0.7 AND MS2NL=formula(C2H7N):INTENSITYPERCENT=0.41267</t>
-  </si>
-  <si>
-    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C25H40NO3):TOLERANCEPPM=6:INTENSITYPERCENT=0.0:EXCLUDED AND MS2NL=formula(C24H38O3):INTENSITYPERCENT=0.01814:EXCLUDED AND MS2NL=formula(C24H38O4):INTENSITYPERCENT=0.024398 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C25H40NO3):TOLERANCEPPM=6:INTENSITYPERCENT=0.0:EXCLUDED AND MS2NL=formula(C24H38O3):INTENSITYPERCENT=0.01814 AND MS2PROD=formula(C24H37O3):INTENSITYPERCENT=0.487587:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C25H40NO3):TOLERANCEPPM=6:INTENSITYPERCENT=0.0</t>
-  </si>
-  <si>
-    <t>QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(CH2O3):TOLERANCEPPM=6:INTENSITYPERCENT=0.3:EXCLUDED AND MS2PROD=formula(C5H9O):INTENSITYPERCENT=0.20356:EXCLUDED AND MS2PROD=formula(C4H7O2):INTENSITYPERCENT=0.796387 ||| QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(CH2O3):TOLERANCEPPM=6:INTENSITYPERCENT=0.3:EXCLUDED AND MS2PROD=formula(C5H9O):INTENSITYPERCENT=0.20356 AND MS2NL=formula(C39H62N6O12):INTENSITYPERCENT=0.013345:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(CH2O3):TOLERANCEPPM=6:INTENSITYPERCENT=0.3 AND MS2NL=formula(CH4O4):INTENSITYPERCENT=0.00048:EXCLUDED AND MS2PROD=formula(C3H5O):INTENSITYPERCENT=0.003108:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(CH2O3):TOLERANCEPPM=6:INTENSITYPERCENT=0.3 AND MS2NL=formula(CH4O4):INTENSITYPERCENT=0.00048:EXCLUDED AND MS2PROD=formula(C3H5O):INTENSITYPERCENT=0.003108 ||| QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(CH2O3):TOLERANCEPPM=6:INTENSITYPERCENT=0.3 AND MS2NL=formula(CH4O4):INTENSITYPERCENT=0.00048 AND MS2NL=formula(C3H4O4):INTENSITYPERCENT=0.081803</t>
-  </si>
-  <si>
-    <t>QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(C24H38O3):TOLERANCEPPM=6:INTENSITYPERCENT=0.0:EXCLUDED AND MS2PROD=formula(C23H37O2):INTENSITYPERCENT=0.05712:EXCLUDED AND MS2PROD=formula(C23H39O3):INTENSITYPERCENT=0.003521 ||| QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(C24H38O3):TOLERANCEPPM=6:INTENSITYPERCENT=0.0:EXCLUDED AND MS2PROD=formula(C23H37O2):INTENSITYPERCENT=0.05712 AND MS2PROD=formula(C24H35O3):INTENSITYPERCENT=0.042916:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(C24H38O3):TOLERANCEPPM=6:INTENSITYPERCENT=0.0 AND MS2PROD=formula(C4H6NO):INTENSITYPERCENT=0.00165:EXCLUDED AND MS2PROD=formula(C23H35O2):INTENSITYPERCENT=0.000119 ||| QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(C24H38O3):TOLERANCEPPM=6:INTENSITYPERCENT=0.0 AND MS2PROD=formula(C4H6NO):INTENSITYPERCENT=0.00165</t>
-  </si>
-  <si>
-    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C14H7O3):TOLERANCEPPM=6:INTENSITYPERCENT=0.0:EXCLUDED AND MS2PROD=formula(C15H8O5):INTENSITYPERCENT=0.02743:EXCLUDED AND MS2PROD=formula(C24H21O5):INTENSITYPERCENT=0.014475 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C14H7O3):TOLERANCEPPM=6:INTENSITYPERCENT=0.0:EXCLUDED AND MS2PROD=formula(C15H8O5):INTENSITYPERCENT=0.02743 AND MS2PROD=formula(C8H4O2):INTENSITYPERCENT=0.002826 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C14H7O3):TOLERANCEPPM=6:INTENSITYPERCENT=0.0 AND MS2PROD=formula(C8H4O2):INTENSITYPERCENT=0.00132:EXCLUDED AND MS2NL=formula(C4H8):INTENSITYPERCENT=0.003422 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C14H7O3):TOLERANCEPPM=6:INTENSITYPERCENT=0.0 AND MS2PROD=formula(C8H4O2):INTENSITYPERCENT=0.00132 AND MS2PROD=formula(C8H5O):INTENSITYPERCENT=0.038652:EXCLUDED</t>
-  </si>
-  <si>
-    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C5H8N3):TOLERANCEPPM=6:INTENSITYPERCENT=0.3:EXCLUDED AND MS2PROD=formula(C5H10N3):INTENSITYPERCENT=0.31455 AND MS2PROD=formula(C5H7N2):INTENSITYPERCENT=0.012994 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C5H8N3):TOLERANCEPPM=6:INTENSITYPERCENT=0.3 AND MS2PROD=formula(C7H12N3):INTENSITYPERCENT=0.03098:EXCLUDED AND MS2PROD=formula(C4H7N2):INTENSITYPERCENT=0.003077:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C5H8N3):TOLERANCEPPM=6:INTENSITYPERCENT=0.3 AND MS2PROD=formula(C7H12N3):INTENSITYPERCENT=0.03098:EXCLUDED AND MS2PROD=formula(C4H7N2):INTENSITYPERCENT=0.003077</t>
-  </si>
-  <si>
-    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C20H27O):TOLERANCEPPM=6:INTENSITYPERCENT=0.0:EXCLUDED AND MS2PROD=formula(C10H19F2O3):INTENSITYPERCENT=0.01270:EXCLUDED AND MS2PROD=formula(C22H35O3):INTENSITYPERCENT=0.006115 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C20H27O):TOLERANCEPPM=6:INTENSITYPERCENT=0.0:EXCLUDED AND MS2PROD=formula(C10H19F2O3):INTENSITYPERCENT=0.01270 AND MS2PROD=formula(C17H15F):INTENSITYPERCENT=0.000012:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C20H27O):TOLERANCEPPM=6:INTENSITYPERCENT=0.0 AND MS2PROD=formula(C5H11):INTENSITYPERCENT=0.00046:EXCLUDED AND MS2NL=formula(C7H18O2):INTENSITYPERCENT=0.000944 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C20H27O):TOLERANCEPPM=6:INTENSITYPERCENT=0.0 AND MS2PROD=formula(C5H11):INTENSITYPERCENT=0.00046 AND MS2PROD=formula(C17H21):INTENSITYPERCENT=0.000489:EXCLUDED</t>
-  </si>
-  <si>
-    <t>QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(C16H42N2O5S):TOLERANCEPPM=6:INTENSITYPERCENT=0.0:EXCLUDED AND MS2NL=formula(C16H42N2O6S):INTENSITYPERCENT=0.00811:EXCLUDED AND MS2PROD=formula(C23H35O2):INTENSITYPERCENT=0.019021 ||| QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(C16H42N2O5S):TOLERANCEPPM=6:INTENSITYPERCENT=0.0:EXCLUDED AND MS2NL=formula(C16H42N2O6S):INTENSITYPERCENT=0.00811 AND MS2NL=formula(C13H24N3O3):INTENSITYPERCENT=0.004777:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(C16H42N2O5S):TOLERANCEPPM=6:INTENSITYPERCENT=0.0 AND MS2NL=formula(C25H40N3O2):INTENSITYPERCENT=0.06889:EXCLUDED AND MS2NL=formula(C15H35N9S):INTENSITYPERCENT=0.109837:EXCLUDED</t>
-  </si>
-  <si>
-    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C29H43O3):TOLERANCEPPM=6:INTENSITYPERCENT=0.0:EXCLUDED AND MS2PROD=formula(C30H47O3):INTENSITYPERCENT=0.00001:EXCLUDED AND MS2PROD=formula(C30H47O4):INTENSITYPERCENT=0.000190 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C29H43O3):TOLERANCEPPM=6:INTENSITYPERCENT=0.0:EXCLUDED AND MS2PROD=formula(C30H47O3):INTENSITYPERCENT=0.00001 AND MS2NL=formula(C27H43N3O3S):INTENSITYPERCENT=0.000096:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C29H43O3):TOLERANCEPPM=6:INTENSITYPERCENT=0.0 AND MS2PROD=formula(C24H38NO2):INTENSITYPERCENT=0.00044:EXCLUDED AND MS2NL=formula(C9H18N6O9):INTENSITYPERCENT=0.006425:EXCLUDED</t>
-  </si>
-  <si>
-    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C23H21O6):TOLERANCEPPM=6:INTENSITYPERCENT=0.0:EXCLUDED AND MS2PROD=formula(C23H24O7):INTENSITYPERCENT=0.03636:EXCLUDED AND MS2PROD=formula(C13H6O5):INTENSITYPERCENT=0.393985 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C23H21O6):TOLERANCEPPM=6:INTENSITYPERCENT=0.0:EXCLUDED AND MS2PROD=formula(C23H24O7):INTENSITYPERCENT=0.03636 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C23H21O6):TOLERANCEPPM=6:INTENSITYPERCENT=0.0 AND MS2PROD=formula(C19H15O6):INTENSITYPERCENT=0.00131:EXCLUDED AND MS2PROD=formula(C19H13O6):INTENSITYPERCENT=0.008984 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C23H21O6):TOLERANCEPPM=6:INTENSITYPERCENT=0.0 AND MS2PROD=formula(C19H15O6):INTENSITYPERCENT=0.00131</t>
-  </si>
-  <si>
-    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C14H23O5):TOLERANCEPPM=6:INTENSITYPERCENT=0.0:EXCLUDED AND MS2PROD=formula(C22H40N):INTENSITYPERCENT=0.01263:EXCLUDED AND MS2PROD=formula(C18H31O8):INTENSITYPERCENT=0.009209 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C14H23O5):TOLERANCEPPM=6:INTENSITYPERCENT=0.0:EXCLUDED AND MS2PROD=formula(C22H40N):INTENSITYPERCENT=0.01263 AND MS2PROD=formula(C22H40N):INTENSITYPERCENT=0.342627:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C14H23O5):TOLERANCEPPM=6:INTENSITYPERCENT=0.0 AND MS2PROD=formula(C8H13O3):INTENSITYPERCENT=0.04663</t>
-  </si>
-  <si>
-    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C24H33):TOLERANCEPPM=6:INTENSITYPERCENT=0.0:EXCLUDED AND MS2PROD=formula(C24H33O):INTENSITYPERCENT=0.01497:EXCLUDED AND MS2PROD=formula(C8H7O7):INTENSITYPERCENT=0.162655 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C24H33):TOLERANCEPPM=6:INTENSITYPERCENT=0.0:EXCLUDED AND MS2PROD=formula(C24H33O):INTENSITYPERCENT=0.01497 AND MS2PROD=formula(C10H13O):INTENSITYPERCENT=0.005582:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C24H33):TOLERANCEPPM=6:INTENSITYPERCENT=0.0 AND MS2PROD=formula(C12H15):INTENSITYPERCENT=0.02879:EXCLUDED AND MS2NL=formula(C8H14O2):INTENSITYPERCENT=0.004970:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C24H33):TOLERANCEPPM=6:INTENSITYPERCENT=0.0 AND MS2PROD=formula(C12H15):INTENSITYPERCENT=0.02879 AND MS2PROD=formula(C14H19O):INTENSITYPERCENT=0.002210:EXCLUDED</t>
-  </si>
-  <si>
-    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C24H12O6S):TOLERANCEPPM=6:INTENSITYPERCENT=0.0:EXCLUDED AND MS2PROD=formula(C11H19O):INTENSITYPERCENT=0.01581:EXCLUDED AND MS2PROD=formula(C4H3O3):INTENSITYPERCENT=0.378989 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C24H12O6S):TOLERANCEPPM=6:INTENSITYPERCENT=0.0:EXCLUDED AND MS2PROD=formula(C11H19O):INTENSITYPERCENT=0.01581 AND MS2PROD=formula(C8H11):INTENSITYPERCENT=0.000777:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C24H12O6S):TOLERANCEPPM=6:INTENSITYPERCENT=0.0 AND MS2PROD=formula(C31H40N6):INTENSITYPERCENT=0.00107:EXCLUDED AND MS2PROD=formula(C11H17N4O10P3S):INTENSITYPERCENT=0.000424:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C24H12O6S):TOLERANCEPPM=6:INTENSITYPERCENT=0.0 AND MS2PROD=formula(C31H40N6):INTENSITYPERCENT=0.00107:EXCLUDED AND MS2PROD=formula(C11H17N4O10P3S):INTENSITYPERCENT=0.000424</t>
-  </si>
-  <si>
-    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C24H35O):TOLERANCEPPM=6:INTENSITYPERCENT=0.0:EXCLUDED AND MS2PROD=formula(C24H33O):INTENSITYPERCENT=0.00228 AND MS2PROD=formula(C24H33O):INTENSITYPERCENT=0.016520:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C24H35O):TOLERANCEPPM=6:INTENSITYPERCENT=0.0:EXCLUDED AND MS2PROD=formula(C24H33O):INTENSITYPERCENT=0.00228 AND MS2PROD=formula(C24H33O):INTENSITYPERCENT=0.016520 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C24H35O):TOLERANCEPPM=6:INTENSITYPERCENT=0.0 AND MS2PROD=formula(C26H37O):INTENSITYPERCENT=0.00069:EXCLUDED AND MS2PROD=formula(C24H33):INTENSITYPERCENT=0.001553:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C24H35O):TOLERANCEPPM=6:INTENSITYPERCENT=0.0 AND MS2PROD=formula(C26H37O):INTENSITYPERCENT=0.00069:EXCLUDED AND MS2PROD=formula(C24H33):INTENSITYPERCENT=0.001553 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C24H35O):TOLERANCEPPM=6:INTENSITYPERCENT=0.0 AND MS2PROD=formula(C26H37O):INTENSITYPERCENT=0.00069 AND MS2PROD=formula(C22H29O):INTENSITYPERCENT=0.004287</t>
-  </si>
-  <si>
-    <t>QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(C22H37N2O4P):TOLERANCEPPM=6:INTENSITYPERCENT=0.1:EXCLUDED AND MS2PROD=formula(C8H10NO3):INTENSITYPERCENT=0.03386:EXCLUDED AND MS2PROD=formula(C11H17O5):INTENSITYPERCENT=0.072294 ||| QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(C22H37N2O4P):TOLERANCEPPM=6:INTENSITYPERCENT=0.1:EXCLUDED AND MS2PROD=formula(C8H10NO3):INTENSITYPERCENT=0.03386 AND MS2PROD=formula(C8H9NO3):INTENSITYPERCENT=0.095392 ||| QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(C22H37N2O4P):TOLERANCEPPM=6:INTENSITYPERCENT=0.1 AND MS2PROD=formula(C10H7NO):INTENSITYPERCENT=0.06490:EXCLUDED</t>
-  </si>
-  <si>
-    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C6H11O3):TOLERANCEPPM=6:INTENSITYPERCENT=0.1:EXCLUDED AND MS2NL=formula(C25H45N11O3):INTENSITYPERCENT=0.09116:EXCLUDED AND MS2PROD=formula(C18H29O6):INTENSITYPERCENT=0.296343 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C6H11O3):TOLERANCEPPM=6:INTENSITYPERCENT=0.1:EXCLUDED AND MS2NL=formula(C25H45N11O3):INTENSITYPERCENT=0.09116 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C6H11O3):TOLERANCEPPM=6:INTENSITYPERCENT=0.1 AND MS2NL=formula(C59H56O):INTENSITYPERCENT=0.00145:EXCLUDED AND MS2PROD=formula(C4H9N3O2):INTENSITYPERCENT=0.156155:EXCLUDED</t>
-  </si>
-  <si>
-    <t>QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(C9H21N4O8P):TOLERANCEPPM=6:INTENSITYPERCENT=0.0:EXCLUDED AND MS2PROD=formula(C6H11O6):INTENSITYPERCENT=0.00010 AND MS2PROD=formula(C9H7O3):INTENSITYPERCENT=0.002123 ||| QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(C9H21N4O8P):TOLERANCEPPM=6:INTENSITYPERCENT=0.0 AND MS2NL=formula(C14H17N2PS):INTENSITYPERCENT=0.00597:EXCLUDED AND MS2PROD=formula(C4H7O4):INTENSITYPERCENT=0.013345 ||| QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(C9H21N4O8P):TOLERANCEPPM=6:INTENSITYPERCENT=0.0 AND MS2NL=formula(C14H17N2PS):INTENSITYPERCENT=0.00597 AND MS2NL=formula(C9H23N4O6P):INTENSITYPERCENT=0.000637:EXCLUDED</t>
-  </si>
-  <si>
-    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C14H11O3):TOLERANCEPPM=6:INTENSITYPERCENT=0.4:EXCLUDED AND MS2PROD=formula(C12H9O2):INTENSITYPERCENT=0.25447:EXCLUDED AND MS2PROD=formula(C30H25O6):INTENSITYPERCENT=0.007034 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C14H11O3):TOLERANCEPPM=6:INTENSITYPERCENT=0.4:EXCLUDED AND MS2PROD=formula(C12H9O2):INTENSITYPERCENT=0.25447 AND MS2PROD=formula(C13H11O):INTENSITYPERCENT=0.045496 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C14H11O3):TOLERANCEPPM=6:INTENSITYPERCENT=0.4 AND MS2PROD=formula(C12H9O2):INTENSITYPERCENT=0.00047:EXCLUDED AND MS2PROD=formula(C14H11O3):INTENSITYPERCENT=0.907702 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C14H11O3):TOLERANCEPPM=6:INTENSITYPERCENT=0.4 AND MS2PROD=formula(C12H9O2):INTENSITYPERCENT=0.00047</t>
-  </si>
-  <si>
-    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C20H21O6):TOLERANCEPPM=6:INTENSITYPERCENT=0.1:EXCLUDED AND MS2PROD=formula(C24H19O8):INTENSITYPERCENT=0.00336:EXCLUDED AND MS2PROD=formula(C22H25O8):INTENSITYPERCENT=0.005552 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C20H21O6):TOLERANCEPPM=6:INTENSITYPERCENT=0.1:EXCLUDED AND MS2PROD=formula(C24H19O8):INTENSITYPERCENT=0.00336 AND MS2PROD=formula(C12H5N4O3):INTENSITYPERCENT=0.005004:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C20H21O6):TOLERANCEPPM=6:INTENSITYPERCENT=0.1 AND MS2PROD=formula(C11H13O4):INTENSITYPERCENT=0.05508:EXCLUDED</t>
-  </si>
-  <si>
-    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C10H18N4O):TOLERANCEPPM=6:INTENSITYPERCENT=0.0:EXCLUDED AND MS2PROD=formula(C11H20N6O2):INTENSITYPERCENT=0.00002:EXCLUDED AND MS2PROD=formula(C9H17N5O):INTENSITYPERCENT=0.001586 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C10H18N4O):TOLERANCEPPM=6:INTENSITYPERCENT=0.0:EXCLUDED AND MS2PROD=formula(C11H20N6O2):INTENSITYPERCENT=0.00002 AND MS2PROD=formula(C3H6N):INTENSITYPERCENT=0.000388:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C10H18N4O):TOLERANCEPPM=6:INTENSITYPERCENT=0.0 AND MS2PROD=formula(C6H11):INTENSITYPERCENT=0.00503:EXCLUDED AND MS2PROD=formula(C12H17O2):INTENSITYPERCENT=0.002559:EXCLUDED</t>
-  </si>
-  <si>
-    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C4H4N3):TOLERANCEPPM=6:INTENSITYPERCENT=0.0:EXCLUDED AND MS2PROD=formula(C9H13):INTENSITYPERCENT=0.00000:EXCLUDED AND MS2PROD=formula(C5H6N5):INTENSITYPERCENT=0.000052 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C4H4N3):TOLERANCEPPM=6:INTENSITYPERCENT=0.0:EXCLUDED AND MS2PROD=formula(C9H13):INTENSITYPERCENT=0.00000 AND MS2PROD=formula(C4H5N2O2):INTENSITYPERCENT=0.000062 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C4H4N3):TOLERANCEPPM=6:INTENSITYPERCENT=0.0 AND MS2PROD=formula(C5H9N2O):INTENSITYPERCENT=0.03352:EXCLUDED AND MS2PROD=formula(C7H7OS):INTENSITYPERCENT=0.000250:EXCLUDED</t>
-  </si>
-  <si>
-    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C6H9O4):TOLERANCEPPM=6:INTENSITYPERCENT=0.0:EXCLUDED AND MS2NL=formula(C6H10O5):INTENSITYPERCENT=0.09856 AND MS2PROD=formula(C13H15O):INTENSITYPERCENT=0.000355:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C6H9O4):TOLERANCEPPM=6:INTENSITYPERCENT=0.0 AND MS2PROD=formula(C4H5O2):INTENSITYPERCENT=0.00331:EXCLUDED AND MS2PROD=formula(C6H11O5):INTENSITYPERCENT=0.000298 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C6H9O4):TOLERANCEPPM=6:INTENSITYPERCENT=0.0 AND MS2PROD=formula(C4H5O2):INTENSITYPERCENT=0.00331 AND MS2NL=formula(CH6O4):INTENSITYPERCENT=0.000486:EXCLUDED</t>
-  </si>
-  <si>
-    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C9H14NO2S):TOLERANCEPPM=6:INTENSITYPERCENT=0.0:EXCLUDED AND MS2PROD=formula(C6H4N4OS):INTENSITYPERCENT=0.59832:EXCLUDED AND MS2PROD=formula(C21H15ClFN3O):INTENSITYPERCENT=0.013215 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C9H14NO2S):TOLERANCEPPM=6:INTENSITYPERCENT=0.0:EXCLUDED AND MS2PROD=formula(C6H4N4OS):INTENSITYPERCENT=0.59832 AND MS2PROD=formula(C6H5N4OS):INTENSITYPERCENT=0.079913 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C9H14NO2S):TOLERANCEPPM=6:INTENSITYPERCENT=0.0 AND MS2PROD=formula(C9H12NO2):INTENSITYPERCENT=0.39123:EXCLUDED</t>
-  </si>
-  <si>
-    <t>QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(C18H17N7O7S):TOLERANCEPPM=6:INTENSITYPERCENT=0.1:EXCLUDED AND MS2PROD=formula(C11H6O4):INTENSITYPERCENT=0.48988:EXCLUDED AND MS2NL=formula(C8H5F4OP):INTENSITYPERCENT=0.057326 ||| QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(C18H17N7O7S):TOLERANCEPPM=6:INTENSITYPERCENT=0.1:EXCLUDED AND MS2PROD=formula(C11H6O4):INTENSITYPERCENT=0.48988 ||| QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(C18H17N7O7S):TOLERANCEPPM=6:INTENSITYPERCENT=0.1</t>
-  </si>
-  <si>
-    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C2H4NO2):TOLERANCEPPM=6:INTENSITYPERCENT=0.0:EXCLUDED AND MS2NL=formula(CH3NO2):INTENSITYPERCENT=0.00022 AND MS2NL=formula(CH3NO2):INTENSITYPERCENT=0.034983 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C2H4NO2):TOLERANCEPPM=6:INTENSITYPERCENT=0.0 AND MS2NL=formula(CO2):INTENSITYPERCENT=0.00022:EXCLUDED AND MS2NL=formula(C3H5NO2):INTENSITYPERCENT=0.000605 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C2H4NO2):TOLERANCEPPM=6:INTENSITYPERCENT=0.0 AND MS2NL=formula(CO2):INTENSITYPERCENT=0.00022 AND MS2PROD=formula(C9H14NO2):INTENSITYPERCENT=0.011885:EXCLUDED</t>
-  </si>
-  <si>
-    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C10H6O5):TOLERANCEPPM=6:INTENSITYPERCENT=0.0:EXCLUDED AND MS2PROD=formula(C12H11O3):INTENSITYPERCENT=0.51892:EXCLUDED AND MS2PROD=formula(C9H4O4):INTENSITYPERCENT=0.071486 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C10H6O5):TOLERANCEPPM=6:INTENSITYPERCENT=0.0:EXCLUDED AND MS2PROD=formula(C12H11O3):INTENSITYPERCENT=0.51892 AND MS2NL=formula(C4H16N2O5S):INTENSITYPERCENT=0.113233:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C10H6O5):TOLERANCEPPM=6:INTENSITYPERCENT=0.0 AND MS2PROD=formula(C9H3O5):INTENSITYPERCENT=0.00098:EXCLUDED AND MS2PROD=formula(C9H4O5):INTENSITYPERCENT=0.000303 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C10H6O5):TOLERANCEPPM=6:INTENSITYPERCENT=0.0 AND MS2PROD=formula(C9H3O5):INTENSITYPERCENT=0.00098 AND MS2PROD=formula(C9H3O6):INTENSITYPERCENT=0.000276:EXCLUDED</t>
-  </si>
-  <si>
-    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C3HO2):TOLERANCEPPM=6:INTENSITYPERCENT=1.0:EXCLUDED AND MS2PROD=formula(C11HO):INTENSITYPERCENT=0.10380 AND MS2PROD=formula(C11HO):INTENSITYPERCENT=0.639490:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C3HO2):TOLERANCEPPM=6:INTENSITYPERCENT=1.0 AND MS2PROD=formula(C3H3O2):INTENSITYPERCENT=0.00474:EXCLUDED AND MS2NL=formula(C24H16N2O3):INTENSITYPERCENT=0.500000:EXCLUDED</t>
-  </si>
-  <si>
-    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C7H11O6):TOLERANCEPPM=6:INTENSITYPERCENT=0.1:EXCLUDED AND MS2NL=formula(C12H8N10S):INTENSITYPERCENT=0.03033 AND MS2PROD=formula(C9H7O4):INTENSITYPERCENT=0.009130 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C7H11O6):TOLERANCEPPM=6:INTENSITYPERCENT=0.1 AND MS2NL=formula(C2H6N6OS):INTENSITYPERCENT=0.00757:EXCLUDED AND MS2NL=formula(C20H20O2P2):INTENSITYPERCENT=0.002460 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C7H11O6):TOLERANCEPPM=6:INTENSITYPERCENT=0.1 AND MS2NL=formula(C2H6N6OS):INTENSITYPERCENT=0.00757</t>
-  </si>
-  <si>
-    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C8H16NO2):TOLERANCEPPM=6:INTENSITYPERCENT=0.1:EXCLUDED AND MS2PROD=formula(C8H16NO3):INTENSITYPERCENT=0.03454:EXCLUDED AND MS2NL=formula(C17H40N6S3):INTENSITYPERCENT=0.011652 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C8H16NO2):TOLERANCEPPM=6:INTENSITYPERCENT=0.1:EXCLUDED AND MS2PROD=formula(C8H16NO3):INTENSITYPERCENT=0.03454 AND MS2PROD=formula(C5H10NO2):INTENSITYPERCENT=0.007872 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C8H16NO2):TOLERANCEPPM=6:INTENSITYPERCENT=0.1 AND MS2PROD=formula(C6H14NO):INTENSITYPERCENT=0.00088:EXCLUDED AND MS2NL=formula(C49H52N4O2):INTENSITYPERCENT=0.087956 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C8H16NO2):TOLERANCEPPM=6:INTENSITYPERCENT=0.1 AND MS2PROD=formula(C6H14NO):INTENSITYPERCENT=0.00088 AND MS2NL=formula(C4H8):INTENSITYPERCENT=0.005326:EXCLUDED</t>
-  </si>
-  <si>
     <t>Thomas Harwood and Ben Bowen</t>
   </si>
   <si>
-    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C3F7):TOLERANCEPPM=6:INTENSITYPERCENT=0.0:EXCLUDED AND MS2PROD=formula(C2H3O2):INTENSITYPERCENT=0.00001:EXCLUDED AND MS2PROD=formula(C2F5):INTENSITYPERCENT=0.000752 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C3F7):TOLERANCEPPM=6:INTENSITYPERCENT=0.0 AND MS2NL=formula(CH5F2O4P):INTENSITYPERCENT=0.07685:EXCLUDED AND MS2PROD=formula(C12H11F3O2):INTENSITYPERCENT=0.015713:EXCLUDED</t>
-  </si>
-  <si>
     <t>Perfluoroalkyl and Polyfluoroalkyl Substances (FCC(F)F substructure) (ML-generated using ChemEcho) [Ionization mode: negative]</t>
   </si>
   <si>
@@ -840,6 +687,159 @@
   </si>
   <si>
     <t>FCC(F)F</t>
+  </si>
+  <si>
+    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C3F7):TOLERANCEPPM=10:INTENSITYPERCENT=0.001762:EXCLUDED AND MS2PROD=formula(C2H3O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.000012:EXCLUDED AND MS2PROD=formula(C2F5):TOLERANCEPPM=10:INTENSITYPERCENT=0.000752 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C3F7):TOLERANCEPPM=10:INTENSITYPERCENT=0.001762 AND MS2NL=formula(CH5F2O4P):TOLERANCEPPM=10:INTENSITYPERCENT=0.076847:EXCLUDED AND MS2PROD=formula(C12H11F3O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.015713:EXCLUDED</t>
+  </si>
+  <si>
+    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C2H3O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.003175:EXCLUDED AND MS2PROD=formula(O3P):TOLERANCEPPM=10:INTENSITYPERCENT=0.000194:EXCLUDED AND MS2PROD=formula(C8H6N):TOLERANCEPPM=10:INTENSITYPERCENT=0.000046:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C2H3O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.003175:EXCLUDED AND MS2PROD=formula(O3P):TOLERANCEPPM=10:INTENSITYPERCENT=0.000194:EXCLUDED AND MS2PROD=formula(C8H6N):TOLERANCEPPM=10:INTENSITYPERCENT=0.000046 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C2H3O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.003175:EXCLUDED AND MS2PROD=formula(O3P):TOLERANCEPPM=10:INTENSITYPERCENT=0.000194 AND MS2PROD=formula(C6H5O):TOLERANCEPPM=10:INTENSITYPERCENT=0.000727 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C2H3O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.003175 AND MS2PROD=formula(C8H5O):TOLERANCEPPM=10:INTENSITYPERCENT=0.000020:EXCLUDED AND MS2PROD=formula(C7H5O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.000566 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C2H3O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.003175 AND MS2PROD=formula(C8H5O):TOLERANCEPPM=10:INTENSITYPERCENT=0.000020 AND MS2PROD=formula(CHO2):TOLERANCEPPM=10:INTENSITYPERCENT=0.026492:EXCLUDED</t>
+  </si>
+  <si>
+    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(O3S):TOLERANCEPPM=10:INTENSITYPERCENT=0.000811:EXCLUDED AND MS2PROD=formula(HO4S):TOLERANCEPPM=10:INTENSITYPERCENT=0.001632:EXCLUDED AND MS2NL=formula(O3S):TOLERANCEPPM=10:INTENSITYPERCENT=0.002914 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(O3S):TOLERANCEPPM=10:INTENSITYPERCENT=0.000811:EXCLUDED AND MS2PROD=formula(HO4S):TOLERANCEPPM=10:INTENSITYPERCENT=0.001632 AND MS2PROD=formula(C7H11NO6S):TOLERANCEPPM=10:INTENSITYPERCENT=0.001570:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(O3S):TOLERANCEPPM=10:INTENSITYPERCENT=0.000811 AND MS2PROD=formula(NO2S):TOLERANCEPPM=10:INTENSITYPERCENT=0.002864:EXCLUDED AND MS2PROD=formula(C6H5NO2S):TOLERANCEPPM=10:INTENSITYPERCENT=0.000320:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(O3S):TOLERANCEPPM=10:INTENSITYPERCENT=0.000811 AND MS2PROD=formula(NO2S):TOLERANCEPPM=10:INTENSITYPERCENT=0.002864 AND MS2PROD=formula(C15H3N2O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.002061</t>
+  </si>
+  <si>
+    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C6H10O8P):TOLERANCEPPM=10:INTENSITYPERCENT=0.009138:EXCLUDED AND MS2PROD=formula(C9O11P):TOLERANCEPPM=10:INTENSITYPERCENT=0.003507:EXCLUDED AND MS2PROD=formula(C39H18O4P):TOLERANCEPPM=10:INTENSITYPERCENT=0.115346 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C6H10O8P):TOLERANCEPPM=10:INTENSITYPERCENT=0.009138:EXCLUDED AND MS2PROD=formula(C9O11P):TOLERANCEPPM=10:INTENSITYPERCENT=0.003507 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C6H10O8P):TOLERANCEPPM=10:INTENSITYPERCENT=0.009138 AND MS2PROD=formula(H2O4P):TOLERANCEPPM=10:INTENSITYPERCENT=0.034397:EXCLUDED AND MS2PROD=formula(C6H11O11P2):TOLERANCEPPM=10:INTENSITYPERCENT=0.000636:EXCLUDED</t>
+  </si>
+  <si>
+    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C24H33):TOLERANCEPPM=10:INTENSITYPERCENT=0.004144:EXCLUDED AND MS2PROD=formula(C24H33O):TOLERANCEPPM=10:INTENSITYPERCENT=0.014517:EXCLUDED AND MS2NL=formula(C23H39N2P):TOLERANCEPPM=10:INTENSITYPERCENT=0.184262 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C24H33):TOLERANCEPPM=10:INTENSITYPERCENT=0.004144:EXCLUDED AND MS2PROD=formula(C24H33O):TOLERANCEPPM=10:INTENSITYPERCENT=0.014517 AND MS2NL=formula(C20H42N2OS2):TOLERANCEPPM=10:INTENSITYPERCENT=0.008663 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C24H33):TOLERANCEPPM=10:INTENSITYPERCENT=0.004144 AND MS2NL=formula(C12H22O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.001918:EXCLUDED AND MS2PROD=formula(C16H21O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.001793:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C24H33):TOLERANCEPPM=10:INTENSITYPERCENT=0.004144 AND MS2NL=formula(C12H22O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.001918 AND MS2PROD=formula(C18H27O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.010528</t>
+  </si>
+  <si>
+    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C6H10NO2S):TOLERANCEPPM=10:INTENSITYPERCENT=0.030424:EXCLUDED AND MS2PROD=formula(H5N5O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.001250:EXCLUDED AND MS2PROD=formula(C7H7N4OS2):TOLERANCEPPM=10:INTENSITYPERCENT=0.000602 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C6H10NO2S):TOLERANCEPPM=10:INTENSITYPERCENT=0.030424:EXCLUDED AND MS2PROD=formula(H5N5O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.001250 AND MS2PROD=formula(C5H6NS):TOLERANCEPPM=10:INTENSITYPERCENT=0.002949 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C6H10NO2S):TOLERANCEPPM=10:INTENSITYPERCENT=0.030424 AND MS2PROD=formula(C3H6N):TOLERANCEPPM=10:INTENSITYPERCENT=0.000990:EXCLUDED AND MS2PROD=formula(C14H6N2):TOLERANCEPPM=10:INTENSITYPERCENT=0.006564:EXCLUDED</t>
+  </si>
+  <si>
+    <t>QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(C24H38O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.001176:EXCLUDED AND MS2PROD=formula(C23H35O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.000073:EXCLUDED AND MS2NL=formula(C25H34N4):TOLERANCEPPM=10:INTENSITYPERCENT=0.000982 ||| QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(C24H38O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.001176:EXCLUDED AND MS2PROD=formula(C23H35O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.000073 AND MS2PROD=formula(C22H31O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.000077:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(C24H38O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.001176 AND MS2NL=formula(C15H41N7O7):TOLERANCEPPM=10:INTENSITYPERCENT=0.000512:EXCLUDED AND MS2PROD=formula(C6H13N2O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.880451:EXCLUDED</t>
+  </si>
+  <si>
+    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C3H6O5P):TOLERANCEPPM=10:INTENSITYPERCENT=0.001914:EXCLUDED AND MS2PROD=formula(C5H11NO5P):TOLERANCEPPM=10:INTENSITYPERCENT=0.000460:EXCLUDED AND MS2PROD=formula(C18H33O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.045027 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C3H6O5P):TOLERANCEPPM=10:INTENSITYPERCENT=0.001914:EXCLUDED AND MS2PROD=formula(C5H11NO5P):TOLERANCEPPM=10:INTENSITYPERCENT=0.000460 AND MS2NL=formula(C8H3N7):TOLERANCEPPM=10:INTENSITYPERCENT=0.952171:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C3H6O5P):TOLERANCEPPM=10:INTENSITYPERCENT=0.001914 AND MS2PROD=formula(O3P):TOLERANCEPPM=10:INTENSITYPERCENT=0.462538:EXCLUDED AND MS2NL=formula(H5O5P):TOLERANCEPPM=10:INTENSITYPERCENT=0.030577:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C3H6O5P):TOLERANCEPPM=10:INTENSITYPERCENT=0.001914 AND MS2PROD=formula(O3P):TOLERANCEPPM=10:INTENSITYPERCENT=0.462538 AND MS2PROD=formula(C6H9O10P2):TOLERANCEPPM=10:INTENSITYPERCENT=0.002631</t>
+  </si>
+  <si>
+    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C7H3O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.004616:EXCLUDED AND MS2PROD=formula(C15H9O6):TOLERANCEPPM=10:INTENSITYPERCENT=0.008312:EXCLUDED AND MS2PROD=formula(C15H8O7):TOLERANCEPPM=10:INTENSITYPERCENT=0.016601 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C7H3O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.004616:EXCLUDED AND MS2PROD=formula(C15H9O6):TOLERANCEPPM=10:INTENSITYPERCENT=0.008312 AND MS2PROD=formula(C15H9O6):TOLERANCEPPM=10:INTENSITYPERCENT=0.122768:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C7H3O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.004616:EXCLUDED AND MS2PROD=formula(C15H9O6):TOLERANCEPPM=10:INTENSITYPERCENT=0.008312 AND MS2PROD=formula(C15H9O6):TOLERANCEPPM=10:INTENSITYPERCENT=0.122768 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C7H3O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.004616 AND MS2PROD=formula(C6H3O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.000987:EXCLUDED AND MS2PROD=formula(C8H6O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.000394:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C7H3O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.004616 AND MS2PROD=formula(C6H3O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.000987 AND MS2PROD=formula(C12H7O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.004171</t>
+  </si>
+  <si>
+    <t>QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(C5H8O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.283732:EXCLUDED AND MS2PROD=formula(C5H6N5):TOLERANCEPPM=10:INTENSITYPERCENT=0.736998:EXCLUDED AND MS2NL=formula(C8H8N2OS2):TOLERANCEPPM=10:INTENSITYPERCENT=0.127969 ||| QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(C5H8O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.283732:EXCLUDED AND MS2PROD=formula(C5H6N5):TOLERANCEPPM=10:INTENSITYPERCENT=0.736998 AND MS2PROD=formula(C6H6N5):TOLERANCEPPM=10:INTENSITYPERCENT=0.005699:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(C5H8O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.283732 AND MS2NL=formula(C5H11NO4):TOLERANCEPPM=10:INTENSITYPERCENT=0.000099:EXCLUDED AND MS2NL=formula(C5H8O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.919773 ||| QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(C5H8O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.283732 AND MS2NL=formula(C5H11NO4):TOLERANCEPPM=10:INTENSITYPERCENT=0.000099 AND MS2PROD=formula(C7H5N4O):TOLERANCEPPM=10:INTENSITYPERCENT=0.013940:EXCLUDED</t>
+  </si>
+  <si>
+    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C6H9O5):TOLERANCEPPM=10:INTENSITYPERCENT=0.000004:EXCLUDED AND MS2NL=formula(C7H14S2):TOLERANCEPPM=10:INTENSITYPERCENT=0.092304:EXCLUDED AND MS2NL=formula(C13H24O4S2):TOLERANCEPPM=10:INTENSITYPERCENT=0.056189 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C6H9O5):TOLERANCEPPM=10:INTENSITYPERCENT=0.000004:EXCLUDED AND MS2NL=formula(C7H14S2):TOLERANCEPPM=10:INTENSITYPERCENT=0.092304 AND MS2NL=formula(C3H6O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.008776:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C6H9O5):TOLERANCEPPM=10:INTENSITYPERCENT=0.000004 AND MS2PROD=formula(C6H7O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.002829:EXCLUDED AND MS2PROD=formula(C9H7NO2):TOLERANCEPPM=10:INTENSITYPERCENT=0.000115:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C6H9O5):TOLERANCEPPM=10:INTENSITYPERCENT=0.000004 AND MS2PROD=formula(C6H7O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.002829 AND MS2NL=formula(C3H8O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.018492:EXCLUDED</t>
+  </si>
+  <si>
+    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C5H10N6O):TOLERANCEPPM=10:INTENSITYPERCENT=0.001951:EXCLUDED AND MS2PROD=formula(C7H11N5O):TOLERANCEPPM=10:INTENSITYPERCENT=0.000637:EXCLUDED AND MS2PROD=formula(C2H6N6O):TOLERANCEPPM=10:INTENSITYPERCENT=0.004135 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C5H10N6O):TOLERANCEPPM=10:INTENSITYPERCENT=0.001951:EXCLUDED AND MS2PROD=formula(C7H11N5O):TOLERANCEPPM=10:INTENSITYPERCENT=0.000637 AND MS2PROD=formula(C9H13N5O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.001688:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C5H10N6O):TOLERANCEPPM=10:INTENSITYPERCENT=0.001951 AND MS2NL=formula(C24H43N3O6P2):TOLERANCEPPM=10:INTENSITYPERCENT=0.001160:EXCLUDED AND MS2PROD=formula(C8H14N5O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.000451:EXCLUDED</t>
+  </si>
+  <si>
+    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C3H8O5P):TOLERANCEPPM=10:INTENSITYPERCENT=0.001440:EXCLUDED AND MS2PROD=formula(C3H7NaO5P):TOLERANCEPPM=10:INTENSITYPERCENT=0.000395:EXCLUDED AND MS2NL=formula(C3H4N5P):TOLERANCEPPM=10:INTENSITYPERCENT=0.338294 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C3H8O5P):TOLERANCEPPM=10:INTENSITYPERCENT=0.001440:EXCLUDED AND MS2PROD=formula(C3H7NaO5P):TOLERANCEPPM=10:INTENSITYPERCENT=0.000395 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C3H8O5P):TOLERANCEPPM=10:INTENSITYPERCENT=0.001440 AND MS2NL=formula(C16H18N2O2S3):TOLERANCEPPM=10:INTENSITYPERCENT=0.004532:EXCLUDED</t>
+  </si>
+  <si>
+    <t>QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(C5H8O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.172707:EXCLUDED AND MS2PROD=formula(C3H6N3O6P):TOLERANCEPPM=10:INTENSITYPERCENT=0.010060:EXCLUDED AND MS2NL=formula(C4H7NO4):TOLERANCEPPM=10:INTENSITYPERCENT=0.029269 ||| QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(C5H8O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.172707:EXCLUDED AND MS2PROD=formula(C3H6N3O6P):TOLERANCEPPM=10:INTENSITYPERCENT=0.010060 AND MS2PROD=formula(C19H2N7O5):TOLERANCEPPM=10:INTENSITYPERCENT=0.007694:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(C5H8O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.172707 AND MS2NL=formula(C6H9NO5):TOLERANCEPPM=10:INTENSITYPERCENT=0.001242:EXCLUDED AND MS2NL=formula(C5H8O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.858722 ||| QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(C5H8O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.172707 AND MS2NL=formula(C6H9NO5):TOLERANCEPPM=10:INTENSITYPERCENT=0.001242 AND MS2PROD=formula(C7H3N4O):TOLERANCEPPM=10:INTENSITYPERCENT=0.196133:EXCLUDED</t>
+  </si>
+  <si>
+    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C24H35O):TOLERANCEPPM=10:INTENSITYPERCENT=0.010829:EXCLUDED AND MS2PROD=formula(C24H33O):TOLERANCEPPM=10:INTENSITYPERCENT=0.009579 AND MS2PROD=formula(C16H17):TOLERANCEPPM=10:INTENSITYPERCENT=0.012364 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C24H35O):TOLERANCEPPM=10:INTENSITYPERCENT=0.010829 AND MS2PROD=formula(C16H23):TOLERANCEPPM=10:INTENSITYPERCENT=0.013950:EXCLUDED AND MS2PROD=formula(C28H42NO3):TOLERANCEPPM=10:INTENSITYPERCENT=0.000191 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C24H35O):TOLERANCEPPM=10:INTENSITYPERCENT=0.010829 AND MS2PROD=formula(C16H23):TOLERANCEPPM=10:INTENSITYPERCENT=0.013950 AND MS2NL=formula(C22H37NO3):TOLERANCEPPM=10:INTENSITYPERCENT=0.004929:EXCLUDED</t>
+  </si>
+  <si>
+    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C9H13):TOLERANCEPPM=10:INTENSITYPERCENT=0.000976:EXCLUDED AND MS2PROD=formula(C7H7):TOLERANCEPPM=10:INTENSITYPERCENT=0.000213:EXCLUDED AND MS2PROD=formula(C6H5):TOLERANCEPPM=10:INTENSITYPERCENT=0.000258 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C9H13):TOLERANCEPPM=10:INTENSITYPERCENT=0.000976:EXCLUDED AND MS2PROD=formula(C7H7):TOLERANCEPPM=10:INTENSITYPERCENT=0.000213 AND MS2PROD=formula(C6H9):TOLERANCEPPM=10:INTENSITYPERCENT=0.001077:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C9H13):TOLERANCEPPM=10:INTENSITYPERCENT=0.000976 AND MS2PROD=formula(C9H7O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.000929 AND MS2PROD=formula(C12H13):TOLERANCEPPM=10:INTENSITYPERCENT=0.003782:EXCLUDED</t>
+  </si>
+  <si>
+    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C9H13):TOLERANCEPPM=10:INTENSITYPERCENT=0.000815:EXCLUDED AND MS2PROD=formula(C7H7):TOLERANCEPPM=10:INTENSITYPERCENT=0.000084:EXCLUDED AND MS2PROD=formula(C9H8N):TOLERANCEPPM=10:INTENSITYPERCENT=0.000181 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C9H13):TOLERANCEPPM=10:INTENSITYPERCENT=0.000815:EXCLUDED AND MS2PROD=formula(C7H7):TOLERANCEPPM=10:INTENSITYPERCENT=0.000084 AND MS2PROD=formula(C6H9):TOLERANCEPPM=10:INTENSITYPERCENT=0.001348:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C9H13):TOLERANCEPPM=10:INTENSITYPERCENT=0.000815 AND MS2PROD=formula(C9H7O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.000154:EXCLUDED AND MS2PROD=formula(C9H8N):TOLERANCEPPM=10:INTENSITYPERCENT=0.001364 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C9H13):TOLERANCEPPM=10:INTENSITYPERCENT=0.000815 AND MS2PROD=formula(C9H7O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.000154 AND MS2PROD=formula(C12H13):TOLERANCEPPM=10:INTENSITYPERCENT=0.002894:EXCLUDED</t>
+  </si>
+  <si>
+    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C6H9O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.103127:EXCLUDED AND MS2PROD=formula(C13H22NO7):TOLERANCEPPM=10:INTENSITYPERCENT=0.076942:EXCLUDED AND MS2NL=formula(C2H10O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.060764 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C6H9O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.103127:EXCLUDED AND MS2PROD=formula(C13H22NO7):TOLERANCEPPM=10:INTENSITYPERCENT=0.076942 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C6H9O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.103127 AND MS2NL=formula(C7H16OS2):TOLERANCEPPM=10:INTENSITYPERCENT=0.000630:EXCLUDED AND MS2PROD=formula(C6H7O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.131305 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C6H9O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.103127 AND MS2NL=formula(C7H16OS2):TOLERANCEPPM=10:INTENSITYPERCENT=0.000630 AND MS2PROD=formula(C6H11O5):TOLERANCEPPM=10:INTENSITYPERCENT=0.004699</t>
+  </si>
+  <si>
+    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C19H29O):TOLERANCEPPM=10:INTENSITYPERCENT=0.003675:EXCLUDED AND MS2PROD=formula(C14H17O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.021058:EXCLUDED AND MS2PROD=formula(C19H29):TOLERANCEPPM=10:INTENSITYPERCENT=0.050000 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C19H29O):TOLERANCEPPM=10:INTENSITYPERCENT=0.003675:EXCLUDED AND MS2PROD=formula(C14H17O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.021058 AND MS2PROD=formula(C7H9O):TOLERANCEPPM=10:INTENSITYPERCENT=0.001107 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C19H29O):TOLERANCEPPM=10:INTENSITYPERCENT=0.003675 AND MS2PROD=formula(C2H3O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.000332:EXCLUDED AND MS2PROD=formula(C14H19O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.004220 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C19H29O):TOLERANCEPPM=10:INTENSITYPERCENT=0.003675 AND MS2PROD=formula(C2H3O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.000332 AND MS2NL=formula(C4N4):TOLERANCEPPM=10:INTENSITYPERCENT=0.007086:EXCLUDED</t>
+  </si>
+  <si>
+    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C30H47O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.008097:EXCLUDED AND MS2PROD=formula(C28H41O):TOLERANCEPPM=10:INTENSITYPERCENT=0.000262:EXCLUDED AND MS2PROD=formula(C35H55O7):TOLERANCEPPM=10:INTENSITYPERCENT=0.008906 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C30H47O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.008097:EXCLUDED AND MS2PROD=formula(C28H41O):TOLERANCEPPM=10:INTENSITYPERCENT=0.000262 AND MS2PROD=formula(C28H43O):TOLERANCEPPM=10:INTENSITYPERCENT=0.004046:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C30H47O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.008097 AND MS2NL=formula(C39H39O6PS):TOLERANCEPPM=10:INTENSITYPERCENT=0.000088:EXCLUDED AND MS2PROD=formula(C30H47O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.996306:EXCLUDED</t>
+  </si>
+  <si>
+    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C23H24O7):TOLERANCEPPM=10:INTENSITYPERCENT=0.053501:EXCLUDED AND MS2PROD=formula(C13H5Cl2O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.017382:EXCLUDED AND MS2PROD=formula(C13H6O5):TOLERANCEPPM=10:INTENSITYPERCENT=0.385088 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C23H24O7):TOLERANCEPPM=10:INTENSITYPERCENT=0.053501:EXCLUDED AND MS2PROD=formula(C13H5Cl2O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.017382 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C23H24O7):TOLERANCEPPM=10:INTENSITYPERCENT=0.053501</t>
+  </si>
+  <si>
+    <t>QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(C2H8O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.075320:EXCLUDED AND MS2PROD=formula(C12H21O11):TOLERANCEPPM=10:INTENSITYPERCENT=0.022838:EXCLUDED AND MS2NL=formula(CH17N4O7P):TOLERANCEPPM=10:INTENSITYPERCENT=0.019822 ||| QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(C2H8O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.075320:EXCLUDED AND MS2PROD=formula(C12H21O11):TOLERANCEPPM=10:INTENSITYPERCENT=0.022838 AND MS2PROD=formula(C12H19O10):TOLERANCEPPM=10:INTENSITYPERCENT=0.023576:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(C2H8O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.075320 AND MS2PROD=formula(C3H5O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.042708:EXCLUDED AND MS2PROD=formula(C4H5O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.135896 ||| QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(C2H8O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.075320 AND MS2PROD=formula(C3H5O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.042708 AND MS2PROD=formula(C4H6NO):TOLERANCEPPM=10:INTENSITYPERCENT=0.001751:EXCLUDED</t>
+  </si>
+  <si>
+    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C9H8N):TOLERANCEPPM=10:INTENSITYPERCENT=0.705815:EXCLUDED AND MS2PROD=formula(C10H11N2):TOLERANCEPPM=10:INTENSITYPERCENT=0.018431 AND MS2PROD=formula(C11H10NO2):TOLERANCEPPM=10:INTENSITYPERCENT=0.001119 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C9H8N):TOLERANCEPPM=10:INTENSITYPERCENT=0.705815 AND MS2NL=formula(C2H7N):TOLERANCEPPM=10:INTENSITYPERCENT=0.412665:EXCLUDED AND MS2PROD=formula(C8H7):TOLERANCEPPM=10:INTENSITYPERCENT=0.015723 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C9H8N):TOLERANCEPPM=10:INTENSITYPERCENT=0.705815 AND MS2NL=formula(C2H7N):TOLERANCEPPM=10:INTENSITYPERCENT=0.412665</t>
+  </si>
+  <si>
+    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C25H40NO3):TOLERANCEPPM=10:INTENSITYPERCENT=0.000155:EXCLUDED AND MS2NL=formula(C24H38O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.018143:EXCLUDED AND MS2NL=formula(C24H38O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.024398 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C25H40NO3):TOLERANCEPPM=10:INTENSITYPERCENT=0.000155:EXCLUDED AND MS2NL=formula(C24H38O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.018143 AND MS2PROD=formula(C24H37O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.487587:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C25H40NO3):TOLERANCEPPM=10:INTENSITYPERCENT=0.000155</t>
+  </si>
+  <si>
+    <t>QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(CH2O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.272980:EXCLUDED AND MS2PROD=formula(C5H9O):TOLERANCEPPM=10:INTENSITYPERCENT=0.203558:EXCLUDED AND MS2PROD=formula(C4H7O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.796387 ||| QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(CH2O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.272980:EXCLUDED AND MS2PROD=formula(C5H9O):TOLERANCEPPM=10:INTENSITYPERCENT=0.203558 AND MS2NL=formula(C39H62N6O12):TOLERANCEPPM=10:INTENSITYPERCENT=0.013345:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(CH2O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.272980 AND MS2NL=formula(CH4O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.000476:EXCLUDED AND MS2PROD=formula(C3H5O):TOLERANCEPPM=10:INTENSITYPERCENT=0.003108:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(CH2O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.272980 AND MS2NL=formula(CH4O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.000476:EXCLUDED AND MS2PROD=formula(C3H5O):TOLERANCEPPM=10:INTENSITYPERCENT=0.003108 ||| QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(CH2O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.272980 AND MS2NL=formula(CH4O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.000476 AND MS2NL=formula(C3H4O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.081803</t>
+  </si>
+  <si>
+    <t>QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(C24H38O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.016080:EXCLUDED AND MS2PROD=formula(C23H37O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.057117:EXCLUDED AND MS2PROD=formula(C23H39O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.003521 ||| QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(C24H38O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.016080:EXCLUDED AND MS2PROD=formula(C23H37O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.057117 AND MS2PROD=formula(C24H35O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.042916:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(C24H38O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.016080 AND MS2PROD=formula(C4H6NO):TOLERANCEPPM=10:INTENSITYPERCENT=0.001655:EXCLUDED AND MS2PROD=formula(C23H35O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.000119 ||| QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(C24H38O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.016080 AND MS2PROD=formula(C4H6NO):TOLERANCEPPM=10:INTENSITYPERCENT=0.001655</t>
+  </si>
+  <si>
+    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C14H7O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.005224:EXCLUDED AND MS2PROD=formula(C15H8O5):TOLERANCEPPM=10:INTENSITYPERCENT=0.027431:EXCLUDED AND MS2PROD=formula(C24H21O5):TOLERANCEPPM=10:INTENSITYPERCENT=0.014475 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C14H7O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.005224:EXCLUDED AND MS2PROD=formula(C15H8O5):TOLERANCEPPM=10:INTENSITYPERCENT=0.027431 AND MS2PROD=formula(C8H4O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.002826 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C14H7O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.005224 AND MS2PROD=formula(C8H4O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.001316:EXCLUDED AND MS2NL=formula(C4H8):TOLERANCEPPM=10:INTENSITYPERCENT=0.003422 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C14H7O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.005224 AND MS2PROD=formula(C8H4O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.001316 AND MS2PROD=formula(C8H5O):TOLERANCEPPM=10:INTENSITYPERCENT=0.038652:EXCLUDED</t>
+  </si>
+  <si>
+    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C5H8N3):TOLERANCEPPM=10:INTENSITYPERCENT=0.269307:EXCLUDED AND MS2PROD=formula(C5H10N3):TOLERANCEPPM=10:INTENSITYPERCENT=0.314554 AND MS2PROD=formula(C5H7N2):TOLERANCEPPM=10:INTENSITYPERCENT=0.012994 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C5H8N3):TOLERANCEPPM=10:INTENSITYPERCENT=0.269307 AND MS2PROD=formula(C7H12N3):TOLERANCEPPM=10:INTENSITYPERCENT=0.030982:EXCLUDED AND MS2PROD=formula(C4H7N2):TOLERANCEPPM=10:INTENSITYPERCENT=0.003077:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C5H8N3):TOLERANCEPPM=10:INTENSITYPERCENT=0.269307 AND MS2PROD=formula(C7H12N3):TOLERANCEPPM=10:INTENSITYPERCENT=0.030982:EXCLUDED AND MS2PROD=formula(C4H7N2):TOLERANCEPPM=10:INTENSITYPERCENT=0.003077</t>
+  </si>
+  <si>
+    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C20H27O):TOLERANCEPPM=10:INTENSITYPERCENT=0.012507:EXCLUDED AND MS2PROD=formula(C10H19F2O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.012699:EXCLUDED AND MS2PROD=formula(C22H35O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.006115 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C20H27O):TOLERANCEPPM=10:INTENSITYPERCENT=0.012507:EXCLUDED AND MS2PROD=formula(C10H19F2O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.012699 AND MS2PROD=formula(C17H15F):TOLERANCEPPM=10:INTENSITYPERCENT=0.000012:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C20H27O):TOLERANCEPPM=10:INTENSITYPERCENT=0.012507 AND MS2PROD=formula(C5H11):TOLERANCEPPM=10:INTENSITYPERCENT=0.000462:EXCLUDED AND MS2NL=formula(C7H18O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.000944 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C20H27O):TOLERANCEPPM=10:INTENSITYPERCENT=0.012507 AND MS2PROD=formula(C5H11):TOLERANCEPPM=10:INTENSITYPERCENT=0.000462 AND MS2PROD=formula(C17H21):TOLERANCEPPM=10:INTENSITYPERCENT=0.000489:EXCLUDED</t>
+  </si>
+  <si>
+    <t>QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(C16H42N2O5S):TOLERANCEPPM=10:INTENSITYPERCENT=0.002428:EXCLUDED AND MS2NL=formula(C16H42N2O6S):TOLERANCEPPM=10:INTENSITYPERCENT=0.008114:EXCLUDED AND MS2PROD=formula(C23H35O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.019021 ||| QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(C16H42N2O5S):TOLERANCEPPM=10:INTENSITYPERCENT=0.002428:EXCLUDED AND MS2NL=formula(C16H42N2O6S):TOLERANCEPPM=10:INTENSITYPERCENT=0.008114 AND MS2NL=formula(C13H24N3O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.004777:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(C16H42N2O5S):TOLERANCEPPM=10:INTENSITYPERCENT=0.002428 AND MS2NL=formula(C25H40N3O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.068889:EXCLUDED AND MS2NL=formula(C15H35N9S):TOLERANCEPPM=10:INTENSITYPERCENT=0.109837:EXCLUDED</t>
+  </si>
+  <si>
+    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C29H43O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.000286:EXCLUDED AND MS2PROD=formula(C30H47O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.000009:EXCLUDED AND MS2PROD=formula(C30H47O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.000190 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C29H43O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.000286:EXCLUDED AND MS2PROD=formula(C30H47O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.000009 AND MS2NL=formula(C27H43N3O3S):TOLERANCEPPM=10:INTENSITYPERCENT=0.000096:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C29H43O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.000286 AND MS2PROD=formula(C24H38NO2):TOLERANCEPPM=10:INTENSITYPERCENT=0.000439:EXCLUDED AND MS2NL=formula(C9H18N6O9):TOLERANCEPPM=10:INTENSITYPERCENT=0.006425:EXCLUDED</t>
+  </si>
+  <si>
+    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C23H21O6):TOLERANCEPPM=10:INTENSITYPERCENT=0.012203:EXCLUDED AND MS2PROD=formula(C23H24O7):TOLERANCEPPM=10:INTENSITYPERCENT=0.036362:EXCLUDED AND MS2PROD=formula(C13H6O5):TOLERANCEPPM=10:INTENSITYPERCENT=0.393985 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C23H21O6):TOLERANCEPPM=10:INTENSITYPERCENT=0.012203:EXCLUDED AND MS2PROD=formula(C23H24O7):TOLERANCEPPM=10:INTENSITYPERCENT=0.036362 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C23H21O6):TOLERANCEPPM=10:INTENSITYPERCENT=0.012203 AND MS2PROD=formula(C19H15O6):TOLERANCEPPM=10:INTENSITYPERCENT=0.001310:EXCLUDED AND MS2PROD=formula(C19H13O6):TOLERANCEPPM=10:INTENSITYPERCENT=0.008984 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C23H21O6):TOLERANCEPPM=10:INTENSITYPERCENT=0.012203 AND MS2PROD=formula(C19H15O6):TOLERANCEPPM=10:INTENSITYPERCENT=0.001310</t>
+  </si>
+  <si>
+    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C14H23O5):TOLERANCEPPM=10:INTENSITYPERCENT=0.034095:EXCLUDED AND MS2PROD=formula(C22H40N):TOLERANCEPPM=10:INTENSITYPERCENT=0.012631:EXCLUDED AND MS2PROD=formula(C18H31O8):TOLERANCEPPM=10:INTENSITYPERCENT=0.009209 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C14H23O5):TOLERANCEPPM=10:INTENSITYPERCENT=0.034095:EXCLUDED AND MS2PROD=formula(C22H40N):TOLERANCEPPM=10:INTENSITYPERCENT=0.012631 AND MS2PROD=formula(C22H40N):TOLERANCEPPM=10:INTENSITYPERCENT=0.342627:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C14H23O5):TOLERANCEPPM=10:INTENSITYPERCENT=0.034095 AND MS2PROD=formula(C8H13O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.046630</t>
+  </si>
+  <si>
+    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C24H33):TOLERANCEPPM=10:INTENSITYPERCENT=0.004383:EXCLUDED AND MS2PROD=formula(C24H33O):TOLERANCEPPM=10:INTENSITYPERCENT=0.014967:EXCLUDED AND MS2PROD=formula(C8H7O7):TOLERANCEPPM=10:INTENSITYPERCENT=0.162655 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C24H33):TOLERANCEPPM=10:INTENSITYPERCENT=0.004383:EXCLUDED AND MS2PROD=formula(C24H33O):TOLERANCEPPM=10:INTENSITYPERCENT=0.014967 AND MS2PROD=formula(C10H13O):TOLERANCEPPM=10:INTENSITYPERCENT=0.005582:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C24H33):TOLERANCEPPM=10:INTENSITYPERCENT=0.004383 AND MS2PROD=formula(C12H15):TOLERANCEPPM=10:INTENSITYPERCENT=0.028788:EXCLUDED AND MS2NL=formula(C8H14O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.004970:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C24H33):TOLERANCEPPM=10:INTENSITYPERCENT=0.004383 AND MS2PROD=formula(C12H15):TOLERANCEPPM=10:INTENSITYPERCENT=0.028788 AND MS2PROD=formula(C14H19O):TOLERANCEPPM=10:INTENSITYPERCENT=0.002210:EXCLUDED</t>
+  </si>
+  <si>
+    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C24H12O6S):TOLERANCEPPM=10:INTENSITYPERCENT=0.034951:EXCLUDED AND MS2PROD=formula(C11H19O):TOLERANCEPPM=10:INTENSITYPERCENT=0.015808:EXCLUDED AND MS2PROD=formula(C4H3O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.378989 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C24H12O6S):TOLERANCEPPM=10:INTENSITYPERCENT=0.034951:EXCLUDED AND MS2PROD=formula(C11H19O):TOLERANCEPPM=10:INTENSITYPERCENT=0.015808 AND MS2PROD=formula(C8H11):TOLERANCEPPM=10:INTENSITYPERCENT=0.000777:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C24H12O6S):TOLERANCEPPM=10:INTENSITYPERCENT=0.034951 AND MS2PROD=formula(C31H40N6):TOLERANCEPPM=10:INTENSITYPERCENT=0.001067:EXCLUDED AND MS2PROD=formula(C11H17N4O10P3S):TOLERANCEPPM=10:INTENSITYPERCENT=0.000424:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C24H12O6S):TOLERANCEPPM=10:INTENSITYPERCENT=0.034951 AND MS2PROD=formula(C31H40N6):TOLERANCEPPM=10:INTENSITYPERCENT=0.001067:EXCLUDED AND MS2PROD=formula(C11H17N4O10P3S):TOLERANCEPPM=10:INTENSITYPERCENT=0.000424</t>
+  </si>
+  <si>
+    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C24H35O):TOLERANCEPPM=10:INTENSITYPERCENT=0.001551:EXCLUDED AND MS2PROD=formula(C24H33O):TOLERANCEPPM=10:INTENSITYPERCENT=0.002283 AND MS2PROD=formula(C24H33O):TOLERANCEPPM=10:INTENSITYPERCENT=0.016520:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C24H35O):TOLERANCEPPM=10:INTENSITYPERCENT=0.001551:EXCLUDED AND MS2PROD=formula(C24H33O):TOLERANCEPPM=10:INTENSITYPERCENT=0.002283 AND MS2PROD=formula(C24H33O):TOLERANCEPPM=10:INTENSITYPERCENT=0.016520 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C24H35O):TOLERANCEPPM=10:INTENSITYPERCENT=0.001551 AND MS2PROD=formula(C26H37O):TOLERANCEPPM=10:INTENSITYPERCENT=0.000693:EXCLUDED AND MS2PROD=formula(C24H33):TOLERANCEPPM=10:INTENSITYPERCENT=0.001553:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C24H35O):TOLERANCEPPM=10:INTENSITYPERCENT=0.001551 AND MS2PROD=formula(C26H37O):TOLERANCEPPM=10:INTENSITYPERCENT=0.000693:EXCLUDED AND MS2PROD=formula(C24H33):TOLERANCEPPM=10:INTENSITYPERCENT=0.001553 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C24H35O):TOLERANCEPPM=10:INTENSITYPERCENT=0.001551 AND MS2PROD=formula(C26H37O):TOLERANCEPPM=10:INTENSITYPERCENT=0.000693 AND MS2PROD=formula(C22H29O):TOLERANCEPPM=10:INTENSITYPERCENT=0.004287</t>
+  </si>
+  <si>
+    <t>QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(C22H37N2O4P):TOLERANCEPPM=10:INTENSITYPERCENT=0.087401:EXCLUDED AND MS2PROD=formula(C8H10NO3):TOLERANCEPPM=10:INTENSITYPERCENT=0.033861:EXCLUDED AND MS2PROD=formula(C11H17O5):TOLERANCEPPM=10:INTENSITYPERCENT=0.072294 ||| QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(C22H37N2O4P):TOLERANCEPPM=10:INTENSITYPERCENT=0.087401:EXCLUDED AND MS2PROD=formula(C8H10NO3):TOLERANCEPPM=10:INTENSITYPERCENT=0.033861 AND MS2PROD=formula(C8H9NO3):TOLERANCEPPM=10:INTENSITYPERCENT=0.095392 ||| QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(C22H37N2O4P):TOLERANCEPPM=10:INTENSITYPERCENT=0.087401 AND MS2PROD=formula(C10H7NO):TOLERANCEPPM=10:INTENSITYPERCENT=0.064899:EXCLUDED</t>
+  </si>
+  <si>
+    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C6H11O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.101660:EXCLUDED AND MS2NL=formula(C25H45N11O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.091156:EXCLUDED AND MS2PROD=formula(C18H29O6):TOLERANCEPPM=10:INTENSITYPERCENT=0.296343 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C6H11O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.101660:EXCLUDED AND MS2NL=formula(C25H45N11O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.091156 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C6H11O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.101660 AND MS2NL=formula(C59H56O):TOLERANCEPPM=10:INTENSITYPERCENT=0.001450:EXCLUDED AND MS2PROD=formula(C4H9N3O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.156155:EXCLUDED</t>
+  </si>
+  <si>
+    <t>QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(C9H21N4O8P):TOLERANCEPPM=10:INTENSITYPERCENT=0.005939:EXCLUDED AND MS2PROD=formula(C6H11O6):TOLERANCEPPM=10:INTENSITYPERCENT=0.000096 AND MS2PROD=formula(C9H7O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.002123 ||| QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(C9H21N4O8P):TOLERANCEPPM=10:INTENSITYPERCENT=0.005939 AND MS2NL=formula(C14H17N2PS):TOLERANCEPPM=10:INTENSITYPERCENT=0.005967:EXCLUDED AND MS2PROD=formula(C4H7O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.013345 ||| QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(C9H21N4O8P):TOLERANCEPPM=10:INTENSITYPERCENT=0.005939 AND MS2NL=formula(C14H17N2PS):TOLERANCEPPM=10:INTENSITYPERCENT=0.005967 AND MS2NL=formula(C9H23N4O6P):TOLERANCEPPM=10:INTENSITYPERCENT=0.000637:EXCLUDED</t>
+  </si>
+  <si>
+    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C14H11O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.371433:EXCLUDED AND MS2PROD=formula(C12H9O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.254468:EXCLUDED AND MS2PROD=formula(C30H25O6):TOLERANCEPPM=10:INTENSITYPERCENT=0.007034 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C14H11O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.371433:EXCLUDED AND MS2PROD=formula(C12H9O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.254468 AND MS2PROD=formula(C13H11O):TOLERANCEPPM=10:INTENSITYPERCENT=0.045496 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C14H11O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.371433 AND MS2PROD=formula(C12H9O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.000469:EXCLUDED AND MS2PROD=formula(C14H11O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.907702 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C14H11O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.371433 AND MS2PROD=formula(C12H9O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.000469</t>
+  </si>
+  <si>
+    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C20H21O6):TOLERANCEPPM=10:INTENSITYPERCENT=0.059631:EXCLUDED AND MS2PROD=formula(C24H19O8):TOLERANCEPPM=10:INTENSITYPERCENT=0.003361:EXCLUDED AND MS2PROD=formula(C22H25O8):TOLERANCEPPM=10:INTENSITYPERCENT=0.005552 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C20H21O6):TOLERANCEPPM=10:INTENSITYPERCENT=0.059631:EXCLUDED AND MS2PROD=formula(C24H19O8):TOLERANCEPPM=10:INTENSITYPERCENT=0.003361 AND MS2PROD=formula(C12H5N4O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.005004:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C20H21O6):TOLERANCEPPM=10:INTENSITYPERCENT=0.059631 AND MS2PROD=formula(C11H13O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.055084:EXCLUDED</t>
+  </si>
+  <si>
+    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C10H18N4O):TOLERANCEPPM=10:INTENSITYPERCENT=0.000696:EXCLUDED AND MS2PROD=formula(C11H20N6O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.000021:EXCLUDED AND MS2PROD=formula(C9H17N5O):TOLERANCEPPM=10:INTENSITYPERCENT=0.001586 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C10H18N4O):TOLERANCEPPM=10:INTENSITYPERCENT=0.000696:EXCLUDED AND MS2PROD=formula(C11H20N6O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.000021 AND MS2PROD=formula(C3H6N):TOLERANCEPPM=10:INTENSITYPERCENT=0.000388:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C10H18N4O):TOLERANCEPPM=10:INTENSITYPERCENT=0.000696 AND MS2PROD=formula(C6H11):TOLERANCEPPM=10:INTENSITYPERCENT=0.005027:EXCLUDED AND MS2PROD=formula(C12H17O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.002559:EXCLUDED</t>
+  </si>
+  <si>
+    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C4H4N3):TOLERANCEPPM=10:INTENSITYPERCENT=0.000016:EXCLUDED AND MS2PROD=formula(C9H13):TOLERANCEPPM=10:INTENSITYPERCENT=0.000001:EXCLUDED AND MS2PROD=formula(C5H6N5):TOLERANCEPPM=10:INTENSITYPERCENT=0.000052 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C4H4N3):TOLERANCEPPM=10:INTENSITYPERCENT=0.000016:EXCLUDED AND MS2PROD=formula(C9H13):TOLERANCEPPM=10:INTENSITYPERCENT=0.000001 AND MS2PROD=formula(C4H5N2O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.000062 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C4H4N3):TOLERANCEPPM=10:INTENSITYPERCENT=0.000016 AND MS2PROD=formula(C5H9N2O):TOLERANCEPPM=10:INTENSITYPERCENT=0.033524:EXCLUDED AND MS2PROD=formula(C7H7OS):TOLERANCEPPM=10:INTENSITYPERCENT=0.000250:EXCLUDED</t>
+  </si>
+  <si>
+    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C6H9O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.001322:EXCLUDED AND MS2NL=formula(C6H10O5):TOLERANCEPPM=10:INTENSITYPERCENT=0.098563 AND MS2PROD=formula(C13H15O):TOLERANCEPPM=10:INTENSITYPERCENT=0.000355:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C6H9O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.001322 AND MS2PROD=formula(C4H5O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.003312:EXCLUDED AND MS2PROD=formula(C6H11O5):TOLERANCEPPM=10:INTENSITYPERCENT=0.000298 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C6H9O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.001322 AND MS2PROD=formula(C4H5O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.003312 AND MS2NL=formula(CH6O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.000486:EXCLUDED</t>
+  </si>
+  <si>
+    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C9H14NO2S):TOLERANCEPPM=10:INTENSITYPERCENT=0.017714:EXCLUDED AND MS2PROD=formula(C6H4N4OS):TOLERANCEPPM=10:INTENSITYPERCENT=0.598320:EXCLUDED AND MS2PROD=formula(C21H15ClFN3O):TOLERANCEPPM=10:INTENSITYPERCENT=0.013215 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C9H14NO2S):TOLERANCEPPM=10:INTENSITYPERCENT=0.017714:EXCLUDED AND MS2PROD=formula(C6H4N4OS):TOLERANCEPPM=10:INTENSITYPERCENT=0.598320 AND MS2PROD=formula(C6H5N4OS):TOLERANCEPPM=10:INTENSITYPERCENT=0.079913 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C9H14NO2S):TOLERANCEPPM=10:INTENSITYPERCENT=0.017714 AND MS2PROD=formula(C9H12NO2):TOLERANCEPPM=10:INTENSITYPERCENT=0.391231:EXCLUDED</t>
+  </si>
+  <si>
+    <t>QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(C18H17N7O7S):TOLERANCEPPM=10:INTENSITYPERCENT=0.104574:EXCLUDED AND MS2PROD=formula(C11H6O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.489875:EXCLUDED AND MS2NL=formula(C8H5F4OP):TOLERANCEPPM=10:INTENSITYPERCENT=0.057326 ||| QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(C18H17N7O7S):TOLERANCEPPM=10:INTENSITYPERCENT=0.104574:EXCLUDED AND MS2PROD=formula(C11H6O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.489875 ||| QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(C18H17N7O7S):TOLERANCEPPM=10:INTENSITYPERCENT=0.104574</t>
+  </si>
+  <si>
+    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C2H4NO2):TOLERANCEPPM=10:INTENSITYPERCENT=0.000197:EXCLUDED AND MS2NL=formula(CH3NO2):TOLERANCEPPM=10:INTENSITYPERCENT=0.000221 AND MS2NL=formula(CH3NO2):TOLERANCEPPM=10:INTENSITYPERCENT=0.034983 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C2H4NO2):TOLERANCEPPM=10:INTENSITYPERCENT=0.000197 AND MS2NL=formula(CO2):TOLERANCEPPM=10:INTENSITYPERCENT=0.000221:EXCLUDED AND MS2NL=formula(C3H5NO2):TOLERANCEPPM=10:INTENSITYPERCENT=0.000605 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C2H4NO2):TOLERANCEPPM=10:INTENSITYPERCENT=0.000197 AND MS2NL=formula(CO2):TOLERANCEPPM=10:INTENSITYPERCENT=0.000221 AND MS2PROD=formula(C9H14NO2):TOLERANCEPPM=10:INTENSITYPERCENT=0.011885:EXCLUDED</t>
+  </si>
+  <si>
+    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C10H6O5):TOLERANCEPPM=10:INTENSITYPERCENT=0.005194:EXCLUDED AND MS2PROD=formula(C12H11O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.518921:EXCLUDED AND MS2PROD=formula(C9H4O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.071486 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C10H6O5):TOLERANCEPPM=10:INTENSITYPERCENT=0.005194:EXCLUDED AND MS2PROD=formula(C12H11O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.518921 AND MS2NL=formula(C4H16N2O5S):TOLERANCEPPM=10:INTENSITYPERCENT=0.113233:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C10H6O5):TOLERANCEPPM=10:INTENSITYPERCENT=0.005194 AND MS2PROD=formula(C9H3O5):TOLERANCEPPM=10:INTENSITYPERCENT=0.000981:EXCLUDED AND MS2PROD=formula(C9H4O5):TOLERANCEPPM=10:INTENSITYPERCENT=0.000303 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C10H6O5):TOLERANCEPPM=10:INTENSITYPERCENT=0.005194 AND MS2PROD=formula(C9H3O5):TOLERANCEPPM=10:INTENSITYPERCENT=0.000981 AND MS2PROD=formula(C9H3O6):TOLERANCEPPM=10:INTENSITYPERCENT=0.000276:EXCLUDED</t>
+  </si>
+  <si>
+    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C3HO2):TOLERANCEPPM=10:INTENSITYPERCENT=0.964735:EXCLUDED AND MS2PROD=formula(C11HO):TOLERANCEPPM=10:INTENSITYPERCENT=0.103805 AND MS2PROD=formula(C11HO):TOLERANCEPPM=10:INTENSITYPERCENT=0.639490:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C3HO2):TOLERANCEPPM=10:INTENSITYPERCENT=0.964735 AND MS2PROD=formula(C3H3O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.004739:EXCLUDED AND MS2NL=formula(C24H16N2O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.500000:EXCLUDED</t>
+  </si>
+  <si>
+    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C7H11O6):TOLERANCEPPM=10:INTENSITYPERCENT=0.100112:EXCLUDED AND MS2NL=formula(C12H8N10S):TOLERANCEPPM=10:INTENSITYPERCENT=0.030334 AND MS2PROD=formula(C9H7O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.009130 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C7H11O6):TOLERANCEPPM=10:INTENSITYPERCENT=0.100112 AND MS2NL=formula(C2H6N6OS):TOLERANCEPPM=10:INTENSITYPERCENT=0.007571:EXCLUDED AND MS2NL=formula(C20H20O2P2):TOLERANCEPPM=10:INTENSITYPERCENT=0.002460 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C7H11O6):TOLERANCEPPM=10:INTENSITYPERCENT=0.100112 AND MS2NL=formula(C2H6N6OS):TOLERANCEPPM=10:INTENSITYPERCENT=0.007571</t>
+  </si>
+  <si>
+    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C8H16NO2):TOLERANCEPPM=10:INTENSITYPERCENT=0.103991:EXCLUDED AND MS2PROD=formula(C8H16NO3):TOLERANCEPPM=10:INTENSITYPERCENT=0.034541:EXCLUDED AND MS2NL=formula(C17H40N6S3):TOLERANCEPPM=10:INTENSITYPERCENT=0.011652 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C8H16NO2):TOLERANCEPPM=10:INTENSITYPERCENT=0.103991:EXCLUDED AND MS2PROD=formula(C8H16NO3):TOLERANCEPPM=10:INTENSITYPERCENT=0.034541 AND MS2PROD=formula(C5H10NO2):TOLERANCEPPM=10:INTENSITYPERCENT=0.007872 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C8H16NO2):TOLERANCEPPM=10:INTENSITYPERCENT=0.103991 AND MS2PROD=formula(C6H14NO):TOLERANCEPPM=10:INTENSITYPERCENT=0.000878:EXCLUDED AND MS2NL=formula(C49H52N4O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.087956 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C8H16NO2):TOLERANCEPPM=10:INTENSITYPERCENT=0.103991 AND MS2PROD=formula(C6H14NO):TOLERANCEPPM=10:INTENSITYPERCENT=0.000878 AND MS2NL=formula(C4H8):TOLERANCEPPM=10:INTENSITYPERCENT=0.005326:EXCLUDED</t>
   </si>
 </sst>
 </file>
@@ -1138,8 +1138,8 @@
   <dimension ref="A1:F88"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F35" sqref="F35"/>
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C88" sqref="C88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1150,7 +1150,7 @@
     <col min="4" max="11" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1167,10 +1167,10 @@
         <v>4</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>44818.990344537036</v>
       </c>
@@ -1187,7 +1187,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>45029.261823807872</v>
       </c>
@@ -1204,7 +1204,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>13</v>
       </c>
@@ -1218,7 +1218,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>13</v>
       </c>
@@ -1232,7 +1232,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>13</v>
       </c>
@@ -1246,7 +1246,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>13</v>
       </c>
@@ -1260,7 +1260,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>13</v>
       </c>
@@ -1274,7 +1274,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>13</v>
       </c>
@@ -1288,7 +1288,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>13</v>
       </c>
@@ -1302,7 +1302,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>13</v>
       </c>
@@ -1316,7 +1316,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>13</v>
       </c>
@@ -1330,7 +1330,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>13</v>
       </c>
@@ -1344,7 +1344,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>13</v>
       </c>
@@ -1358,7 +1358,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>13</v>
       </c>
@@ -1372,7 +1372,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>13</v>
       </c>
@@ -1386,7 +1386,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>13</v>
       </c>
@@ -1400,7 +1400,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>13</v>
       </c>
@@ -1414,7 +1414,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>13</v>
       </c>
@@ -1428,7 +1428,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>13</v>
       </c>
@@ -1442,7 +1442,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>13</v>
       </c>
@@ -1456,7 +1456,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>13</v>
       </c>
@@ -1470,7 +1470,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>13</v>
       </c>
@@ -1484,7 +1484,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>13</v>
       </c>
@@ -1498,7 +1498,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>13</v>
       </c>
@@ -1512,7 +1512,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>13</v>
       </c>
@@ -1526,7 +1526,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>13</v>
       </c>
@@ -1540,7 +1540,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>13</v>
       </c>
@@ -1554,7 +1554,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>13</v>
       </c>
@@ -1568,7 +1568,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>13</v>
       </c>
@@ -1582,7 +1582,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>13</v>
       </c>
@@ -1596,7 +1596,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>13</v>
       </c>
@@ -1610,7 +1610,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>13</v>
       </c>
@@ -1624,7 +1624,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>13</v>
       </c>
@@ -1638,7 +1638,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>13</v>
       </c>
@@ -1652,7 +1652,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>13</v>
       </c>
@@ -1666,7 +1666,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>13</v>
       </c>
@@ -1687,14 +1687,14 @@
       <c r="B38" t="s">
         <v>114</v>
       </c>
-      <c r="C38" t="s">
-        <v>164</v>
+      <c r="C38" s="3" t="s">
+        <v>203</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>214</v>
+        <v>164</v>
       </c>
       <c r="F38" t="s">
-        <v>218</v>
+        <v>167</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1704,14 +1704,14 @@
       <c r="B39" t="s">
         <v>115</v>
       </c>
-      <c r="C39" t="s">
-        <v>165</v>
+      <c r="C39" s="3" t="s">
+        <v>204</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>214</v>
+        <v>164</v>
       </c>
       <c r="F39" t="s">
-        <v>219</v>
+        <v>168</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1721,14 +1721,14 @@
       <c r="B40" t="s">
         <v>116</v>
       </c>
-      <c r="C40" t="s">
-        <v>166</v>
+      <c r="C40" s="3" t="s">
+        <v>205</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>214</v>
+        <v>164</v>
       </c>
       <c r="F40" t="s">
-        <v>220</v>
+        <v>169</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1738,14 +1738,14 @@
       <c r="B41" t="s">
         <v>117</v>
       </c>
-      <c r="C41" t="s">
-        <v>167</v>
+      <c r="C41" s="3" t="s">
+        <v>206</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>214</v>
+        <v>164</v>
       </c>
       <c r="F41" t="s">
-        <v>221</v>
+        <v>170</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1755,14 +1755,14 @@
       <c r="B42" t="s">
         <v>118</v>
       </c>
-      <c r="C42" t="s">
-        <v>168</v>
+      <c r="C42" s="3" t="s">
+        <v>207</v>
       </c>
       <c r="D42" s="7" t="s">
-        <v>214</v>
+        <v>164</v>
       </c>
       <c r="F42" t="s">
-        <v>222</v>
+        <v>171</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1772,14 +1772,14 @@
       <c r="B43" t="s">
         <v>119</v>
       </c>
-      <c r="C43" t="s">
-        <v>169</v>
+      <c r="C43" s="3" t="s">
+        <v>208</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>214</v>
+        <v>164</v>
       </c>
       <c r="F43" t="s">
-        <v>223</v>
+        <v>172</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1789,14 +1789,14 @@
       <c r="B44" t="s">
         <v>120</v>
       </c>
-      <c r="C44" t="s">
-        <v>170</v>
+      <c r="C44" s="3" t="s">
+        <v>209</v>
       </c>
       <c r="D44" s="7" t="s">
-        <v>214</v>
+        <v>164</v>
       </c>
       <c r="F44" t="s">
-        <v>224</v>
+        <v>173</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1806,14 +1806,14 @@
       <c r="B45" t="s">
         <v>121</v>
       </c>
-      <c r="C45" t="s">
-        <v>171</v>
+      <c r="C45" s="3" t="s">
+        <v>210</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>214</v>
+        <v>164</v>
       </c>
       <c r="F45" t="s">
-        <v>225</v>
+        <v>174</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1823,14 +1823,14 @@
       <c r="B46" t="s">
         <v>122</v>
       </c>
-      <c r="C46" t="s">
-        <v>172</v>
+      <c r="C46" s="3" t="s">
+        <v>211</v>
       </c>
       <c r="D46" s="7" t="s">
-        <v>214</v>
+        <v>164</v>
       </c>
       <c r="F46" t="s">
-        <v>226</v>
+        <v>175</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1840,14 +1840,14 @@
       <c r="B47" t="s">
         <v>123</v>
       </c>
-      <c r="C47" t="s">
-        <v>173</v>
+      <c r="C47" s="3" t="s">
+        <v>212</v>
       </c>
       <c r="D47" s="7" t="s">
-        <v>214</v>
+        <v>164</v>
       </c>
       <c r="F47" t="s">
-        <v>227</v>
+        <v>176</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1857,14 +1857,14 @@
       <c r="B48" t="s">
         <v>124</v>
       </c>
-      <c r="C48" t="s">
-        <v>174</v>
+      <c r="C48" s="3" t="s">
+        <v>213</v>
       </c>
       <c r="D48" s="7" t="s">
-        <v>214</v>
+        <v>164</v>
       </c>
       <c r="F48" t="s">
-        <v>228</v>
+        <v>177</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1874,14 +1874,14 @@
       <c r="B49" t="s">
         <v>125</v>
       </c>
-      <c r="C49" t="s">
-        <v>175</v>
+      <c r="C49" s="3" t="s">
+        <v>214</v>
       </c>
       <c r="D49" s="7" t="s">
-        <v>214</v>
+        <v>164</v>
       </c>
       <c r="F49" t="s">
-        <v>224</v>
+        <v>173</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1891,14 +1891,14 @@
       <c r="B50" t="s">
         <v>126</v>
       </c>
-      <c r="C50" t="s">
-        <v>176</v>
+      <c r="C50" s="3" t="s">
+        <v>215</v>
       </c>
       <c r="D50" s="7" t="s">
-        <v>214</v>
+        <v>164</v>
       </c>
       <c r="F50" t="s">
-        <v>226</v>
+        <v>175</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1908,14 +1908,14 @@
       <c r="B51" t="s">
         <v>127</v>
       </c>
-      <c r="C51" t="s">
-        <v>177</v>
+      <c r="C51" s="3" t="s">
+        <v>216</v>
       </c>
       <c r="D51" s="7" t="s">
-        <v>214</v>
+        <v>164</v>
       </c>
       <c r="F51" t="s">
-        <v>223</v>
+        <v>172</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1925,14 +1925,14 @@
       <c r="B52" t="s">
         <v>128</v>
       </c>
-      <c r="C52" t="s">
-        <v>178</v>
+      <c r="C52" s="3" t="s">
+        <v>217</v>
       </c>
       <c r="D52" s="7" t="s">
-        <v>214</v>
+        <v>164</v>
       </c>
       <c r="F52" t="s">
-        <v>218</v>
+        <v>167</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1942,14 +1942,14 @@
       <c r="B53" t="s">
         <v>129</v>
       </c>
-      <c r="C53" t="s">
-        <v>179</v>
+      <c r="C53" s="3" t="s">
+        <v>218</v>
       </c>
       <c r="D53" s="7" t="s">
-        <v>214</v>
+        <v>164</v>
       </c>
       <c r="F53" t="s">
-        <v>218</v>
+        <v>167</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1959,14 +1959,14 @@
       <c r="B54" t="s">
         <v>130</v>
       </c>
-      <c r="C54" t="s">
-        <v>180</v>
+      <c r="C54" s="3" t="s">
+        <v>219</v>
       </c>
       <c r="D54" s="7" t="s">
-        <v>214</v>
+        <v>164</v>
       </c>
       <c r="F54" t="s">
-        <v>229</v>
+        <v>178</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1976,14 +1976,14 @@
       <c r="B55" t="s">
         <v>131</v>
       </c>
-      <c r="C55" t="s">
-        <v>181</v>
+      <c r="C55" s="3" t="s">
+        <v>220</v>
       </c>
       <c r="D55" s="7" t="s">
-        <v>214</v>
+        <v>164</v>
       </c>
       <c r="F55" t="s">
-        <v>230</v>
+        <v>179</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1993,14 +1993,14 @@
       <c r="B56" t="s">
         <v>132</v>
       </c>
-      <c r="C56" t="s">
-        <v>182</v>
+      <c r="C56" s="3" t="s">
+        <v>221</v>
       </c>
       <c r="D56" s="7" t="s">
-        <v>214</v>
+        <v>164</v>
       </c>
       <c r="F56" t="s">
-        <v>231</v>
+        <v>180</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2010,14 +2010,14 @@
       <c r="B57" t="s">
         <v>133</v>
       </c>
-      <c r="C57" t="s">
-        <v>183</v>
+      <c r="C57" s="3" t="s">
+        <v>222</v>
       </c>
       <c r="D57" s="7" t="s">
-        <v>214</v>
+        <v>164</v>
       </c>
       <c r="F57" t="s">
-        <v>232</v>
+        <v>181</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2027,14 +2027,14 @@
       <c r="B58" t="s">
         <v>134</v>
       </c>
-      <c r="C58" t="s">
-        <v>184</v>
+      <c r="C58" s="3" t="s">
+        <v>223</v>
       </c>
       <c r="D58" s="7" t="s">
-        <v>214</v>
+        <v>164</v>
       </c>
       <c r="F58" t="s">
-        <v>229</v>
+        <v>178</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2044,14 +2044,14 @@
       <c r="B59" t="s">
         <v>135</v>
       </c>
-      <c r="C59" t="s">
-        <v>185</v>
+      <c r="C59" s="3" t="s">
+        <v>224</v>
       </c>
       <c r="D59" s="7" t="s">
-        <v>214</v>
+        <v>164</v>
       </c>
       <c r="F59" t="s">
-        <v>233</v>
+        <v>182</v>
       </c>
     </row>
     <row r="60" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2061,14 +2061,14 @@
       <c r="B60" t="s">
         <v>136</v>
       </c>
-      <c r="C60" t="s">
-        <v>186</v>
+      <c r="C60" s="3" t="s">
+        <v>225</v>
       </c>
       <c r="D60" s="7" t="s">
-        <v>214</v>
+        <v>164</v>
       </c>
       <c r="F60" t="s">
-        <v>221</v>
+        <v>170</v>
       </c>
     </row>
     <row r="61" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2078,14 +2078,14 @@
       <c r="B61" t="s">
         <v>137</v>
       </c>
-      <c r="C61" t="s">
-        <v>187</v>
+      <c r="C61" s="3" t="s">
+        <v>226</v>
       </c>
       <c r="D61" s="7" t="s">
-        <v>214</v>
+        <v>164</v>
       </c>
       <c r="F61" t="s">
-        <v>234</v>
+        <v>183</v>
       </c>
     </row>
     <row r="62" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2095,14 +2095,14 @@
       <c r="B62" t="s">
         <v>138</v>
       </c>
-      <c r="C62" t="s">
-        <v>188</v>
+      <c r="C62" s="3" t="s">
+        <v>227</v>
       </c>
       <c r="D62" s="7" t="s">
-        <v>214</v>
+        <v>164</v>
       </c>
       <c r="F62" t="s">
-        <v>221</v>
+        <v>170</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2112,14 +2112,14 @@
       <c r="B63" t="s">
         <v>139</v>
       </c>
-      <c r="C63" t="s">
-        <v>189</v>
+      <c r="C63" s="3" t="s">
+        <v>228</v>
       </c>
       <c r="D63" s="7" t="s">
-        <v>214</v>
+        <v>164</v>
       </c>
       <c r="F63" t="s">
-        <v>235</v>
+        <v>184</v>
       </c>
     </row>
     <row r="64" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2129,14 +2129,14 @@
       <c r="B64" t="s">
         <v>140</v>
       </c>
-      <c r="C64" t="s">
-        <v>190</v>
+      <c r="C64" s="3" t="s">
+        <v>229</v>
       </c>
       <c r="D64" s="7" t="s">
-        <v>214</v>
+        <v>164</v>
       </c>
       <c r="F64" t="s">
-        <v>236</v>
+        <v>185</v>
       </c>
     </row>
     <row r="65" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2146,14 +2146,14 @@
       <c r="B65" t="s">
         <v>141</v>
       </c>
-      <c r="C65" t="s">
-        <v>191</v>
+      <c r="C65" s="3" t="s">
+        <v>230</v>
       </c>
       <c r="D65" s="7" t="s">
-        <v>214</v>
+        <v>164</v>
       </c>
       <c r="F65" t="s">
-        <v>230</v>
+        <v>179</v>
       </c>
     </row>
     <row r="66" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2163,14 +2163,14 @@
       <c r="B66" t="s">
         <v>142</v>
       </c>
-      <c r="C66" t="s">
-        <v>192</v>
+      <c r="C66" s="3" t="s">
+        <v>231</v>
       </c>
       <c r="D66" s="7" t="s">
-        <v>214</v>
+        <v>164</v>
       </c>
       <c r="F66" t="s">
-        <v>237</v>
+        <v>186</v>
       </c>
     </row>
     <row r="67" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2180,14 +2180,14 @@
       <c r="B67" t="s">
         <v>143</v>
       </c>
-      <c r="C67" t="s">
-        <v>193</v>
+      <c r="C67" s="3" t="s">
+        <v>232</v>
       </c>
       <c r="D67" s="7" t="s">
-        <v>214</v>
+        <v>164</v>
       </c>
       <c r="F67" t="s">
-        <v>238</v>
+        <v>187</v>
       </c>
     </row>
     <row r="68" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2197,14 +2197,14 @@
       <c r="B68" t="s">
         <v>144</v>
       </c>
-      <c r="C68" t="s">
-        <v>194</v>
+      <c r="C68" s="3" t="s">
+        <v>233</v>
       </c>
       <c r="D68" s="7" t="s">
-        <v>214</v>
+        <v>164</v>
       </c>
       <c r="F68" t="s">
-        <v>232</v>
+        <v>181</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2214,14 +2214,14 @@
       <c r="B69" t="s">
         <v>145</v>
       </c>
-      <c r="C69" t="s">
-        <v>195</v>
+      <c r="C69" s="3" t="s">
+        <v>234</v>
       </c>
       <c r="D69" s="7" t="s">
-        <v>214</v>
+        <v>164</v>
       </c>
       <c r="F69" t="s">
-        <v>239</v>
+        <v>188</v>
       </c>
     </row>
     <row r="70" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2231,14 +2231,14 @@
       <c r="B70" t="s">
         <v>146</v>
       </c>
-      <c r="C70" t="s">
-        <v>196</v>
+      <c r="C70" s="3" t="s">
+        <v>235</v>
       </c>
       <c r="D70" s="7" t="s">
-        <v>214</v>
+        <v>164</v>
       </c>
       <c r="F70" t="s">
-        <v>221</v>
+        <v>170</v>
       </c>
     </row>
     <row r="71" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2248,14 +2248,14 @@
       <c r="B71" t="s">
         <v>147</v>
       </c>
-      <c r="C71" t="s">
-        <v>197</v>
+      <c r="C71" s="3" t="s">
+        <v>236</v>
       </c>
       <c r="D71" s="7" t="s">
-        <v>214</v>
+        <v>164</v>
       </c>
       <c r="F71" t="s">
-        <v>240</v>
+        <v>189</v>
       </c>
     </row>
     <row r="72" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2265,14 +2265,14 @@
       <c r="B72" t="s">
         <v>148</v>
       </c>
-      <c r="C72" t="s">
-        <v>198</v>
+      <c r="C72" s="3" t="s">
+        <v>237</v>
       </c>
       <c r="D72" s="7" t="s">
-        <v>214</v>
+        <v>164</v>
       </c>
       <c r="F72" t="s">
-        <v>237</v>
+        <v>186</v>
       </c>
     </row>
     <row r="73" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2282,14 +2282,14 @@
       <c r="B73" t="s">
         <v>149</v>
       </c>
-      <c r="C73" t="s">
-        <v>199</v>
+      <c r="C73" s="3" t="s">
+        <v>238</v>
       </c>
       <c r="D73" s="7" t="s">
-        <v>214</v>
+        <v>164</v>
       </c>
       <c r="F73" t="s">
-        <v>241</v>
+        <v>190</v>
       </c>
     </row>
     <row r="74" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2299,14 +2299,14 @@
       <c r="B74" t="s">
         <v>150</v>
       </c>
-      <c r="C74" t="s">
-        <v>200</v>
+      <c r="C74" s="3" t="s">
+        <v>239</v>
       </c>
       <c r="D74" s="7" t="s">
-        <v>214</v>
+        <v>164</v>
       </c>
       <c r="F74" t="s">
-        <v>239</v>
+        <v>188</v>
       </c>
     </row>
     <row r="75" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2316,14 +2316,14 @@
       <c r="B75" t="s">
         <v>151</v>
       </c>
-      <c r="C75" t="s">
-        <v>201</v>
+      <c r="C75" s="3" t="s">
+        <v>240</v>
       </c>
       <c r="D75" s="7" t="s">
-        <v>214</v>
+        <v>164</v>
       </c>
       <c r="F75" t="s">
-        <v>242</v>
+        <v>191</v>
       </c>
     </row>
     <row r="76" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2333,14 +2333,14 @@
       <c r="B76" t="s">
         <v>152</v>
       </c>
-      <c r="C76" t="s">
-        <v>202</v>
+      <c r="C76" s="3" t="s">
+        <v>241</v>
       </c>
       <c r="D76" s="7" t="s">
-        <v>214</v>
+        <v>164</v>
       </c>
       <c r="F76" t="s">
-        <v>243</v>
+        <v>192</v>
       </c>
     </row>
     <row r="77" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2350,14 +2350,14 @@
       <c r="B77" t="s">
         <v>153</v>
       </c>
-      <c r="C77" t="s">
-        <v>203</v>
+      <c r="C77" s="3" t="s">
+        <v>242</v>
       </c>
       <c r="D77" s="7" t="s">
-        <v>214</v>
+        <v>164</v>
       </c>
       <c r="F77" t="s">
-        <v>244</v>
+        <v>193</v>
       </c>
     </row>
     <row r="78" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2367,14 +2367,14 @@
       <c r="B78" t="s">
         <v>154</v>
       </c>
-      <c r="C78" t="s">
-        <v>204</v>
+      <c r="C78" s="3" t="s">
+        <v>243</v>
       </c>
       <c r="D78" s="7" t="s">
-        <v>214</v>
+        <v>164</v>
       </c>
       <c r="F78" t="s">
-        <v>228</v>
+        <v>177</v>
       </c>
     </row>
     <row r="79" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2384,14 +2384,14 @@
       <c r="B79" t="s">
         <v>155</v>
       </c>
-      <c r="C79" t="s">
-        <v>205</v>
+      <c r="C79" s="3" t="s">
+        <v>244</v>
       </c>
       <c r="D79" s="7" t="s">
-        <v>214</v>
+        <v>164</v>
       </c>
       <c r="F79" t="s">
-        <v>245</v>
+        <v>194</v>
       </c>
     </row>
     <row r="80" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2401,14 +2401,14 @@
       <c r="B80" t="s">
         <v>156</v>
       </c>
-      <c r="C80" t="s">
-        <v>206</v>
+      <c r="C80" s="3" t="s">
+        <v>245</v>
       </c>
       <c r="D80" s="7" t="s">
-        <v>214</v>
+        <v>164</v>
       </c>
       <c r="F80" t="s">
-        <v>246</v>
+        <v>195</v>
       </c>
     </row>
     <row r="81" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2418,14 +2418,14 @@
       <c r="B81" t="s">
         <v>157</v>
       </c>
-      <c r="C81" t="s">
-        <v>207</v>
+      <c r="C81" s="3" t="s">
+        <v>246</v>
       </c>
       <c r="D81" s="7" t="s">
-        <v>214</v>
+        <v>164</v>
       </c>
       <c r="F81" t="s">
-        <v>247</v>
+        <v>196</v>
       </c>
     </row>
     <row r="82" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2435,14 +2435,14 @@
       <c r="B82" t="s">
         <v>158</v>
       </c>
-      <c r="C82" t="s">
-        <v>208</v>
+      <c r="C82" s="3" t="s">
+        <v>247</v>
       </c>
       <c r="D82" s="7" t="s">
-        <v>214</v>
+        <v>164</v>
       </c>
       <c r="F82" t="s">
-        <v>248</v>
+        <v>197</v>
       </c>
     </row>
     <row r="83" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2452,14 +2452,14 @@
       <c r="B83" t="s">
         <v>159</v>
       </c>
-      <c r="C83" t="s">
-        <v>209</v>
+      <c r="C83" s="3" t="s">
+        <v>248</v>
       </c>
       <c r="D83" s="7" t="s">
-        <v>214</v>
+        <v>164</v>
       </c>
       <c r="F83" t="s">
-        <v>249</v>
+        <v>198</v>
       </c>
     </row>
     <row r="84" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2469,14 +2469,14 @@
       <c r="B84" t="s">
         <v>160</v>
       </c>
-      <c r="C84" t="s">
-        <v>210</v>
+      <c r="C84" s="3" t="s">
+        <v>249</v>
       </c>
       <c r="D84" s="7" t="s">
-        <v>214</v>
+        <v>164</v>
       </c>
       <c r="F84" t="s">
-        <v>250</v>
+        <v>199</v>
       </c>
     </row>
     <row r="85" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2486,14 +2486,14 @@
       <c r="B85" t="s">
         <v>161</v>
       </c>
-      <c r="C85" t="s">
-        <v>211</v>
+      <c r="C85" s="3" t="s">
+        <v>250</v>
       </c>
       <c r="D85" s="7" t="s">
-        <v>214</v>
+        <v>164</v>
       </c>
       <c r="F85" t="s">
-        <v>234</v>
+        <v>183</v>
       </c>
     </row>
     <row r="86" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2503,14 +2503,14 @@
       <c r="B86" t="s">
         <v>162</v>
       </c>
-      <c r="C86" t="s">
-        <v>212</v>
+      <c r="C86" s="3" t="s">
+        <v>251</v>
       </c>
       <c r="D86" s="7" t="s">
-        <v>214</v>
+        <v>164</v>
       </c>
       <c r="F86" t="s">
-        <v>251</v>
+        <v>200</v>
       </c>
     </row>
     <row r="87" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2520,14 +2520,14 @@
       <c r="B87" t="s">
         <v>163</v>
       </c>
-      <c r="C87" t="s">
-        <v>213</v>
+      <c r="C87" s="3" t="s">
+        <v>252</v>
       </c>
       <c r="D87" s="7" t="s">
-        <v>214</v>
+        <v>164</v>
       </c>
       <c r="F87" t="s">
-        <v>241</v>
+        <v>190</v>
       </c>
     </row>
     <row r="88" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2535,16 +2535,16 @@
         <v>13</v>
       </c>
       <c r="B88" s="6" t="s">
-        <v>216</v>
-      </c>
-      <c r="C88" s="6" t="s">
-        <v>215</v>
+        <v>165</v>
+      </c>
+      <c r="C88" s="3" t="s">
+        <v>202</v>
       </c>
       <c r="D88" s="7" t="s">
-        <v>214</v>
+        <v>164</v>
       </c>
       <c r="F88" t="s">
-        <v>252</v>
+        <v>201</v>
       </c>
     </row>
   </sheetData>
@@ -2552,5 +2552,6 @@
     <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update chemecho queries for resubmission
</commit_message>
<xml_diff>
--- a/assets/compendium.xlsx
+++ b/assets/compendium.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tharwood\Desktop\ChemEcho\fixed_queries\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tharwood\Desktop\ChemEcho\SecondSubmissionACS\massql\MassQL_Dashboard\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{513BAA34-3A2F-4A0B-BC4D-A8EB3E7AA72D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9B5E42B-4FB9-4082-ACAE-9C6D1FB27758}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="16125" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="253">
   <si>
     <t>Timestamp</t>
   </si>
@@ -425,421 +425,421 @@
     <t>Roland Kersten</t>
   </si>
   <si>
-    <t>Benzene ring substructure (ML-Generated using ChemEcho) [Ionization mode: negative]</t>
-  </si>
-  <si>
-    <t>Sulfonic acid functional group ('O=S(=O)(O)*1') (ML-generated using ChemEcho) [Ionization mode: negative]</t>
-  </si>
-  <si>
-    <t>Glycerophosphoinositols from NP-Classifier (ML-generated using ChemEcho) [Ionization mode: negative]</t>
-  </si>
-  <si>
-    <t>Steranes (CC12C3CC(*1)C4(C)C(CCC4*1)C3C(*1)C(*1)C1CC(*1)CC2*1) (ML-generated using ChemEcho) [Ionization mode: positive]</t>
-  </si>
-  <si>
-    <t>Beta-lactams from NP-Classifier (ML-generated using ChemEcho) [Ionization mode: positive]</t>
-  </si>
-  <si>
-    <t>Cholane steroids from NP-Classifier (ML-generated using ChemEcho) [Ionization mode: negative]</t>
-  </si>
-  <si>
-    <t>Glycerophospholipids from NP-Classifier (ML-generated using ChemEcho) [Ionization mode: negative]</t>
-  </si>
-  <si>
-    <t>Flavonoids from NP-Classifier (ML-generated using ChemEcho) [Ionization mode: negative]</t>
-  </si>
-  <si>
-    <t>Nucleosides from NP-Classifier (ML-generated using ChemEcho) [Ionization mode: positive]</t>
-  </si>
-  <si>
-    <t>Tetrahydropyran ring substructure (ML-generated using ChemEcho) [Ionization mode: negative]</t>
-  </si>
-  <si>
-    <t>Oligopeptides from NP-Classifier (ML-generated using ChemEcho) [Ionization mode: negative]</t>
-  </si>
-  <si>
-    <t>Glycerophospholipids from NP-Classifier (ML-generated using ChemEcho) [Ionization mode: positive]</t>
-  </si>
-  <si>
-    <t>Nucleosides from NP-Classifier (ML-generated using ChemEcho) [Ionization mode: negative]</t>
-  </si>
-  <si>
-    <t>Cholane steroids from NP-Classifier (ML-generated using ChemEcho) [Ionization mode: positive]</t>
-  </si>
-  <si>
-    <t>Benzene ring substructure with 4 attachment points (C1=C(*1)C=C(*1)C(*1)=C1*1) (ML-generated using ChemEcho) [Ionization mode: positive]</t>
-  </si>
-  <si>
-    <t>Benzene ring substructure (ML-generated using ChemEcho) [Ionization mode: positive]</t>
-  </si>
-  <si>
-    <t>Saccharides from NP-Classifier (ML-generated using ChemEcho) [Ionization mode: positive]</t>
-  </si>
-  <si>
-    <t>Eicosanoids from NP-Classifier (ML-generated using ChemEcho) [Ionization mode: negative]</t>
-  </si>
-  <si>
-    <t>Picene-like substructure ([#6]1=[#6]2-[#6]3-[#6]-[#6]-[#6]-[#6]-[#6]-3-[#6]-[#6]-[#6]-2-[#6]2-[#6]-[#6]-[#6]3-[#6]-[#6]-[#6]-[#6]-[#6]-3-[#6]-2-[#6]-1) (ML-generated using ChemEcho) [Ionization mode: negative]</t>
-  </si>
-  <si>
-    <t>Xanthone substructure ([#8]=[#6]1:[#6]2:[#6]:[#6]:[#6]:[#6]:[#6]:2:[#8]:[#6]2:[#6]:[#6]:[#6]:[#6]:[#6]:1:2) (ML-generated using ChemEcho) [Ionization mode: negative]</t>
-  </si>
-  <si>
-    <t>Saccharides from NP-Classifier (ML-generated using ChemEcho) [Ionization mode: negative]</t>
-  </si>
-  <si>
-    <t>Indole substructure (C1=CC=C2C(=C1)NC=C2*1) (ML-generated using ChemEcho) [Ionization mode: positive]</t>
-  </si>
-  <si>
-    <t>Steranes ([#6]1-[#6]-[#6]-[#6]2-[#6](-[#6]-1)-[#6]-[#6]-[#6]1-[#6]3-[#6]-[#6]-[#6]-[#6]-3-[#6]-[#6]-[#6]-2-1) (ML-generated using ChemEcho) [Ionization mode: negative]</t>
-  </si>
-  <si>
-    <t>Fatty Acids and Conjugates from NP-Classifier (ML-generated using ChemEcho) [Ionization mode: negative]</t>
-  </si>
-  <si>
-    <t>Steranes (CC12CCC(*1)CC1CC(*1)C1C2CC(*1)C2(C)C1CCC2*1) (ML-generated using ChemEcho) [Ionization mode: negative]</t>
-  </si>
-  <si>
-    <t>Isoflavonoids from NP-Classifier (ML-generated using ChemEcho) [Ionization mode: negative]</t>
-  </si>
-  <si>
-    <t>Imidazole substructure with 3 attachment points (N1=C(*1)NC(*1)=C1*1) (ML-generated using ChemEcho) [Ionization mode: positive]</t>
-  </si>
-  <si>
-    <t>Eicosanoids from NP-Classifier (ML-generated using ChemEcho) [Ionization mode: positive]</t>
-  </si>
-  <si>
-    <t>Steroids from NP-Classifier (ML-generated using ChemEcho) [Ionization mode: negative]</t>
-  </si>
-  <si>
-    <t>Triterpenoids from NP-Classifier (ML-generated using ChemEcho) [Ionization mode: negative]</t>
-  </si>
-  <si>
-    <t>Xanthones from NP-Classifier (ML-generated using ChemEcho) [Ionization mode: negative]</t>
-  </si>
-  <si>
-    <t>Linear polyketides from NP-Classifier (ML-generated using ChemEcho) [Ionization mode: positive]</t>
-  </si>
-  <si>
-    <t>Steranes ([#6]1-[#6]-[#6]-[#6]2-[#6](-[#6]-1)-[#6]-[#6]-[#6]1-[#6]3-[#6]-[#6]-[#6]-[#6]-3-[#6]-[#6]-[#6]-2-1) (ML-generated using ChemEcho) [Ionization mode: positive]</t>
-  </si>
-  <si>
-    <t>Fatty esters from NP-Classifier (ML-generated using ChemEcho) [Ionization mode: positive]</t>
-  </si>
-  <si>
-    <t>Steroids from NP-Classifier (ML-generated using ChemEcho) [Ionization mode: positive]</t>
-  </si>
-  <si>
-    <t>Macrolides from NP-Classifier (ML-generated using ChemEcho) [Ionization mode: negative]</t>
-  </si>
-  <si>
-    <t>Linear polyketide from NP-Classifier (ML-generated using ChemEcho) [Ionization mode: negative]</t>
-  </si>
-  <si>
-    <t>Monoterpenoids from NP-Classifier (ML-generated using ChemEcho) [Ionization mode: negative]</t>
-  </si>
-  <si>
-    <t>Stilbenoids from NP-Classifier (ML-generated using ChemEcho) [Ionization mode: negative]</t>
-  </si>
-  <si>
-    <t>Lignans from NP-Classifier (ML-generated using ChemEcho) [Ionization mode: negative]</t>
-  </si>
-  <si>
-    <t>Oligopeptides from NP-Classifier (ML-generated using ChemEcho) [Ionization mode: positive]</t>
-  </si>
-  <si>
-    <t>Pyrimidine substructure ([#6]1:[#6]:[#7]:[#6]:[#7]:[#6]:1) (ML-generated using ChemEcho) [Ionization mode: positive]</t>
-  </si>
-  <si>
-    <t>Pyran substructure ([#6]1-[#6]-[#6]-[#8]-[#6]-[#6]-1) (ML-generated using ChemEcho) [Ionization mode: positive]</t>
-  </si>
-  <si>
-    <t>Histidine alkaloids from NP-Classifier (ML-generated using ChemEcho) [Ionization mode: negative]</t>
-  </si>
-  <si>
-    <t>Naphthalenes from NP-Classifier (ML-generated using ChemEcho) [Ionization mode: negative]</t>
-  </si>
-  <si>
-    <t>Small peptides from NP-Classifier (ML-generated using ChemEcho) [Ionization mode: negative]</t>
-  </si>
-  <si>
-    <t>Coumarins from NP-Classifier (ML-generated using ChemEcho) [Ionization mode: negative]</t>
-  </si>
-  <si>
-    <t>Fatty Acids and Conjugate from NP-Classifier (ML-generated using ChemEcho) [Ionization mode: positive]</t>
-  </si>
-  <si>
-    <t>Phenylpropanoids (C6-C3) from NP-Classifier (ML-generated using ChemEcho) [Ionization mode: negative]</t>
-  </si>
-  <si>
-    <t>Macrolides from NP-Classifier (ML-generated using ChemEcho) [Ionization mode: positive]</t>
-  </si>
-  <si>
     <t>Thomas Harwood and Ben Bowen</t>
   </si>
   <si>
-    <t>Perfluoroalkyl and Polyfluoroalkyl Substances (FCC(F)F substructure) (ML-generated using ChemEcho) [Ionization mode: negative]</t>
-  </si>
-  <si>
     <t>Representative SMILES</t>
   </si>
   <si>
-    <t>C1=CC=CC=C1</t>
-  </si>
-  <si>
     <t>O=S(=O)(O)</t>
   </si>
   <si>
-    <t>C([C@H](COP(=O)(O)OC1[C@@H]([C@H](C([C@H]([C@H]1O)O)O)O)O)O)O</t>
-  </si>
-  <si>
     <t>C[C@@]12CCC[C@H]1[C@@H]3CC[C@H]4CCCC[C@@]4([C@H]3CC2)C</t>
   </si>
   <si>
-    <t>C1CNC1=O</t>
-  </si>
-  <si>
-    <t>CCC[C@@H](C)[C@H]1CC[C@@H]2[C@@]1(CC[C@H]3[C@H]2CC[C@H]4[C@@]3(CCCC4)C)C</t>
-  </si>
-  <si>
     <t>CCCCCCCC/C=C\CCCCCCCC(=O)OC[C@H](COP(=O)(O)O)OC(=O)CCCCCCC/C=C\C/C=C\C/C=C\CC</t>
   </si>
   <si>
-    <t>C1=CC=C(C=C1)C2=CC(=O)C3=CC=CC=C3O2</t>
-  </si>
-  <si>
-    <t>C1=NC2=C(N1[C@H]3[C@@H]([C@@H]([C@H](O3)CO)O)O)N=C(NC2=O)N</t>
-  </si>
-  <si>
     <t>C1CCOCC1</t>
   </si>
   <si>
-    <t>C1=C(NC=N1)C[C@@H](C(=O)O)NC(=O)CCN</t>
-  </si>
-  <si>
-    <t>C([C@@H]1[C@H]([C@@H]([C@H](C(O1)O)O)O)O)O</t>
-  </si>
-  <si>
-    <t>CCCCC[C@@H](/C=C/C=C\C/C=C\C/C=C\CCCC(=O)O)O</t>
-  </si>
-  <si>
-    <t>C1=C2C3CCCCC3CCC2C2CCC3CCCCC3C2C1</t>
-  </si>
-  <si>
-    <t>C1=CC=C2C(=C1)C(=O)C3=CC=CC=C3O2</t>
-  </si>
-  <si>
     <t>C1=CC=C2C(=C1)C=CN2</t>
   </si>
   <si>
-    <t>CCCCCCCCCCCC(=O)O</t>
-  </si>
-  <si>
-    <t>C1=CC=C(C=C1)C2=COC3=CC=CC=C3C2=O</t>
-  </si>
-  <si>
-    <t>C1=CN=CN1</t>
-  </si>
-  <si>
-    <t>C[C@H](CCC=C(C)C)[C@H]1CC[C@@]2([C@@]1(CCC3=C2CC[C@@H]4[C@@]3(CC[C@@H](C4(C)C)O)C)C)C</t>
-  </si>
-  <si>
-    <t>CC1(CCC2(CCC3(C(=CCC4C3(CC=C5C4(CC(C(C5(C)O)O)O)C)C)C2C1)C)C(=O)O)C</t>
-  </si>
-  <si>
-    <t>CC(=O)CC(=O)CC(=O)CC(=O)O</t>
-  </si>
-  <si>
-    <t>CCCCCCCCCCCCCCCC(=O)OC</t>
-  </si>
-  <si>
-    <t>CC[C@@H]1[C@@]([C@@H]([C@H](C(=O)[C@@H](C[C@@]([C@@H]([C@H]([C@@H]([C@H](C(=O)O1)C)O[C@H]2C[C@@]([C@H]([C@@H](O2)C)O)(C)OC)C)O[C@H]3[C@@H]([C@H](C[C@H](O3)C)N(C)C)O)(C)O)C)C)O)(C)O</t>
-  </si>
-  <si>
-    <t>CC1CCC(C(C1)O)C(C)C</t>
-  </si>
-  <si>
-    <t>C1=CC(=CC=C1/C=C/C2=CC(=CC(=C2)O)O)O</t>
-  </si>
-  <si>
-    <t>COC1=C(C=CC(=C1)C[C@@H](CO)[C@@H](CC2=CC(=C(C=C2)O)OC)CO)O</t>
-  </si>
-  <si>
-    <t>C1=CN=CN=C1</t>
-  </si>
-  <si>
     <t>C1C=CC=CO1</t>
   </si>
   <si>
-    <t>C1=C(NC=N1)C[C@@H](C(=O)O)</t>
-  </si>
-  <si>
-    <t>C1=CC=C2C=CC=CC2=C1</t>
-  </si>
-  <si>
-    <t>C1C[C@H](N(C1)C(=O)[C@@H]2CCCN2C(=O)[C@H](CCCN=C(N)N)N)C(=O)NCC(=O)N[C@@H](CC3=CC=CC=C3)C(=O)N[C@@H](CO)C(=O)N4CCC[C@H]4C(=O)N[C@@H](CC5=CC=CC=C5)C(=O)N[C@@H](CCCN=C(N)N)C(=O)O</t>
-  </si>
-  <si>
-    <t>C1=CC=C2C(=C1)C=CC(=O)O2</t>
-  </si>
-  <si>
-    <t>C1=CC=C(C=C1)/C=C/C(=O)O</t>
-  </si>
-  <si>
     <t>FCC(F)F</t>
   </si>
   <si>
-    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C3F7):TOLERANCEPPM=10:INTENSITYPERCENT=0.001762:EXCLUDED AND MS2PROD=formula(C2H3O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.000012:EXCLUDED AND MS2PROD=formula(C2F5):TOLERANCEPPM=10:INTENSITYPERCENT=0.000752 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C3F7):TOLERANCEPPM=10:INTENSITYPERCENT=0.001762 AND MS2NL=formula(CH5F2O4P):TOLERANCEPPM=10:INTENSITYPERCENT=0.076847:EXCLUDED AND MS2PROD=formula(C12H11F3O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.015713:EXCLUDED</t>
-  </si>
-  <si>
-    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C2H3O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.003175:EXCLUDED AND MS2PROD=formula(O3P):TOLERANCEPPM=10:INTENSITYPERCENT=0.000194:EXCLUDED AND MS2PROD=formula(C8H6N):TOLERANCEPPM=10:INTENSITYPERCENT=0.000046:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C2H3O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.003175:EXCLUDED AND MS2PROD=formula(O3P):TOLERANCEPPM=10:INTENSITYPERCENT=0.000194:EXCLUDED AND MS2PROD=formula(C8H6N):TOLERANCEPPM=10:INTENSITYPERCENT=0.000046 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C2H3O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.003175:EXCLUDED AND MS2PROD=formula(O3P):TOLERANCEPPM=10:INTENSITYPERCENT=0.000194 AND MS2PROD=formula(C6H5O):TOLERANCEPPM=10:INTENSITYPERCENT=0.000727 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C2H3O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.003175 AND MS2PROD=formula(C8H5O):TOLERANCEPPM=10:INTENSITYPERCENT=0.000020:EXCLUDED AND MS2PROD=formula(C7H5O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.000566 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C2H3O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.003175 AND MS2PROD=formula(C8H5O):TOLERANCEPPM=10:INTENSITYPERCENT=0.000020 AND MS2PROD=formula(CHO2):TOLERANCEPPM=10:INTENSITYPERCENT=0.026492:EXCLUDED</t>
-  </si>
-  <si>
-    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(O3S):TOLERANCEPPM=10:INTENSITYPERCENT=0.000811:EXCLUDED AND MS2PROD=formula(HO4S):TOLERANCEPPM=10:INTENSITYPERCENT=0.001632:EXCLUDED AND MS2NL=formula(O3S):TOLERANCEPPM=10:INTENSITYPERCENT=0.002914 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(O3S):TOLERANCEPPM=10:INTENSITYPERCENT=0.000811:EXCLUDED AND MS2PROD=formula(HO4S):TOLERANCEPPM=10:INTENSITYPERCENT=0.001632 AND MS2PROD=formula(C7H11NO6S):TOLERANCEPPM=10:INTENSITYPERCENT=0.001570:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(O3S):TOLERANCEPPM=10:INTENSITYPERCENT=0.000811 AND MS2PROD=formula(NO2S):TOLERANCEPPM=10:INTENSITYPERCENT=0.002864:EXCLUDED AND MS2PROD=formula(C6H5NO2S):TOLERANCEPPM=10:INTENSITYPERCENT=0.000320:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(O3S):TOLERANCEPPM=10:INTENSITYPERCENT=0.000811 AND MS2PROD=formula(NO2S):TOLERANCEPPM=10:INTENSITYPERCENT=0.002864 AND MS2PROD=formula(C15H3N2O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.002061</t>
-  </si>
-  <si>
-    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C6H10O8P):TOLERANCEPPM=10:INTENSITYPERCENT=0.009138:EXCLUDED AND MS2PROD=formula(C9O11P):TOLERANCEPPM=10:INTENSITYPERCENT=0.003507:EXCLUDED AND MS2PROD=formula(C39H18O4P):TOLERANCEPPM=10:INTENSITYPERCENT=0.115346 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C6H10O8P):TOLERANCEPPM=10:INTENSITYPERCENT=0.009138:EXCLUDED AND MS2PROD=formula(C9O11P):TOLERANCEPPM=10:INTENSITYPERCENT=0.003507 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C6H10O8P):TOLERANCEPPM=10:INTENSITYPERCENT=0.009138 AND MS2PROD=formula(H2O4P):TOLERANCEPPM=10:INTENSITYPERCENT=0.034397:EXCLUDED AND MS2PROD=formula(C6H11O11P2):TOLERANCEPPM=10:INTENSITYPERCENT=0.000636:EXCLUDED</t>
-  </si>
-  <si>
-    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C24H33):TOLERANCEPPM=10:INTENSITYPERCENT=0.004144:EXCLUDED AND MS2PROD=formula(C24H33O):TOLERANCEPPM=10:INTENSITYPERCENT=0.014517:EXCLUDED AND MS2NL=formula(C23H39N2P):TOLERANCEPPM=10:INTENSITYPERCENT=0.184262 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C24H33):TOLERANCEPPM=10:INTENSITYPERCENT=0.004144:EXCLUDED AND MS2PROD=formula(C24H33O):TOLERANCEPPM=10:INTENSITYPERCENT=0.014517 AND MS2NL=formula(C20H42N2OS2):TOLERANCEPPM=10:INTENSITYPERCENT=0.008663 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C24H33):TOLERANCEPPM=10:INTENSITYPERCENT=0.004144 AND MS2NL=formula(C12H22O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.001918:EXCLUDED AND MS2PROD=formula(C16H21O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.001793:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C24H33):TOLERANCEPPM=10:INTENSITYPERCENT=0.004144 AND MS2NL=formula(C12H22O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.001918 AND MS2PROD=formula(C18H27O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.010528</t>
-  </si>
-  <si>
-    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C6H10NO2S):TOLERANCEPPM=10:INTENSITYPERCENT=0.030424:EXCLUDED AND MS2PROD=formula(H5N5O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.001250:EXCLUDED AND MS2PROD=formula(C7H7N4OS2):TOLERANCEPPM=10:INTENSITYPERCENT=0.000602 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C6H10NO2S):TOLERANCEPPM=10:INTENSITYPERCENT=0.030424:EXCLUDED AND MS2PROD=formula(H5N5O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.001250 AND MS2PROD=formula(C5H6NS):TOLERANCEPPM=10:INTENSITYPERCENT=0.002949 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C6H10NO2S):TOLERANCEPPM=10:INTENSITYPERCENT=0.030424 AND MS2PROD=formula(C3H6N):TOLERANCEPPM=10:INTENSITYPERCENT=0.000990:EXCLUDED AND MS2PROD=formula(C14H6N2):TOLERANCEPPM=10:INTENSITYPERCENT=0.006564:EXCLUDED</t>
-  </si>
-  <si>
-    <t>QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(C24H38O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.001176:EXCLUDED AND MS2PROD=formula(C23H35O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.000073:EXCLUDED AND MS2NL=formula(C25H34N4):TOLERANCEPPM=10:INTENSITYPERCENT=0.000982 ||| QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(C24H38O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.001176:EXCLUDED AND MS2PROD=formula(C23H35O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.000073 AND MS2PROD=formula(C22H31O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.000077:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(C24H38O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.001176 AND MS2NL=formula(C15H41N7O7):TOLERANCEPPM=10:INTENSITYPERCENT=0.000512:EXCLUDED AND MS2PROD=formula(C6H13N2O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.880451:EXCLUDED</t>
-  </si>
-  <si>
-    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C3H6O5P):TOLERANCEPPM=10:INTENSITYPERCENT=0.001914:EXCLUDED AND MS2PROD=formula(C5H11NO5P):TOLERANCEPPM=10:INTENSITYPERCENT=0.000460:EXCLUDED AND MS2PROD=formula(C18H33O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.045027 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C3H6O5P):TOLERANCEPPM=10:INTENSITYPERCENT=0.001914:EXCLUDED AND MS2PROD=formula(C5H11NO5P):TOLERANCEPPM=10:INTENSITYPERCENT=0.000460 AND MS2NL=formula(C8H3N7):TOLERANCEPPM=10:INTENSITYPERCENT=0.952171:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C3H6O5P):TOLERANCEPPM=10:INTENSITYPERCENT=0.001914 AND MS2PROD=formula(O3P):TOLERANCEPPM=10:INTENSITYPERCENT=0.462538:EXCLUDED AND MS2NL=formula(H5O5P):TOLERANCEPPM=10:INTENSITYPERCENT=0.030577:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C3H6O5P):TOLERANCEPPM=10:INTENSITYPERCENT=0.001914 AND MS2PROD=formula(O3P):TOLERANCEPPM=10:INTENSITYPERCENT=0.462538 AND MS2PROD=formula(C6H9O10P2):TOLERANCEPPM=10:INTENSITYPERCENT=0.002631</t>
-  </si>
-  <si>
-    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C7H3O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.004616:EXCLUDED AND MS2PROD=formula(C15H9O6):TOLERANCEPPM=10:INTENSITYPERCENT=0.008312:EXCLUDED AND MS2PROD=formula(C15H8O7):TOLERANCEPPM=10:INTENSITYPERCENT=0.016601 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C7H3O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.004616:EXCLUDED AND MS2PROD=formula(C15H9O6):TOLERANCEPPM=10:INTENSITYPERCENT=0.008312 AND MS2PROD=formula(C15H9O6):TOLERANCEPPM=10:INTENSITYPERCENT=0.122768:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C7H3O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.004616:EXCLUDED AND MS2PROD=formula(C15H9O6):TOLERANCEPPM=10:INTENSITYPERCENT=0.008312 AND MS2PROD=formula(C15H9O6):TOLERANCEPPM=10:INTENSITYPERCENT=0.122768 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C7H3O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.004616 AND MS2PROD=formula(C6H3O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.000987:EXCLUDED AND MS2PROD=formula(C8H6O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.000394:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C7H3O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.004616 AND MS2PROD=formula(C6H3O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.000987 AND MS2PROD=formula(C12H7O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.004171</t>
-  </si>
-  <si>
-    <t>QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(C5H8O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.283732:EXCLUDED AND MS2PROD=formula(C5H6N5):TOLERANCEPPM=10:INTENSITYPERCENT=0.736998:EXCLUDED AND MS2NL=formula(C8H8N2OS2):TOLERANCEPPM=10:INTENSITYPERCENT=0.127969 ||| QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(C5H8O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.283732:EXCLUDED AND MS2PROD=formula(C5H6N5):TOLERANCEPPM=10:INTENSITYPERCENT=0.736998 AND MS2PROD=formula(C6H6N5):TOLERANCEPPM=10:INTENSITYPERCENT=0.005699:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(C5H8O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.283732 AND MS2NL=formula(C5H11NO4):TOLERANCEPPM=10:INTENSITYPERCENT=0.000099:EXCLUDED AND MS2NL=formula(C5H8O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.919773 ||| QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(C5H8O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.283732 AND MS2NL=formula(C5H11NO4):TOLERANCEPPM=10:INTENSITYPERCENT=0.000099 AND MS2PROD=formula(C7H5N4O):TOLERANCEPPM=10:INTENSITYPERCENT=0.013940:EXCLUDED</t>
-  </si>
-  <si>
-    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C6H9O5):TOLERANCEPPM=10:INTENSITYPERCENT=0.000004:EXCLUDED AND MS2NL=formula(C7H14S2):TOLERANCEPPM=10:INTENSITYPERCENT=0.092304:EXCLUDED AND MS2NL=formula(C13H24O4S2):TOLERANCEPPM=10:INTENSITYPERCENT=0.056189 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C6H9O5):TOLERANCEPPM=10:INTENSITYPERCENT=0.000004:EXCLUDED AND MS2NL=formula(C7H14S2):TOLERANCEPPM=10:INTENSITYPERCENT=0.092304 AND MS2NL=formula(C3H6O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.008776:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C6H9O5):TOLERANCEPPM=10:INTENSITYPERCENT=0.000004 AND MS2PROD=formula(C6H7O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.002829:EXCLUDED AND MS2PROD=formula(C9H7NO2):TOLERANCEPPM=10:INTENSITYPERCENT=0.000115:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C6H9O5):TOLERANCEPPM=10:INTENSITYPERCENT=0.000004 AND MS2PROD=formula(C6H7O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.002829 AND MS2NL=formula(C3H8O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.018492:EXCLUDED</t>
-  </si>
-  <si>
-    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C5H10N6O):TOLERANCEPPM=10:INTENSITYPERCENT=0.001951:EXCLUDED AND MS2PROD=formula(C7H11N5O):TOLERANCEPPM=10:INTENSITYPERCENT=0.000637:EXCLUDED AND MS2PROD=formula(C2H6N6O):TOLERANCEPPM=10:INTENSITYPERCENT=0.004135 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C5H10N6O):TOLERANCEPPM=10:INTENSITYPERCENT=0.001951:EXCLUDED AND MS2PROD=formula(C7H11N5O):TOLERANCEPPM=10:INTENSITYPERCENT=0.000637 AND MS2PROD=formula(C9H13N5O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.001688:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C5H10N6O):TOLERANCEPPM=10:INTENSITYPERCENT=0.001951 AND MS2NL=formula(C24H43N3O6P2):TOLERANCEPPM=10:INTENSITYPERCENT=0.001160:EXCLUDED AND MS2PROD=formula(C8H14N5O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.000451:EXCLUDED</t>
-  </si>
-  <si>
-    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C3H8O5P):TOLERANCEPPM=10:INTENSITYPERCENT=0.001440:EXCLUDED AND MS2PROD=formula(C3H7NaO5P):TOLERANCEPPM=10:INTENSITYPERCENT=0.000395:EXCLUDED AND MS2NL=formula(C3H4N5P):TOLERANCEPPM=10:INTENSITYPERCENT=0.338294 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C3H8O5P):TOLERANCEPPM=10:INTENSITYPERCENT=0.001440:EXCLUDED AND MS2PROD=formula(C3H7NaO5P):TOLERANCEPPM=10:INTENSITYPERCENT=0.000395 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C3H8O5P):TOLERANCEPPM=10:INTENSITYPERCENT=0.001440 AND MS2NL=formula(C16H18N2O2S3):TOLERANCEPPM=10:INTENSITYPERCENT=0.004532:EXCLUDED</t>
-  </si>
-  <si>
-    <t>QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(C5H8O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.172707:EXCLUDED AND MS2PROD=formula(C3H6N3O6P):TOLERANCEPPM=10:INTENSITYPERCENT=0.010060:EXCLUDED AND MS2NL=formula(C4H7NO4):TOLERANCEPPM=10:INTENSITYPERCENT=0.029269 ||| QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(C5H8O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.172707:EXCLUDED AND MS2PROD=formula(C3H6N3O6P):TOLERANCEPPM=10:INTENSITYPERCENT=0.010060 AND MS2PROD=formula(C19H2N7O5):TOLERANCEPPM=10:INTENSITYPERCENT=0.007694:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(C5H8O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.172707 AND MS2NL=formula(C6H9NO5):TOLERANCEPPM=10:INTENSITYPERCENT=0.001242:EXCLUDED AND MS2NL=formula(C5H8O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.858722 ||| QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(C5H8O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.172707 AND MS2NL=formula(C6H9NO5):TOLERANCEPPM=10:INTENSITYPERCENT=0.001242 AND MS2PROD=formula(C7H3N4O):TOLERANCEPPM=10:INTENSITYPERCENT=0.196133:EXCLUDED</t>
-  </si>
-  <si>
-    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C24H35O):TOLERANCEPPM=10:INTENSITYPERCENT=0.010829:EXCLUDED AND MS2PROD=formula(C24H33O):TOLERANCEPPM=10:INTENSITYPERCENT=0.009579 AND MS2PROD=formula(C16H17):TOLERANCEPPM=10:INTENSITYPERCENT=0.012364 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C24H35O):TOLERANCEPPM=10:INTENSITYPERCENT=0.010829 AND MS2PROD=formula(C16H23):TOLERANCEPPM=10:INTENSITYPERCENT=0.013950:EXCLUDED AND MS2PROD=formula(C28H42NO3):TOLERANCEPPM=10:INTENSITYPERCENT=0.000191 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C24H35O):TOLERANCEPPM=10:INTENSITYPERCENT=0.010829 AND MS2PROD=formula(C16H23):TOLERANCEPPM=10:INTENSITYPERCENT=0.013950 AND MS2NL=formula(C22H37NO3):TOLERANCEPPM=10:INTENSITYPERCENT=0.004929:EXCLUDED</t>
-  </si>
-  <si>
-    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C9H13):TOLERANCEPPM=10:INTENSITYPERCENT=0.000976:EXCLUDED AND MS2PROD=formula(C7H7):TOLERANCEPPM=10:INTENSITYPERCENT=0.000213:EXCLUDED AND MS2PROD=formula(C6H5):TOLERANCEPPM=10:INTENSITYPERCENT=0.000258 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C9H13):TOLERANCEPPM=10:INTENSITYPERCENT=0.000976:EXCLUDED AND MS2PROD=formula(C7H7):TOLERANCEPPM=10:INTENSITYPERCENT=0.000213 AND MS2PROD=formula(C6H9):TOLERANCEPPM=10:INTENSITYPERCENT=0.001077:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C9H13):TOLERANCEPPM=10:INTENSITYPERCENT=0.000976 AND MS2PROD=formula(C9H7O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.000929 AND MS2PROD=formula(C12H13):TOLERANCEPPM=10:INTENSITYPERCENT=0.003782:EXCLUDED</t>
-  </si>
-  <si>
-    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C9H13):TOLERANCEPPM=10:INTENSITYPERCENT=0.000815:EXCLUDED AND MS2PROD=formula(C7H7):TOLERANCEPPM=10:INTENSITYPERCENT=0.000084:EXCLUDED AND MS2PROD=formula(C9H8N):TOLERANCEPPM=10:INTENSITYPERCENT=0.000181 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C9H13):TOLERANCEPPM=10:INTENSITYPERCENT=0.000815:EXCLUDED AND MS2PROD=formula(C7H7):TOLERANCEPPM=10:INTENSITYPERCENT=0.000084 AND MS2PROD=formula(C6H9):TOLERANCEPPM=10:INTENSITYPERCENT=0.001348:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C9H13):TOLERANCEPPM=10:INTENSITYPERCENT=0.000815 AND MS2PROD=formula(C9H7O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.000154:EXCLUDED AND MS2PROD=formula(C9H8N):TOLERANCEPPM=10:INTENSITYPERCENT=0.001364 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C9H13):TOLERANCEPPM=10:INTENSITYPERCENT=0.000815 AND MS2PROD=formula(C9H7O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.000154 AND MS2PROD=formula(C12H13):TOLERANCEPPM=10:INTENSITYPERCENT=0.002894:EXCLUDED</t>
-  </si>
-  <si>
-    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C6H9O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.103127:EXCLUDED AND MS2PROD=formula(C13H22NO7):TOLERANCEPPM=10:INTENSITYPERCENT=0.076942:EXCLUDED AND MS2NL=formula(C2H10O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.060764 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C6H9O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.103127:EXCLUDED AND MS2PROD=formula(C13H22NO7):TOLERANCEPPM=10:INTENSITYPERCENT=0.076942 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C6H9O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.103127 AND MS2NL=formula(C7H16OS2):TOLERANCEPPM=10:INTENSITYPERCENT=0.000630:EXCLUDED AND MS2PROD=formula(C6H7O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.131305 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C6H9O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.103127 AND MS2NL=formula(C7H16OS2):TOLERANCEPPM=10:INTENSITYPERCENT=0.000630 AND MS2PROD=formula(C6H11O5):TOLERANCEPPM=10:INTENSITYPERCENT=0.004699</t>
-  </si>
-  <si>
-    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C19H29O):TOLERANCEPPM=10:INTENSITYPERCENT=0.003675:EXCLUDED AND MS2PROD=formula(C14H17O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.021058:EXCLUDED AND MS2PROD=formula(C19H29):TOLERANCEPPM=10:INTENSITYPERCENT=0.050000 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C19H29O):TOLERANCEPPM=10:INTENSITYPERCENT=0.003675:EXCLUDED AND MS2PROD=formula(C14H17O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.021058 AND MS2PROD=formula(C7H9O):TOLERANCEPPM=10:INTENSITYPERCENT=0.001107 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C19H29O):TOLERANCEPPM=10:INTENSITYPERCENT=0.003675 AND MS2PROD=formula(C2H3O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.000332:EXCLUDED AND MS2PROD=formula(C14H19O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.004220 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C19H29O):TOLERANCEPPM=10:INTENSITYPERCENT=0.003675 AND MS2PROD=formula(C2H3O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.000332 AND MS2NL=formula(C4N4):TOLERANCEPPM=10:INTENSITYPERCENT=0.007086:EXCLUDED</t>
-  </si>
-  <si>
-    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C30H47O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.008097:EXCLUDED AND MS2PROD=formula(C28H41O):TOLERANCEPPM=10:INTENSITYPERCENT=0.000262:EXCLUDED AND MS2PROD=formula(C35H55O7):TOLERANCEPPM=10:INTENSITYPERCENT=0.008906 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C30H47O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.008097:EXCLUDED AND MS2PROD=formula(C28H41O):TOLERANCEPPM=10:INTENSITYPERCENT=0.000262 AND MS2PROD=formula(C28H43O):TOLERANCEPPM=10:INTENSITYPERCENT=0.004046:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C30H47O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.008097 AND MS2NL=formula(C39H39O6PS):TOLERANCEPPM=10:INTENSITYPERCENT=0.000088:EXCLUDED AND MS2PROD=formula(C30H47O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.996306:EXCLUDED</t>
-  </si>
-  <si>
-    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C23H24O7):TOLERANCEPPM=10:INTENSITYPERCENT=0.053501:EXCLUDED AND MS2PROD=formula(C13H5Cl2O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.017382:EXCLUDED AND MS2PROD=formula(C13H6O5):TOLERANCEPPM=10:INTENSITYPERCENT=0.385088 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C23H24O7):TOLERANCEPPM=10:INTENSITYPERCENT=0.053501:EXCLUDED AND MS2PROD=formula(C13H5Cl2O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.017382 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C23H24O7):TOLERANCEPPM=10:INTENSITYPERCENT=0.053501</t>
-  </si>
-  <si>
-    <t>QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(C2H8O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.075320:EXCLUDED AND MS2PROD=formula(C12H21O11):TOLERANCEPPM=10:INTENSITYPERCENT=0.022838:EXCLUDED AND MS2NL=formula(CH17N4O7P):TOLERANCEPPM=10:INTENSITYPERCENT=0.019822 ||| QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(C2H8O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.075320:EXCLUDED AND MS2PROD=formula(C12H21O11):TOLERANCEPPM=10:INTENSITYPERCENT=0.022838 AND MS2PROD=formula(C12H19O10):TOLERANCEPPM=10:INTENSITYPERCENT=0.023576:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(C2H8O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.075320 AND MS2PROD=formula(C3H5O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.042708:EXCLUDED AND MS2PROD=formula(C4H5O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.135896 ||| QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(C2H8O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.075320 AND MS2PROD=formula(C3H5O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.042708 AND MS2PROD=formula(C4H6NO):TOLERANCEPPM=10:INTENSITYPERCENT=0.001751:EXCLUDED</t>
-  </si>
-  <si>
-    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C9H8N):TOLERANCEPPM=10:INTENSITYPERCENT=0.705815:EXCLUDED AND MS2PROD=formula(C10H11N2):TOLERANCEPPM=10:INTENSITYPERCENT=0.018431 AND MS2PROD=formula(C11H10NO2):TOLERANCEPPM=10:INTENSITYPERCENT=0.001119 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C9H8N):TOLERANCEPPM=10:INTENSITYPERCENT=0.705815 AND MS2NL=formula(C2H7N):TOLERANCEPPM=10:INTENSITYPERCENT=0.412665:EXCLUDED AND MS2PROD=formula(C8H7):TOLERANCEPPM=10:INTENSITYPERCENT=0.015723 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C9H8N):TOLERANCEPPM=10:INTENSITYPERCENT=0.705815 AND MS2NL=formula(C2H7N):TOLERANCEPPM=10:INTENSITYPERCENT=0.412665</t>
-  </si>
-  <si>
-    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C25H40NO3):TOLERANCEPPM=10:INTENSITYPERCENT=0.000155:EXCLUDED AND MS2NL=formula(C24H38O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.018143:EXCLUDED AND MS2NL=formula(C24H38O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.024398 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C25H40NO3):TOLERANCEPPM=10:INTENSITYPERCENT=0.000155:EXCLUDED AND MS2NL=formula(C24H38O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.018143 AND MS2PROD=formula(C24H37O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.487587:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C25H40NO3):TOLERANCEPPM=10:INTENSITYPERCENT=0.000155</t>
-  </si>
-  <si>
-    <t>QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(CH2O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.272980:EXCLUDED AND MS2PROD=formula(C5H9O):TOLERANCEPPM=10:INTENSITYPERCENT=0.203558:EXCLUDED AND MS2PROD=formula(C4H7O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.796387 ||| QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(CH2O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.272980:EXCLUDED AND MS2PROD=formula(C5H9O):TOLERANCEPPM=10:INTENSITYPERCENT=0.203558 AND MS2NL=formula(C39H62N6O12):TOLERANCEPPM=10:INTENSITYPERCENT=0.013345:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(CH2O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.272980 AND MS2NL=formula(CH4O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.000476:EXCLUDED AND MS2PROD=formula(C3H5O):TOLERANCEPPM=10:INTENSITYPERCENT=0.003108:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(CH2O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.272980 AND MS2NL=formula(CH4O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.000476:EXCLUDED AND MS2PROD=formula(C3H5O):TOLERANCEPPM=10:INTENSITYPERCENT=0.003108 ||| QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(CH2O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.272980 AND MS2NL=formula(CH4O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.000476 AND MS2NL=formula(C3H4O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.081803</t>
-  </si>
-  <si>
-    <t>QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(C24H38O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.016080:EXCLUDED AND MS2PROD=formula(C23H37O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.057117:EXCLUDED AND MS2PROD=formula(C23H39O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.003521 ||| QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(C24H38O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.016080:EXCLUDED AND MS2PROD=formula(C23H37O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.057117 AND MS2PROD=formula(C24H35O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.042916:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(C24H38O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.016080 AND MS2PROD=formula(C4H6NO):TOLERANCEPPM=10:INTENSITYPERCENT=0.001655:EXCLUDED AND MS2PROD=formula(C23H35O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.000119 ||| QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(C24H38O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.016080 AND MS2PROD=formula(C4H6NO):TOLERANCEPPM=10:INTENSITYPERCENT=0.001655</t>
-  </si>
-  <si>
-    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C14H7O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.005224:EXCLUDED AND MS2PROD=formula(C15H8O5):TOLERANCEPPM=10:INTENSITYPERCENT=0.027431:EXCLUDED AND MS2PROD=formula(C24H21O5):TOLERANCEPPM=10:INTENSITYPERCENT=0.014475 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C14H7O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.005224:EXCLUDED AND MS2PROD=formula(C15H8O5):TOLERANCEPPM=10:INTENSITYPERCENT=0.027431 AND MS2PROD=formula(C8H4O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.002826 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C14H7O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.005224 AND MS2PROD=formula(C8H4O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.001316:EXCLUDED AND MS2NL=formula(C4H8):TOLERANCEPPM=10:INTENSITYPERCENT=0.003422 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C14H7O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.005224 AND MS2PROD=formula(C8H4O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.001316 AND MS2PROD=formula(C8H5O):TOLERANCEPPM=10:INTENSITYPERCENT=0.038652:EXCLUDED</t>
-  </si>
-  <si>
-    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C5H8N3):TOLERANCEPPM=10:INTENSITYPERCENT=0.269307:EXCLUDED AND MS2PROD=formula(C5H10N3):TOLERANCEPPM=10:INTENSITYPERCENT=0.314554 AND MS2PROD=formula(C5H7N2):TOLERANCEPPM=10:INTENSITYPERCENT=0.012994 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C5H8N3):TOLERANCEPPM=10:INTENSITYPERCENT=0.269307 AND MS2PROD=formula(C7H12N3):TOLERANCEPPM=10:INTENSITYPERCENT=0.030982:EXCLUDED AND MS2PROD=formula(C4H7N2):TOLERANCEPPM=10:INTENSITYPERCENT=0.003077:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C5H8N3):TOLERANCEPPM=10:INTENSITYPERCENT=0.269307 AND MS2PROD=formula(C7H12N3):TOLERANCEPPM=10:INTENSITYPERCENT=0.030982:EXCLUDED AND MS2PROD=formula(C4H7N2):TOLERANCEPPM=10:INTENSITYPERCENT=0.003077</t>
-  </si>
-  <si>
-    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C20H27O):TOLERANCEPPM=10:INTENSITYPERCENT=0.012507:EXCLUDED AND MS2PROD=formula(C10H19F2O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.012699:EXCLUDED AND MS2PROD=formula(C22H35O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.006115 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C20H27O):TOLERANCEPPM=10:INTENSITYPERCENT=0.012507:EXCLUDED AND MS2PROD=formula(C10H19F2O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.012699 AND MS2PROD=formula(C17H15F):TOLERANCEPPM=10:INTENSITYPERCENT=0.000012:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C20H27O):TOLERANCEPPM=10:INTENSITYPERCENT=0.012507 AND MS2PROD=formula(C5H11):TOLERANCEPPM=10:INTENSITYPERCENT=0.000462:EXCLUDED AND MS2NL=formula(C7H18O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.000944 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C20H27O):TOLERANCEPPM=10:INTENSITYPERCENT=0.012507 AND MS2PROD=formula(C5H11):TOLERANCEPPM=10:INTENSITYPERCENT=0.000462 AND MS2PROD=formula(C17H21):TOLERANCEPPM=10:INTENSITYPERCENT=0.000489:EXCLUDED</t>
-  </si>
-  <si>
-    <t>QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(C16H42N2O5S):TOLERANCEPPM=10:INTENSITYPERCENT=0.002428:EXCLUDED AND MS2NL=formula(C16H42N2O6S):TOLERANCEPPM=10:INTENSITYPERCENT=0.008114:EXCLUDED AND MS2PROD=formula(C23H35O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.019021 ||| QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(C16H42N2O5S):TOLERANCEPPM=10:INTENSITYPERCENT=0.002428:EXCLUDED AND MS2NL=formula(C16H42N2O6S):TOLERANCEPPM=10:INTENSITYPERCENT=0.008114 AND MS2NL=formula(C13H24N3O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.004777:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(C16H42N2O5S):TOLERANCEPPM=10:INTENSITYPERCENT=0.002428 AND MS2NL=formula(C25H40N3O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.068889:EXCLUDED AND MS2NL=formula(C15H35N9S):TOLERANCEPPM=10:INTENSITYPERCENT=0.109837:EXCLUDED</t>
-  </si>
-  <si>
-    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C29H43O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.000286:EXCLUDED AND MS2PROD=formula(C30H47O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.000009:EXCLUDED AND MS2PROD=formula(C30H47O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.000190 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C29H43O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.000286:EXCLUDED AND MS2PROD=formula(C30H47O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.000009 AND MS2NL=formula(C27H43N3O3S):TOLERANCEPPM=10:INTENSITYPERCENT=0.000096:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C29H43O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.000286 AND MS2PROD=formula(C24H38NO2):TOLERANCEPPM=10:INTENSITYPERCENT=0.000439:EXCLUDED AND MS2NL=formula(C9H18N6O9):TOLERANCEPPM=10:INTENSITYPERCENT=0.006425:EXCLUDED</t>
-  </si>
-  <si>
-    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C23H21O6):TOLERANCEPPM=10:INTENSITYPERCENT=0.012203:EXCLUDED AND MS2PROD=formula(C23H24O7):TOLERANCEPPM=10:INTENSITYPERCENT=0.036362:EXCLUDED AND MS2PROD=formula(C13H6O5):TOLERANCEPPM=10:INTENSITYPERCENT=0.393985 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C23H21O6):TOLERANCEPPM=10:INTENSITYPERCENT=0.012203:EXCLUDED AND MS2PROD=formula(C23H24O7):TOLERANCEPPM=10:INTENSITYPERCENT=0.036362 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C23H21O6):TOLERANCEPPM=10:INTENSITYPERCENT=0.012203 AND MS2PROD=formula(C19H15O6):TOLERANCEPPM=10:INTENSITYPERCENT=0.001310:EXCLUDED AND MS2PROD=formula(C19H13O6):TOLERANCEPPM=10:INTENSITYPERCENT=0.008984 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C23H21O6):TOLERANCEPPM=10:INTENSITYPERCENT=0.012203 AND MS2PROD=formula(C19H15O6):TOLERANCEPPM=10:INTENSITYPERCENT=0.001310</t>
-  </si>
-  <si>
-    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C14H23O5):TOLERANCEPPM=10:INTENSITYPERCENT=0.034095:EXCLUDED AND MS2PROD=formula(C22H40N):TOLERANCEPPM=10:INTENSITYPERCENT=0.012631:EXCLUDED AND MS2PROD=formula(C18H31O8):TOLERANCEPPM=10:INTENSITYPERCENT=0.009209 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C14H23O5):TOLERANCEPPM=10:INTENSITYPERCENT=0.034095:EXCLUDED AND MS2PROD=formula(C22H40N):TOLERANCEPPM=10:INTENSITYPERCENT=0.012631 AND MS2PROD=formula(C22H40N):TOLERANCEPPM=10:INTENSITYPERCENT=0.342627:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C14H23O5):TOLERANCEPPM=10:INTENSITYPERCENT=0.034095 AND MS2PROD=formula(C8H13O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.046630</t>
-  </si>
-  <si>
-    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C24H33):TOLERANCEPPM=10:INTENSITYPERCENT=0.004383:EXCLUDED AND MS2PROD=formula(C24H33O):TOLERANCEPPM=10:INTENSITYPERCENT=0.014967:EXCLUDED AND MS2PROD=formula(C8H7O7):TOLERANCEPPM=10:INTENSITYPERCENT=0.162655 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C24H33):TOLERANCEPPM=10:INTENSITYPERCENT=0.004383:EXCLUDED AND MS2PROD=formula(C24H33O):TOLERANCEPPM=10:INTENSITYPERCENT=0.014967 AND MS2PROD=formula(C10H13O):TOLERANCEPPM=10:INTENSITYPERCENT=0.005582:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C24H33):TOLERANCEPPM=10:INTENSITYPERCENT=0.004383 AND MS2PROD=formula(C12H15):TOLERANCEPPM=10:INTENSITYPERCENT=0.028788:EXCLUDED AND MS2NL=formula(C8H14O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.004970:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C24H33):TOLERANCEPPM=10:INTENSITYPERCENT=0.004383 AND MS2PROD=formula(C12H15):TOLERANCEPPM=10:INTENSITYPERCENT=0.028788 AND MS2PROD=formula(C14H19O):TOLERANCEPPM=10:INTENSITYPERCENT=0.002210:EXCLUDED</t>
-  </si>
-  <si>
-    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C24H12O6S):TOLERANCEPPM=10:INTENSITYPERCENT=0.034951:EXCLUDED AND MS2PROD=formula(C11H19O):TOLERANCEPPM=10:INTENSITYPERCENT=0.015808:EXCLUDED AND MS2PROD=formula(C4H3O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.378989 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C24H12O6S):TOLERANCEPPM=10:INTENSITYPERCENT=0.034951:EXCLUDED AND MS2PROD=formula(C11H19O):TOLERANCEPPM=10:INTENSITYPERCENT=0.015808 AND MS2PROD=formula(C8H11):TOLERANCEPPM=10:INTENSITYPERCENT=0.000777:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C24H12O6S):TOLERANCEPPM=10:INTENSITYPERCENT=0.034951 AND MS2PROD=formula(C31H40N6):TOLERANCEPPM=10:INTENSITYPERCENT=0.001067:EXCLUDED AND MS2PROD=formula(C11H17N4O10P3S):TOLERANCEPPM=10:INTENSITYPERCENT=0.000424:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C24H12O6S):TOLERANCEPPM=10:INTENSITYPERCENT=0.034951 AND MS2PROD=formula(C31H40N6):TOLERANCEPPM=10:INTENSITYPERCENT=0.001067:EXCLUDED AND MS2PROD=formula(C11H17N4O10P3S):TOLERANCEPPM=10:INTENSITYPERCENT=0.000424</t>
-  </si>
-  <si>
-    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C24H35O):TOLERANCEPPM=10:INTENSITYPERCENT=0.001551:EXCLUDED AND MS2PROD=formula(C24H33O):TOLERANCEPPM=10:INTENSITYPERCENT=0.002283 AND MS2PROD=formula(C24H33O):TOLERANCEPPM=10:INTENSITYPERCENT=0.016520:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C24H35O):TOLERANCEPPM=10:INTENSITYPERCENT=0.001551:EXCLUDED AND MS2PROD=formula(C24H33O):TOLERANCEPPM=10:INTENSITYPERCENT=0.002283 AND MS2PROD=formula(C24H33O):TOLERANCEPPM=10:INTENSITYPERCENT=0.016520 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C24H35O):TOLERANCEPPM=10:INTENSITYPERCENT=0.001551 AND MS2PROD=formula(C26H37O):TOLERANCEPPM=10:INTENSITYPERCENT=0.000693:EXCLUDED AND MS2PROD=formula(C24H33):TOLERANCEPPM=10:INTENSITYPERCENT=0.001553:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C24H35O):TOLERANCEPPM=10:INTENSITYPERCENT=0.001551 AND MS2PROD=formula(C26H37O):TOLERANCEPPM=10:INTENSITYPERCENT=0.000693:EXCLUDED AND MS2PROD=formula(C24H33):TOLERANCEPPM=10:INTENSITYPERCENT=0.001553 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C24H35O):TOLERANCEPPM=10:INTENSITYPERCENT=0.001551 AND MS2PROD=formula(C26H37O):TOLERANCEPPM=10:INTENSITYPERCENT=0.000693 AND MS2PROD=formula(C22H29O):TOLERANCEPPM=10:INTENSITYPERCENT=0.004287</t>
-  </si>
-  <si>
-    <t>QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(C22H37N2O4P):TOLERANCEPPM=10:INTENSITYPERCENT=0.087401:EXCLUDED AND MS2PROD=formula(C8H10NO3):TOLERANCEPPM=10:INTENSITYPERCENT=0.033861:EXCLUDED AND MS2PROD=formula(C11H17O5):TOLERANCEPPM=10:INTENSITYPERCENT=0.072294 ||| QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(C22H37N2O4P):TOLERANCEPPM=10:INTENSITYPERCENT=0.087401:EXCLUDED AND MS2PROD=formula(C8H10NO3):TOLERANCEPPM=10:INTENSITYPERCENT=0.033861 AND MS2PROD=formula(C8H9NO3):TOLERANCEPPM=10:INTENSITYPERCENT=0.095392 ||| QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(C22H37N2O4P):TOLERANCEPPM=10:INTENSITYPERCENT=0.087401 AND MS2PROD=formula(C10H7NO):TOLERANCEPPM=10:INTENSITYPERCENT=0.064899:EXCLUDED</t>
-  </si>
-  <si>
-    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C6H11O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.101660:EXCLUDED AND MS2NL=formula(C25H45N11O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.091156:EXCLUDED AND MS2PROD=formula(C18H29O6):TOLERANCEPPM=10:INTENSITYPERCENT=0.296343 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C6H11O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.101660:EXCLUDED AND MS2NL=formula(C25H45N11O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.091156 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C6H11O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.101660 AND MS2NL=formula(C59H56O):TOLERANCEPPM=10:INTENSITYPERCENT=0.001450:EXCLUDED AND MS2PROD=formula(C4H9N3O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.156155:EXCLUDED</t>
-  </si>
-  <si>
-    <t>QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(C9H21N4O8P):TOLERANCEPPM=10:INTENSITYPERCENT=0.005939:EXCLUDED AND MS2PROD=formula(C6H11O6):TOLERANCEPPM=10:INTENSITYPERCENT=0.000096 AND MS2PROD=formula(C9H7O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.002123 ||| QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(C9H21N4O8P):TOLERANCEPPM=10:INTENSITYPERCENT=0.005939 AND MS2NL=formula(C14H17N2PS):TOLERANCEPPM=10:INTENSITYPERCENT=0.005967:EXCLUDED AND MS2PROD=formula(C4H7O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.013345 ||| QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(C9H21N4O8P):TOLERANCEPPM=10:INTENSITYPERCENT=0.005939 AND MS2NL=formula(C14H17N2PS):TOLERANCEPPM=10:INTENSITYPERCENT=0.005967 AND MS2NL=formula(C9H23N4O6P):TOLERANCEPPM=10:INTENSITYPERCENT=0.000637:EXCLUDED</t>
-  </si>
-  <si>
-    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C14H11O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.371433:EXCLUDED AND MS2PROD=formula(C12H9O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.254468:EXCLUDED AND MS2PROD=formula(C30H25O6):TOLERANCEPPM=10:INTENSITYPERCENT=0.007034 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C14H11O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.371433:EXCLUDED AND MS2PROD=formula(C12H9O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.254468 AND MS2PROD=formula(C13H11O):TOLERANCEPPM=10:INTENSITYPERCENT=0.045496 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C14H11O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.371433 AND MS2PROD=formula(C12H9O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.000469:EXCLUDED AND MS2PROD=formula(C14H11O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.907702 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C14H11O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.371433 AND MS2PROD=formula(C12H9O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.000469</t>
-  </si>
-  <si>
-    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C20H21O6):TOLERANCEPPM=10:INTENSITYPERCENT=0.059631:EXCLUDED AND MS2PROD=formula(C24H19O8):TOLERANCEPPM=10:INTENSITYPERCENT=0.003361:EXCLUDED AND MS2PROD=formula(C22H25O8):TOLERANCEPPM=10:INTENSITYPERCENT=0.005552 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C20H21O6):TOLERANCEPPM=10:INTENSITYPERCENT=0.059631:EXCLUDED AND MS2PROD=formula(C24H19O8):TOLERANCEPPM=10:INTENSITYPERCENT=0.003361 AND MS2PROD=formula(C12H5N4O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.005004:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C20H21O6):TOLERANCEPPM=10:INTENSITYPERCENT=0.059631 AND MS2PROD=formula(C11H13O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.055084:EXCLUDED</t>
-  </si>
-  <si>
-    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C10H18N4O):TOLERANCEPPM=10:INTENSITYPERCENT=0.000696:EXCLUDED AND MS2PROD=formula(C11H20N6O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.000021:EXCLUDED AND MS2PROD=formula(C9H17N5O):TOLERANCEPPM=10:INTENSITYPERCENT=0.001586 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C10H18N4O):TOLERANCEPPM=10:INTENSITYPERCENT=0.000696:EXCLUDED AND MS2PROD=formula(C11H20N6O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.000021 AND MS2PROD=formula(C3H6N):TOLERANCEPPM=10:INTENSITYPERCENT=0.000388:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C10H18N4O):TOLERANCEPPM=10:INTENSITYPERCENT=0.000696 AND MS2PROD=formula(C6H11):TOLERANCEPPM=10:INTENSITYPERCENT=0.005027:EXCLUDED AND MS2PROD=formula(C12H17O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.002559:EXCLUDED</t>
-  </si>
-  <si>
-    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C4H4N3):TOLERANCEPPM=10:INTENSITYPERCENT=0.000016:EXCLUDED AND MS2PROD=formula(C9H13):TOLERANCEPPM=10:INTENSITYPERCENT=0.000001:EXCLUDED AND MS2PROD=formula(C5H6N5):TOLERANCEPPM=10:INTENSITYPERCENT=0.000052 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C4H4N3):TOLERANCEPPM=10:INTENSITYPERCENT=0.000016:EXCLUDED AND MS2PROD=formula(C9H13):TOLERANCEPPM=10:INTENSITYPERCENT=0.000001 AND MS2PROD=formula(C4H5N2O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.000062 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C4H4N3):TOLERANCEPPM=10:INTENSITYPERCENT=0.000016 AND MS2PROD=formula(C5H9N2O):TOLERANCEPPM=10:INTENSITYPERCENT=0.033524:EXCLUDED AND MS2PROD=formula(C7H7OS):TOLERANCEPPM=10:INTENSITYPERCENT=0.000250:EXCLUDED</t>
-  </si>
-  <si>
-    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C6H9O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.001322:EXCLUDED AND MS2NL=formula(C6H10O5):TOLERANCEPPM=10:INTENSITYPERCENT=0.098563 AND MS2PROD=formula(C13H15O):TOLERANCEPPM=10:INTENSITYPERCENT=0.000355:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C6H9O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.001322 AND MS2PROD=formula(C4H5O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.003312:EXCLUDED AND MS2PROD=formula(C6H11O5):TOLERANCEPPM=10:INTENSITYPERCENT=0.000298 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C6H9O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.001322 AND MS2PROD=formula(C4H5O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.003312 AND MS2NL=formula(CH6O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.000486:EXCLUDED</t>
-  </si>
-  <si>
-    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C9H14NO2S):TOLERANCEPPM=10:INTENSITYPERCENT=0.017714:EXCLUDED AND MS2PROD=formula(C6H4N4OS):TOLERANCEPPM=10:INTENSITYPERCENT=0.598320:EXCLUDED AND MS2PROD=formula(C21H15ClFN3O):TOLERANCEPPM=10:INTENSITYPERCENT=0.013215 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C9H14NO2S):TOLERANCEPPM=10:INTENSITYPERCENT=0.017714:EXCLUDED AND MS2PROD=formula(C6H4N4OS):TOLERANCEPPM=10:INTENSITYPERCENT=0.598320 AND MS2PROD=formula(C6H5N4OS):TOLERANCEPPM=10:INTENSITYPERCENT=0.079913 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C9H14NO2S):TOLERANCEPPM=10:INTENSITYPERCENT=0.017714 AND MS2PROD=formula(C9H12NO2):TOLERANCEPPM=10:INTENSITYPERCENT=0.391231:EXCLUDED</t>
-  </si>
-  <si>
-    <t>QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(C18H17N7O7S):TOLERANCEPPM=10:INTENSITYPERCENT=0.104574:EXCLUDED AND MS2PROD=formula(C11H6O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.489875:EXCLUDED AND MS2NL=formula(C8H5F4OP):TOLERANCEPPM=10:INTENSITYPERCENT=0.057326 ||| QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(C18H17N7O7S):TOLERANCEPPM=10:INTENSITYPERCENT=0.104574:EXCLUDED AND MS2PROD=formula(C11H6O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.489875 ||| QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(C18H17N7O7S):TOLERANCEPPM=10:INTENSITYPERCENT=0.104574</t>
-  </si>
-  <si>
-    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C2H4NO2):TOLERANCEPPM=10:INTENSITYPERCENT=0.000197:EXCLUDED AND MS2NL=formula(CH3NO2):TOLERANCEPPM=10:INTENSITYPERCENT=0.000221 AND MS2NL=formula(CH3NO2):TOLERANCEPPM=10:INTENSITYPERCENT=0.034983 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C2H4NO2):TOLERANCEPPM=10:INTENSITYPERCENT=0.000197 AND MS2NL=formula(CO2):TOLERANCEPPM=10:INTENSITYPERCENT=0.000221:EXCLUDED AND MS2NL=formula(C3H5NO2):TOLERANCEPPM=10:INTENSITYPERCENT=0.000605 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C2H4NO2):TOLERANCEPPM=10:INTENSITYPERCENT=0.000197 AND MS2NL=formula(CO2):TOLERANCEPPM=10:INTENSITYPERCENT=0.000221 AND MS2PROD=formula(C9H14NO2):TOLERANCEPPM=10:INTENSITYPERCENT=0.011885:EXCLUDED</t>
-  </si>
-  <si>
-    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C10H6O5):TOLERANCEPPM=10:INTENSITYPERCENT=0.005194:EXCLUDED AND MS2PROD=formula(C12H11O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.518921:EXCLUDED AND MS2PROD=formula(C9H4O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.071486 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C10H6O5):TOLERANCEPPM=10:INTENSITYPERCENT=0.005194:EXCLUDED AND MS2PROD=formula(C12H11O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.518921 AND MS2NL=formula(C4H16N2O5S):TOLERANCEPPM=10:INTENSITYPERCENT=0.113233:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C10H6O5):TOLERANCEPPM=10:INTENSITYPERCENT=0.005194 AND MS2PROD=formula(C9H3O5):TOLERANCEPPM=10:INTENSITYPERCENT=0.000981:EXCLUDED AND MS2PROD=formula(C9H4O5):TOLERANCEPPM=10:INTENSITYPERCENT=0.000303 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C10H6O5):TOLERANCEPPM=10:INTENSITYPERCENT=0.005194 AND MS2PROD=formula(C9H3O5):TOLERANCEPPM=10:INTENSITYPERCENT=0.000981 AND MS2PROD=formula(C9H3O6):TOLERANCEPPM=10:INTENSITYPERCENT=0.000276:EXCLUDED</t>
-  </si>
-  <si>
-    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C3HO2):TOLERANCEPPM=10:INTENSITYPERCENT=0.964735:EXCLUDED AND MS2PROD=formula(C11HO):TOLERANCEPPM=10:INTENSITYPERCENT=0.103805 AND MS2PROD=formula(C11HO):TOLERANCEPPM=10:INTENSITYPERCENT=0.639490:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C3HO2):TOLERANCEPPM=10:INTENSITYPERCENT=0.964735 AND MS2PROD=formula(C3H3O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.004739:EXCLUDED AND MS2NL=formula(C24H16N2O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.500000:EXCLUDED</t>
-  </si>
-  <si>
-    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C7H11O6):TOLERANCEPPM=10:INTENSITYPERCENT=0.100112:EXCLUDED AND MS2NL=formula(C12H8N10S):TOLERANCEPPM=10:INTENSITYPERCENT=0.030334 AND MS2PROD=formula(C9H7O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.009130 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C7H11O6):TOLERANCEPPM=10:INTENSITYPERCENT=0.100112 AND MS2NL=formula(C2H6N6OS):TOLERANCEPPM=10:INTENSITYPERCENT=0.007571:EXCLUDED AND MS2NL=formula(C20H20O2P2):TOLERANCEPPM=10:INTENSITYPERCENT=0.002460 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C7H11O6):TOLERANCEPPM=10:INTENSITYPERCENT=0.100112 AND MS2NL=formula(C2H6N6OS):TOLERANCEPPM=10:INTENSITYPERCENT=0.007571</t>
-  </si>
-  <si>
-    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C8H16NO2):TOLERANCEPPM=10:INTENSITYPERCENT=0.103991:EXCLUDED AND MS2PROD=formula(C8H16NO3):TOLERANCEPPM=10:INTENSITYPERCENT=0.034541:EXCLUDED AND MS2NL=formula(C17H40N6S3):TOLERANCEPPM=10:INTENSITYPERCENT=0.011652 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C8H16NO2):TOLERANCEPPM=10:INTENSITYPERCENT=0.103991:EXCLUDED AND MS2PROD=formula(C8H16NO3):TOLERANCEPPM=10:INTENSITYPERCENT=0.034541 AND MS2PROD=formula(C5H10NO2):TOLERANCEPPM=10:INTENSITYPERCENT=0.007872 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C8H16NO2):TOLERANCEPPM=10:INTENSITYPERCENT=0.103991 AND MS2PROD=formula(C6H14NO):TOLERANCEPPM=10:INTENSITYPERCENT=0.000878:EXCLUDED AND MS2NL=formula(C49H52N4O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.087956 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C8H16NO2):TOLERANCEPPM=10:INTENSITYPERCENT=0.103991 AND MS2PROD=formula(C6H14NO):TOLERANCEPPM=10:INTENSITYPERCENT=0.000878 AND MS2NL=formula(C4H8):TOLERANCEPPM=10:INTENSITYPERCENT=0.005326:EXCLUDED</t>
+    <t>Iodine containing (ML-generated using ChemEcho) [ionization mode: negative]</t>
+  </si>
+  <si>
+    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(I):TOLERANCEPPM=10:INTENSITYPERCENT=0.000670:EXCLUDED AND MS2NL=formula(H3N5S4):TOLERANCEPPM=10:INTENSITYPERCENT=0.001966:EXCLUDED AND MS2NL=formula(C16H8O8S2):TOLERANCEPPM=10:INTENSITYPERCENT=0.103935 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(I):TOLERANCEPPM=10:INTENSITYPERCENT=0.000670:EXCLUDED AND MS2NL=formula(H3N5S4):TOLERANCEPPM=10:INTENSITYPERCENT=0.001966 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(I):TOLERANCEPPM=10:INTENSITYPERCENT=0.000670</t>
+  </si>
+  <si>
+    <t>*I</t>
+  </si>
+  <si>
+    <t>Amino acid glycosides from NP-Classifier (Note: most molecules of this class in training data are sulfur containing, so this will identify sulfur containing members of this class) (ML-generated using ChemEcho) [ionization mode: negative]</t>
+  </si>
+  <si>
+    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C6H11O9S):TOLERANCEPPM=10:INTENSITYPERCENT=0.020292:EXCLUDED AND MS2PROD=formula(C12H20NO9S2):TOLERANCEPPM=10:INTENSITYPERCENT=0.033670:EXCLUDED AND MS2PROD=formula(C10H11S2):TOLERANCEPPM=10:INTENSITYPERCENT=0.005387 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C6H11O9S):TOLERANCEPPM=10:INTENSITYPERCENT=0.020292:EXCLUDED AND MS2PROD=formula(C12H20NO9S2):TOLERANCEPPM=10:INTENSITYPERCENT=0.033670 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C6H11O9S):TOLERANCEPPM=10:INTENSITYPERCENT=0.020292</t>
+  </si>
+  <si>
+    <t>C1[C@H]([C@@H]([C@H]([C@@H]([C@H]1N)O[C@@H]2[C@@H]([C@H]([C@@H]([C@H](O2)CN)O)O)N)O[C@H]3[C@@H]([C@@H]([C@H](O3)CO)O[C@@H]4[C@@H]([C@H]([C@@H]([C@H](O4)CN)O)O)N)O)O)N</t>
+  </si>
+  <si>
+    <t>Bromine containing (ML-generated using ChemEcho) [ionization mode: negative]</t>
+  </si>
+  <si>
+    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(Br):TOLERANCEPPM=10:INTENSITYPERCENT=0.000252:EXCLUDED AND MS2PROD=formula(C2H3O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.000012:EXCLUDED AND MS2PROD=formula(C6H5BrN):TOLERANCEPPM=10:INTENSITYPERCENT=0.001112 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(Br):TOLERANCEPPM=10:INTENSITYPERCENT=0.000252 AND MS2NL=formula(C24H16ClN5):TOLERANCEPPM=10:INTENSITYPERCENT=0.172009:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(Br):TOLERANCEPPM=10:INTENSITYPERCENT=0.000252 AND MS2NL=formula(C24H16ClN5):TOLERANCEPPM=10:INTENSITYPERCENT=0.172009</t>
+  </si>
+  <si>
+    <t>*Br</t>
+  </si>
+  <si>
+    <t>Bromobenzene substructure (ML-generated using ChemEcho) [ionization mode: negative]</t>
+  </si>
+  <si>
+    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(Br):TOLERANCEPPM=10:INTENSITYPERCENT=0.000252:EXCLUDED AND MS2PROD=formula(C6H5BrN):TOLERANCEPPM=10:INTENSITYPERCENT=0.002684 AND MS2NL=formula(C11H14O4S):TOLERANCEPPM=10:INTENSITYPERCENT=0.035494:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(Br):TOLERANCEPPM=10:INTENSITYPERCENT=0.000252:EXCLUDED AND MS2PROD=formula(C6H5BrN):TOLERANCEPPM=10:INTENSITYPERCENT=0.002684 AND MS2NL=formula(C11H14O4S):TOLERANCEPPM=10:INTENSITYPERCENT=0.035494 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(Br):TOLERANCEPPM=10:INTENSITYPERCENT=0.000252 AND MS2NL=formula(C4H13ClN6):TOLERANCEPPM=10:INTENSITYPERCENT=0.008441:EXCLUDED AND MS2PROD=formula(C3H2BrN2):TOLERANCEPPM=10:INTENSITYPERCENT=0.017113:EXCLUDED</t>
+  </si>
+  <si>
+    <t>Brc1ccccc1</t>
+  </si>
+  <si>
+    <t>Sulfonyl functional group (ML-generated using ChemEcho) [ionization mode: negative]</t>
+  </si>
+  <si>
+    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(O3S):TOLERANCEPPM=10:INTENSITYPERCENT=0.000964:EXCLUDED AND MS2PROD=formula(HO4S):TOLERANCEPPM=10:INTENSITYPERCENT=0.001594:EXCLUDED AND MS2NL=formula(O3S):TOLERANCEPPM=10:INTENSITYPERCENT=0.000230 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(O3S):TOLERANCEPPM=10:INTENSITYPERCENT=0.000964:EXCLUDED AND MS2PROD=formula(HO4S):TOLERANCEPPM=10:INTENSITYPERCENT=0.001594 AND MS2PROD=formula(CH3O2S):TOLERANCEPPM=10:INTENSITYPERCENT=0.001297:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(O3S):TOLERANCEPPM=10:INTENSITYPERCENT=0.000964 AND MS2PROD=formula(C6H6NO2S):TOLERANCEPPM=10:INTENSITYPERCENT=0.000129:EXCLUDED AND MS2PROD=formula(C7H5N2O):TOLERANCEPPM=10:INTENSITYPERCENT=0.006722:EXCLUDED</t>
+  </si>
+  <si>
+    <t>OS(=O)=O</t>
+  </si>
+  <si>
+    <t>Sulfonic acid functional group ('O=S(=O)(O)*1') (ML-generated using ChemEcho) [ionization mode: negative]</t>
+  </si>
+  <si>
+    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(O3S):TOLERANCEPPM=10:INTENSITYPERCENT=0.000147:EXCLUDED AND MS2PROD=formula(HO4S):TOLERANCEPPM=10:INTENSITYPERCENT=0.001632:EXCLUDED AND MS2NL=formula(O3S):TOLERANCEPPM=10:INTENSITYPERCENT=0.000230 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(O3S):TOLERANCEPPM=10:INTENSITYPERCENT=0.000147:EXCLUDED AND MS2PROD=formula(HO4S):TOLERANCEPPM=10:INTENSITYPERCENT=0.001632 AND MS2PROD=formula(CH3O2S):TOLERANCEPPM=10:INTENSITYPERCENT=0.001297:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(O3S):TOLERANCEPPM=10:INTENSITYPERCENT=0.000147 AND MS2PROD=formula(NO2S):TOLERANCEPPM=10:INTENSITYPERCENT=0.030087:EXCLUDED AND MS2PROD=formula(C8H6N):TOLERANCEPPM=10:INTENSITYPERCENT=0.003508:EXCLUDED</t>
+  </si>
+  <si>
+    <t>Phosphate functional group (ML-generated using ChemEcho) [ionization mode: negative]</t>
+  </si>
+  <si>
+    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(O3P):TOLERANCEPPM=10:INTENSITYPERCENT=0.000194:EXCLUDED AND MS2PROD=formula(C18H33O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.000632:EXCLUDED AND MS2PROD=formula(HO6P2):TOLERANCEPPM=10:INTENSITYPERCENT=0.001348 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(O3P):TOLERANCEPPM=10:INTENSITYPERCENT=0.000194:EXCLUDED AND MS2PROD=formula(C18H33O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.000632 AND MS2PROD=formula(C8H13O):TOLERANCEPPM=10:INTENSITYPERCENT=0.000356:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(O3P):TOLERANCEPPM=10:INTENSITYPERCENT=0.000194 AND MS2PROD=formula(HO3P):TOLERANCEPPM=10:INTENSITYPERCENT=0.000154:EXCLUDED AND MS2PROD=formula(C3H5NO3P):TOLERANCEPPM=10:INTENSITYPERCENT=0.002065:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(O3P):TOLERANCEPPM=10:INTENSITYPERCENT=0.000194 AND MS2PROD=formula(HO3P):TOLERANCEPPM=10:INTENSITYPERCENT=0.000154 AND MS2NL=formula(C7H14N6S):TOLERANCEPPM=10:INTENSITYPERCENT=0.183040</t>
+  </si>
+  <si>
+    <t>OP(=O)(O)O</t>
+  </si>
+  <si>
+    <t>Anhydrohexitol substructure (ML-generated using ChemEcho) [ionization mode: negative]</t>
+  </si>
+  <si>
+    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C4H5O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.000030:EXCLUDED AND MS2NL=formula(C7H14S2):TOLERANCEPPM=10:INTENSITYPERCENT=0.002481:EXCLUDED AND MS2NL=formula(C8H16O2S2):TOLERANCEPPM=10:INTENSITYPERCENT=0.000027 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C4H5O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.000030:EXCLUDED AND MS2NL=formula(C7H14S2):TOLERANCEPPM=10:INTENSITYPERCENT=0.002481 AND MS2PROD=formula(C12H13O):TOLERANCEPPM=10:INTENSITYPERCENT=0.000533:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C4H5O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.000030 AND MS2NL=formula(CH2O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.000514:EXCLUDED AND MS2NL=formula(C2H8O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.010681:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C4H5O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.000030 AND MS2NL=formula(CH2O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.000514 AND MS2PROD=formula(C6H9O5):TOLERANCEPPM=10:INTENSITYPERCENT=0.000256</t>
+  </si>
+  <si>
+    <t>OCC1OCC(O)C(O)C1O</t>
+  </si>
+  <si>
+    <t>Substituted tetrahydropyran ring substructure (ML-generated using ChemEcho) [ionization mode: negative]</t>
+  </si>
+  <si>
+    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C4H5O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.000017:EXCLUDED AND MS2NL=formula(C7H14S2):TOLERANCEPPM=10:INTENSITYPERCENT=0.001513:EXCLUDED AND MS2NL=formula(C8H16O2S2):TOLERANCEPPM=10:INTENSITYPERCENT=0.000033 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C4H5O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.000017:EXCLUDED AND MS2NL=formula(C7H14S2):TOLERANCEPPM=10:INTENSITYPERCENT=0.001513 AND MS2PROD=formula(C13H13O):TOLERANCEPPM=10:INTENSITYPERCENT=0.000351:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C4H5O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.000017 AND MS2NL=formula(C2H8O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.010681:EXCLUDED AND MS2NL=formula(CH2O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.000469:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C4H5O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.000017 AND MS2NL=formula(C2H8O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.010681:EXCLUDED AND MS2NL=formula(CH2O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.000469 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C4H5O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.000017 AND MS2NL=formula(C2H8O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.010681 AND MS2PROD=formula(C6H7O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.006415</t>
+  </si>
+  <si>
+    <t>*[CH]1O[CH](*)[CH](*)[CH](*)[CH]1*</t>
+  </si>
+  <si>
+    <t>1,5-Anhydro-l-rhamnitol substructure (ML-generated using ChemEcho) [ionization mode: negative]</t>
+  </si>
+  <si>
+    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C4H5O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.000028:EXCLUDED AND MS2NL=formula(C7H14S2):TOLERANCEPPM=10:INTENSITYPERCENT=0.001513:EXCLUDED AND MS2PROD=formula(C15H9O6):TOLERANCEPPM=10:INTENSITYPERCENT=0.000009 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C4H5O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.000028:EXCLUDED AND MS2NL=formula(C7H14S2):TOLERANCEPPM=10:INTENSITYPERCENT=0.001513 AND MS2PROD=formula(C12H13O):TOLERANCEPPM=10:INTENSITYPERCENT=0.000327:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C4H5O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.000028 AND MS2NL=formula(C2H6O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.002790:EXCLUDED AND MS2PROD=formula(C4H6NO2):TOLERANCEPPM=10:INTENSITYPERCENT=0.001570:EXCLUDED</t>
+  </si>
+  <si>
+    <t>CC1OCC(O)C(O)C1O</t>
+  </si>
+  <si>
+    <t>Tetrahydropyran ring substructure (ML-generated using ChemEcho) [ionization mode: negative]</t>
+  </si>
+  <si>
+    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C4H5O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.000028:EXCLUDED AND MS2NL=formula(C7H14S2):TOLERANCEPPM=10:INTENSITYPERCENT=0.000016:EXCLUDED AND MS2NL=formula(C8H16O2S2):TOLERANCEPPM=10:INTENSITYPERCENT=0.000026 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C4H5O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.000028:EXCLUDED AND MS2NL=formula(C7H14S2):TOLERANCEPPM=10:INTENSITYPERCENT=0.000016 AND MS2NL=formula(C7H14S2):TOLERANCEPPM=10:INTENSITYPERCENT=0.005705:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C4H5O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.000028:EXCLUDED AND MS2NL=formula(C7H14S2):TOLERANCEPPM=10:INTENSITYPERCENT=0.000016 AND MS2NL=formula(C7H14S2):TOLERANCEPPM=10:INTENSITYPERCENT=0.005705 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C4H5O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.000028 AND MS2NL=formula(CH6O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.004072:EXCLUDED AND MS2NL=formula(CH2O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.000977:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C4H5O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.000028 AND MS2NL=formula(CH6O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.004072 AND MS2PROD=formula(C5H3O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.015062</t>
+  </si>
+  <si>
+    <t>Pyran substructure ([#6]1-[#6]-[#6]-[#8]-[#6]-[#6]-1) (ML-generated using ChemEcho) [ionization mode: negative]</t>
+  </si>
+  <si>
+    <t>Fucitol-like substructure (ML-generated using ChemEcho) [ionization mode: negative]</t>
+  </si>
+  <si>
+    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C4H5O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.000028:EXCLUDED AND MS2NL=formula(C7H14S2):TOLERANCEPPM=10:INTENSITYPERCENT=0.000011:EXCLUDED AND MS2PROD=formula(C15H9O6):TOLERANCEPPM=10:INTENSITYPERCENT=0.000009 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C4H5O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.000028:EXCLUDED AND MS2NL=formula(C7H14S2):TOLERANCEPPM=10:INTENSITYPERCENT=0.000011 AND MS2PROD=formula(C12H13O):TOLERANCEPPM=10:INTENSITYPERCENT=0.000493:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C4H5O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.000028 AND MS2PROD=formula(C4H4NO):TOLERANCEPPM=10:INTENSITYPERCENT=0.000055:EXCLUDED AND MS2NL=formula(C3H6S2):TOLERANCEPPM=10:INTENSITYPERCENT=0.001698:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C4H5O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.000028 AND MS2PROD=formula(C4H4NO):TOLERANCEPPM=10:INTENSITYPERCENT=0.000055 AND MS2PROD=formula(C4H6NO2):TOLERANCEPPM=10:INTENSITYPERCENT=0.000162:EXCLUDED</t>
+  </si>
+  <si>
+    <t>CC(O)C(O)C(O)C(O)CO</t>
+  </si>
+  <si>
+    <t>1-deoxy-ribitol substructure (ML-generated using ChemEcho) [ionization mode: negative]</t>
+  </si>
+  <si>
+    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C4H5O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.000028:EXCLUDED AND MS2NL=formula(C7H14S2):TOLERANCEPPM=10:INTENSITYPERCENT=0.000016:EXCLUDED AND MS2NL=formula(C8H16O2S2):TOLERANCEPPM=10:INTENSITYPERCENT=0.000034 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C4H5O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.000028:EXCLUDED AND MS2NL=formula(C7H14S2):TOLERANCEPPM=10:INTENSITYPERCENT=0.000016 AND MS2NL=formula(C7H4N4):TOLERANCEPPM=10:INTENSITYPERCENT=0.000214:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C4H5O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.000028 AND MS2NL=formula(CH2O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.003238:EXCLUDED AND MS2NL=formula(C5H2N4):TOLERANCEPPM=10:INTENSITYPERCENT=0.014586:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C4H5O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.000028 AND MS2NL=formula(CH2O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.003238 AND MS2PROD=formula(C2H3O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.014657</t>
+  </si>
+  <si>
+    <t>CC(O)C(O)C(O)CO</t>
+  </si>
+  <si>
+    <t>1,6-Dideoxy-l-mannitol substructure (ML-generated using ChemEcho) [ionization mode: negative]</t>
+  </si>
+  <si>
+    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C4H5O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.000028:EXCLUDED AND MS2NL=formula(C7H14S2):TOLERANCEPPM=10:INTENSITYPERCENT=0.000016:EXCLUDED AND MS2NL=formula(C8H16O2S2):TOLERANCEPPM=10:INTENSITYPERCENT=0.000026 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C4H5O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.000028:EXCLUDED AND MS2NL=formula(C7H14S2):TOLERANCEPPM=10:INTENSITYPERCENT=0.000016 AND MS2NL=formula(C6H4N4):TOLERANCEPPM=10:INTENSITYPERCENT=0.000106:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C4H5O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.000028 AND MS2PROD=formula(C5H6NO3):TOLERANCEPPM=10:INTENSITYPERCENT=0.000351:EXCLUDED AND MS2NL=formula(CH6O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.060889:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C4H5O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.000028 AND MS2PROD=formula(C5H6NO3):TOLERANCEPPM=10:INTENSITYPERCENT=0.000351 AND MS2NL=formula(C56H60O3P2S):TOLERANCEPPM=10:INTENSITYPERCENT=0.019989</t>
+  </si>
+  <si>
+    <t>CC(O)C(O)C(O)C(C)O</t>
+  </si>
+  <si>
+    <t>Acrylic acid substructure (ML-generated using ChemEcho) [ionization mode: negative]</t>
+  </si>
+  <si>
+    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C9H7O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.014781:EXCLUDED AND MS2PROD=formula(C9H7O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.006300:EXCLUDED AND MS2PROD=formula(C10H9O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.011654 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C9H7O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.014781:EXCLUDED AND MS2PROD=formula(C9H7O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.006300 AND MS2PROD=formula(C9H5O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.008282 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C9H7O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.014781 AND MS2PROD=formula(C9H5O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.017147:EXCLUDED AND MS2PROD=formula(C2H3O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.004128 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C9H7O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.014781 AND MS2PROD=formula(C9H5O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.017147 AND MS2PROD=formula(C10H7O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.005694:EXCLUDED</t>
+  </si>
+  <si>
+    <t>*[CH]=[CH]C(=O)O*</t>
+  </si>
+  <si>
+    <t>Sulfone functional group (ML-generated using ChemEcho) [ionization mode: negative]</t>
+  </si>
+  <si>
+    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(O2S):TOLERANCEPPM=10:INTENSITYPERCENT=0.000097:EXCLUDED AND MS2PROD=formula(O3S):TOLERANCEPPM=10:INTENSITYPERCENT=0.000076:EXCLUDED AND MS2PROD=formula(NO2S):TOLERANCEPPM=10:INTENSITYPERCENT=0.000268 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(O2S):TOLERANCEPPM=10:INTENSITYPERCENT=0.000097:EXCLUDED AND MS2PROD=formula(O3S):TOLERANCEPPM=10:INTENSITYPERCENT=0.000076 AND MS2NL=formula(C21H20NO4PS):TOLERANCEPPM=10:INTENSITYPERCENT=0.002710:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(O2S):TOLERANCEPPM=10:INTENSITYPERCENT=0.000097 AND MS2PROD=formula(C2H4NS):TOLERANCEPPM=10:INTENSITYPERCENT=0.013412:EXCLUDED AND MS2NL=formula(C4H7NO2):TOLERANCEPPM=10:INTENSITYPERCENT=0.045108:EXCLUDED</t>
+  </si>
+  <si>
+    <t>S(*)(=O)=O</t>
+  </si>
+  <si>
+    <t>Sulfonamide functional group (ML-generated using ChemEcho) [ionization mode: negative]</t>
+  </si>
+  <si>
+    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(O2S):TOLERANCEPPM=10:INTENSITYPERCENT=0.000079:EXCLUDED AND MS2PROD=formula(NO2S):TOLERANCEPPM=10:INTENSITYPERCENT=0.000234 AND MS2NL=formula(C4H8O3S):TOLERANCEPPM=10:INTENSITYPERCENT=0.032571:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(O2S):TOLERANCEPPM=10:INTENSITYPERCENT=0.000079 AND MS2PROD=formula(O3S):TOLERANCEPPM=10:INTENSITYPERCENT=0.419958:EXCLUDED AND MS2PROD=formula(CHCl2):TOLERANCEPPM=10:INTENSITYPERCENT=0.001348:EXCLUDED</t>
+  </si>
+  <si>
+    <t>NS(=O)=O</t>
+  </si>
+  <si>
+    <t>Sulfinamide functional group (ML-generated using ChemEcho) [ionization mode: negative]</t>
+  </si>
+  <si>
+    <t>NS=O</t>
+  </si>
+  <si>
+    <t>1-Methoxy-2-propanol substructure (ML-generated using ChemEcho) [ionization mode: negative]</t>
+  </si>
+  <si>
+    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C4H5O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.000030:EXCLUDED AND MS2NL=formula(C7H14S2):TOLERANCEPPM=10:INTENSITYPERCENT=0.000016:EXCLUDED AND MS2NL=formula(C8H16O2S2):TOLERANCEPPM=10:INTENSITYPERCENT=0.000026 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C4H5O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.000030:EXCLUDED AND MS2NL=formula(C7H14S2):TOLERANCEPPM=10:INTENSITYPERCENT=0.000016 AND MS2NL=formula(C7H14S2):TOLERANCEPPM=10:INTENSITYPERCENT=0.005971:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C4H5O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.000030:EXCLUDED AND MS2NL=formula(C7H14S2):TOLERANCEPPM=10:INTENSITYPERCENT=0.000016 AND MS2NL=formula(C7H14S2):TOLERANCEPPM=10:INTENSITYPERCENT=0.005971 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C4H5O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.000030 AND MS2NL=formula(C2H8O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.009271:EXCLUDED AND MS2NL=formula(CH2O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.002690:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C4H5O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.000030 AND MS2NL=formula(C2H8O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.009271 AND MS2PROD=formula(C4H5O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.070475</t>
+  </si>
+  <si>
+    <t>COCC(C)O</t>
+  </si>
+  <si>
+    <t>Glycerophospholipids from NP-Classifier (ML-generated using ChemEcho) [ionization mode: negative]</t>
+  </si>
+  <si>
+    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C18H33O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.000565:EXCLUDED AND MS2PROD=formula(C3H6O5P):TOLERANCEPPM=10:INTENSITYPERCENT=0.000145:EXCLUDED AND MS2PROD=formula(C9H8O5):TOLERANCEPPM=10:INTENSITYPERCENT=0.000918 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C18H33O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.000565:EXCLUDED AND MS2PROD=formula(C3H6O5P):TOLERANCEPPM=10:INTENSITYPERCENT=0.000145 AND MS2PROD=formula(C5H8O7P):TOLERANCEPPM=10:INTENSITYPERCENT=0.000765:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C18H33O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.000565 AND MS2PROD=formula(C10H9O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.000049:EXCLUDED AND MS2PROD=formula(C16H31N3O):TOLERANCEPPM=10:INTENSITYPERCENT=0.000937:EXCLUDED</t>
+  </si>
+  <si>
+    <t>3 Fluorine containing PFAS fragment (ML-generated using ChemEcho) [ionization mode: negative]</t>
+  </si>
+  <si>
+    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C3F7):TOLERANCEPPM=10:INTENSITYPERCENT=0.001762:EXCLUDED AND MS2PROD=formula(C2H3O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.000012:EXCLUDED AND MS2PROD=formula(FO3S):TOLERANCEPPM=10:INTENSITYPERCENT=0.013824 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C3F7):TOLERANCEPPM=10:INTENSITYPERCENT=0.001762 AND MS2NL=formula(C2H2N2O6):TOLERANCEPPM=10:INTENSITYPERCENT=0.076847:EXCLUDED</t>
+  </si>
+  <si>
+    <t>Thioether with methyl group (ML-generated using ChemEcho) [ionization mode: negative]</t>
+  </si>
+  <si>
+    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(CH3O2S):TOLERANCEPPM=10:INTENSITYPERCENT=0.000611:EXCLUDED AND MS2PROD=formula(C5H10NO2S):TOLERANCEPPM=10:INTENSITYPERCENT=0.001517:EXCLUDED AND MS2PROD=formula(CH3S):TOLERANCEPPM=10:INTENSITYPERCENT=0.000401 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(CH3O2S):TOLERANCEPPM=10:INTENSITYPERCENT=0.000611:EXCLUDED AND MS2PROD=formula(C5H10NO2S):TOLERANCEPPM=10:INTENSITYPERCENT=0.001517 AND MS2PROD=formula(O2S):TOLERANCEPPM=10:INTENSITYPERCENT=0.000341:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(CH3O2S):TOLERANCEPPM=10:INTENSITYPERCENT=0.000611 AND MS2PROD=formula(C8H4F3N2):TOLERANCEPPM=10:INTENSITYPERCENT=0.039573:EXCLUDED AND MS2PROD=formula(C12H13N2):TOLERANCEPPM=10:INTENSITYPERCENT=0.079169:EXCLUDED</t>
+  </si>
+  <si>
+    <t>*S[CH3]</t>
+  </si>
+  <si>
+    <t>Linear thioether with two alkyl groups (ML-generated using ChemEcho) [ionization mode: negative]</t>
+  </si>
+  <si>
+    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C2H4NS):TOLERANCEPPM=10:INTENSITYPERCENT=0.000541:EXCLUDED AND MS2PROD=formula(C2H3OS):TOLERANCEPPM=10:INTENSITYPERCENT=0.000670:EXCLUDED AND MS2PROD=formula(C22H6N3O4S):TOLERANCEPPM=10:INTENSITYPERCENT=0.001493 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C2H4NS):TOLERANCEPPM=10:INTENSITYPERCENT=0.000541:EXCLUDED AND MS2PROD=formula(C2H3OS):TOLERANCEPPM=10:INTENSITYPERCENT=0.000670 AND MS2PROD=formula(C4H6NO):TOLERANCEPPM=10:INTENSITYPERCENT=0.030310:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C2H4NS):TOLERANCEPPM=10:INTENSITYPERCENT=0.000541 AND MS2NL=formula(C3H5NOS):TOLERANCEPPM=10:INTENSITYPERCENT=0.008761:EXCLUDED AND MS2PROD=formula(HS2):TOLERANCEPPM=10:INTENSITYPERCENT=0.000466:EXCLUDED</t>
+  </si>
+  <si>
+    <t>CCSCC</t>
+  </si>
+  <si>
+    <t>Adenosine diphosphate derivatives (ML-generated using ChemEcho) [ionization mode: positive]</t>
+  </si>
+  <si>
+    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C24H12O6S):TOLERANCEPPM=10:INTENSITYPERCENT=0.038530:EXCLUDED AND MS2NL=formula(C29H23NO8S3):TOLERANCEPPM=10:INTENSITYPERCENT=0.042135:EXCLUDED AND MS2PROD=formula(C12H20N2O9P2):TOLERANCEPPM=10:INTENSITYPERCENT=0.004757 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C24H12O6S):TOLERANCEPPM=10:INTENSITYPERCENT=0.038530:EXCLUDED AND MS2NL=formula(C29H23NO8S3):TOLERANCEPPM=10:INTENSITYPERCENT=0.042135 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C24H12O6S):TOLERANCEPPM=10:INTENSITYPERCENT=0.038530 AND MS2PROD=formula(C18H17NO7):TOLERANCEPPM=10:INTENSITYPERCENT=0.001370:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C24H12O6S):TOLERANCEPPM=10:INTENSITYPERCENT=0.038530 AND MS2PROD=formula(C18H17NO7):TOLERANCEPPM=10:INTENSITYPERCENT=0.001370 AND MS2PROD=formula(C9H20O4PS):TOLERANCEPPM=10:INTENSITYPERCENT=0.001483</t>
+  </si>
+  <si>
+    <t>CC(O)CCOP(=O)(O)OP(=O)(O)OCC1OC(N2:C:N:C3:C(N):N:C:N:C:3:2)C(O)C1O</t>
+  </si>
+  <si>
+    <t>Steranes (CC12C3CC(*1)C4(C)C(CCC4*1)C3C(*1)C(*1)C1CC(*1)CC2*1) (ML-generated using ChemEcho) [ionization mode: positive]</t>
+  </si>
+  <si>
+    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C24H33):TOLERANCEPPM=10:INTENSITYPERCENT=0.004383:EXCLUDED AND MS2PROD=formula(C24H33O):TOLERANCEPPM=10:INTENSITYPERCENT=0.011434:EXCLUDED AND MS2NL=formula(C18H39N4O2P):TOLERANCEPPM=10:INTENSITYPERCENT=0.141631 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C24H33):TOLERANCEPPM=10:INTENSITYPERCENT=0.004383:EXCLUDED AND MS2PROD=formula(C24H33O):TOLERANCEPPM=10:INTENSITYPERCENT=0.011434 AND MS2NL=formula(C20H42N2OS2):TOLERANCEPPM=10:INTENSITYPERCENT=0.025868 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C24H33):TOLERANCEPPM=10:INTENSITYPERCENT=0.004383 AND MS2NL=formula(C12H22O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.002323:EXCLUDED AND MS2PROD=formula(C15H23O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.007041:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C24H33):TOLERANCEPPM=10:INTENSITYPERCENT=0.004383 AND MS2NL=formula(C12H22O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.002323 AND MS2PROD=formula(C23H35):TOLERANCEPPM=10:INTENSITYPERCENT=0.006007</t>
+  </si>
+  <si>
+    <t>m-Dichlorobenzene substructure (ML-generated using ChemEcho) [ionization mode: positive]</t>
+  </si>
+  <si>
+    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C7H5Cl2):TOLERANCEPPM=10:INTENSITYPERCENT=0.000182:EXCLUDED AND MS2PROD=formula(C7H3Cl2O):TOLERANCEPPM=10:INTENSITYPERCENT=0.000347:EXCLUDED AND MS2PROD=formula(C7H4Cl2N):TOLERANCEPPM=10:INTENSITYPERCENT=0.000224 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C7H5Cl2):TOLERANCEPPM=10:INTENSITYPERCENT=0.000182:EXCLUDED AND MS2PROD=formula(C7H3Cl2O):TOLERANCEPPM=10:INTENSITYPERCENT=0.000347 AND MS2PROD=formula(C13H5ClO2):TOLERANCEPPM=10:INTENSITYPERCENT=0.000474:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C7H5Cl2):TOLERANCEPPM=10:INTENSITYPERCENT=0.000182 AND MS2NL=formula(C3H4FN5OS):TOLERANCEPPM=10:INTENSITYPERCENT=0.000144:EXCLUDED AND MS2PROD=formula(C11H10Cl2N):TOLERANCEPPM=10:INTENSITYPERCENT=0.000382:EXCLUDED</t>
+  </si>
+  <si>
+    <t>Clc1cccc(Cl)c1</t>
+  </si>
+  <si>
+    <t>Para di-substituted benzene ring with sulfonyl group (ML-generated using ChemEcho) [ionization mode: positive]</t>
+  </si>
+  <si>
+    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C6H6NO2S):TOLERANCEPPM=10:INTENSITYPERCENT=0.000206:EXCLUDED AND MS2PROD=formula(C7H7O2S):TOLERANCEPPM=10:INTENSITYPERCENT=0.000117 AND MS2PROD=formula(C8H9O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.000343:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C6H6NO2S):TOLERANCEPPM=10:INTENSITYPERCENT=0.000206 AND MS2PROD=formula(C4H5S):TOLERANCEPPM=10:INTENSITYPERCENT=0.000776:EXCLUDED AND MS2PROD=formula(C5H4NS):TOLERANCEPPM=10:INTENSITYPERCENT=0.000160:EXCLUDED</t>
+  </si>
+  <si>
+    <t>*c1[cH][cH]c(S(*)(=O)=O)[cH][cH]1</t>
+  </si>
+  <si>
+    <t>Bromobenzene substructure (ML-generated using ChemEcho) [ionization mode: positive]</t>
+  </si>
+  <si>
+    <t>QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(Br):TOLERANCEPPM=10:INTENSITYPERCENT=0.000088:EXCLUDED AND MS2PROD=formula(C7H4BrO):TOLERANCEPPM=10:INTENSITYPERCENT=0.000075:EXCLUDED AND MS2PROD=formula(C7H6Br):TOLERANCEPPM=10:INTENSITYPERCENT=0.000084 ||| QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(Br):TOLERANCEPPM=10:INTENSITYPERCENT=0.000088:EXCLUDED AND MS2PROD=formula(C7H4BrO):TOLERANCEPPM=10:INTENSITYPERCENT=0.000075 AND MS2PROD=formula(C5H2BrO2):TOLERANCEPPM=10:INTENSITYPERCENT=0.029616:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(Br):TOLERANCEPPM=10:INTENSITYPERCENT=0.000088 AND MS2PROD=formula(C5H3BrN):TOLERANCEPPM=10:INTENSITYPERCENT=0.000825:EXCLUDED AND MS2PROD=formula(CH2Br):TOLERANCEPPM=10:INTENSITYPERCENT=0.003789:EXCLUDED</t>
+  </si>
+  <si>
+    <t>Para di-substituted benzene ring with sulfide group (ML-generated using ChemEcho) [ionization mode: positive]</t>
+  </si>
+  <si>
+    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C6H6NO2S):TOLERANCEPPM=10:INTENSITYPERCENT=0.000207:EXCLUDED AND MS2PROD=formula(C7H7O2S):TOLERANCEPPM=10:INTENSITYPERCENT=0.000117 AND MS2PROD=formula(C8H8NO2S):TOLERANCEPPM=10:INTENSITYPERCENT=0.000249:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C6H6NO2S):TOLERANCEPPM=10:INTENSITYPERCENT=0.000207 AND MS2PROD=formula(C5H6NO2):TOLERANCEPPM=10:INTENSITYPERCENT=0.000021:EXCLUDED AND MS2PROD=formula(C6H4NOS):TOLERANCEPPM=10:INTENSITYPERCENT=0.003499:EXCLUDED</t>
+  </si>
+  <si>
+    <t>*Sc1[cH][cH]c(*)[cH][cH]1</t>
+  </si>
+  <si>
+    <t>Bromine containing (ML-generated using ChemEcho) [ionization mode: positive]</t>
+  </si>
+  <si>
+    <t>QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(Br):TOLERANCEPPM=10:INTENSITYPERCENT=0.000088:EXCLUDED AND MS2PROD=formula(C7H4BrO):TOLERANCEPPM=10:INTENSITYPERCENT=0.000075:EXCLUDED AND MS2PROD=formula(C7H6Br):TOLERANCEPPM=10:INTENSITYPERCENT=0.000188 ||| QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(Br):TOLERANCEPPM=10:INTENSITYPERCENT=0.000088:EXCLUDED AND MS2PROD=formula(C7H4BrO):TOLERANCEPPM=10:INTENSITYPERCENT=0.000075 ||| QUERY scaninfo(MS2DATA) WHERE MS2NL=formula(Br):TOLERANCEPPM=10:INTENSITYPERCENT=0.000088</t>
+  </si>
+  <si>
+    <t>Substituted benzene ring with trifluoromethyl group (ML-generated using ChemEcho) [ionization mode: positive]</t>
+  </si>
+  <si>
+    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C8H6F3):TOLERANCEPPM=10:INTENSITYPERCENT=0.000118:EXCLUDED AND MS2PROD=formula(C7H4F3):TOLERANCEPPM=10:INTENSITYPERCENT=0.000047:EXCLUDED AND MS2NL=formula(C7H6F3N):TOLERANCEPPM=10:INTENSITYPERCENT=0.000526 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C8H6F3):TOLERANCEPPM=10:INTENSITYPERCENT=0.000118:EXCLUDED AND MS2PROD=formula(C7H4F3):TOLERANCEPPM=10:INTENSITYPERCENT=0.000047 AND MS2PROD=formula(C8H6F2N):TOLERANCEPPM=10:INTENSITYPERCENT=0.008827:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C8H6F3):TOLERANCEPPM=10:INTENSITYPERCENT=0.000118 AND MS2NL=formula(C8H22O7S):TOLERANCEPPM=10:INTENSITYPERCENT=0.000811:EXCLUDED AND MS2NL=formula(C7H14N6OS2):TOLERANCEPPM=10:INTENSITYPERCENT=0.164059:EXCLUDED</t>
+  </si>
+  <si>
+    <t>FC(F)(F)c1ccccc1</t>
+  </si>
+  <si>
+    <t>Linear polyamine (ML-generated using ChemEcho) [ionization mode: positive]</t>
+  </si>
+  <si>
+    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C4H10N6O):TOLERANCEPPM=10:INTENSITYPERCENT=0.025896:EXCLUDED AND MS2PROD=formula(C12H22N5O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.006763:EXCLUDED AND MS2PROD=formula(C8H15N7O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.003751 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C4H10N6O):TOLERANCEPPM=10:INTENSITYPERCENT=0.025896:EXCLUDED AND MS2PROD=formula(C12H22N5O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.006763 AND MS2NL=formula(C10H25N5O4S):TOLERANCEPPM=10:INTENSITYPERCENT=0.012265:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C4H10N6O):TOLERANCEPPM=10:INTENSITYPERCENT=0.025896 AND MS2PROD=formula(C3H7N5):TOLERANCEPPM=10:INTENSITYPERCENT=0.011096:EXCLUDED AND MS2PROD=formula(C4H11N5):TOLERANCEPPM=10:INTENSITYPERCENT=0.009165 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C4H10N6O):TOLERANCEPPM=10:INTENSITYPERCENT=0.025896 AND MS2PROD=formula(C3H7N5):TOLERANCEPPM=10:INTENSITYPERCENT=0.011096 AND MS2PROD=formula(C8H10N):TOLERANCEPPM=10:INTENSITYPERCENT=0.027362:EXCLUDED</t>
+  </si>
+  <si>
+    <t>NCNCCCCN</t>
+  </si>
+  <si>
+    <t>1,6-Dideoxy-l-mannitol substructure (ML-generated using ChemEcho) [ionization mode: positive]</t>
+  </si>
+  <si>
+    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C4H5O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.004240:EXCLUDED AND MS2NL=formula(C6H10O5):TOLERANCEPPM=10:INTENSITYPERCENT=0.052214:EXCLUDED AND MS2PROD=formula(C6H12NaO6):TOLERANCEPPM=10:INTENSITYPERCENT=0.000726 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C4H5O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.004240:EXCLUDED AND MS2NL=formula(C6H10O5):TOLERANCEPPM=10:INTENSITYPERCENT=0.052214 AND MS2NL=formula(C5H10O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.002833:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C4H5O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.004240 AND MS2PROD=formula(C4H6NO):TOLERANCEPPM=10:INTENSITYPERCENT=0.000199:EXCLUDED AND MS2PROD=formula(C6H9O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.000314:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C4H5O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.004240 AND MS2PROD=formula(C4H6NO):TOLERANCEPPM=10:INTENSITYPERCENT=0.000199:EXCLUDED AND MS2PROD=formula(C6H9O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.000314</t>
+  </si>
+  <si>
+    <t>Chlorobenzene substructure (ML-generated using ChemEcho) [ionization mode: positive]</t>
+  </si>
+  <si>
+    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C7H6Cl):TOLERANCEPPM=10:INTENSITYPERCENT=0.000058:EXCLUDED AND MS2PROD=formula(C5H4Cl):TOLERANCEPPM=10:INTENSITYPERCENT=0.000009:EXCLUDED AND MS2PROD=formula(C7H4ClO):TOLERANCEPPM=10:INTENSITYPERCENT=0.000007 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C7H6Cl):TOLERANCEPPM=10:INTENSITYPERCENT=0.000058:EXCLUDED AND MS2PROD=formula(C5H4Cl):TOLERANCEPPM=10:INTENSITYPERCENT=0.000009 AND MS2PROD=formula(C6H5ClN):TOLERANCEPPM=10:INTENSITYPERCENT=0.767068:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C7H6Cl):TOLERANCEPPM=10:INTENSITYPERCENT=0.000058 AND MS2PROD=formula(C7OS):TOLERANCEPPM=10:INTENSITYPERCENT=0.000683:EXCLUDED AND MS2NL=formula(C2H2N4O3S):TOLERANCEPPM=10:INTENSITYPERCENT=0.016569:EXCLUDED</t>
+  </si>
+  <si>
+    <t>Clc1ccccc1</t>
+  </si>
+  <si>
+    <t>Phenylalanine derivative (ML-generated using ChemEcho) [ionization mode: positive]</t>
+  </si>
+  <si>
+    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C8H10N):TOLERANCEPPM=10:INTENSITYPERCENT=0.029464:EXCLUDED AND MS2NL=formula(C10H11NO3):TOLERANCEPPM=10:INTENSITYPERCENT=0.054138:EXCLUDED AND MS2PROD=formula(C10H16N4O):TOLERANCEPPM=10:INTENSITYPERCENT=0.010879 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C8H10N):TOLERANCEPPM=10:INTENSITYPERCENT=0.029464:EXCLUDED AND MS2NL=formula(C10H11NO3):TOLERANCEPPM=10:INTENSITYPERCENT=0.054138 AND MS2PROD=formula(C8H10N):TOLERANCEPPM=10:INTENSITYPERCENT=0.000112 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C8H10N):TOLERANCEPPM=10:INTENSITYPERCENT=0.029464 AND MS2PROD=formula(C9H12NO2):TOLERANCEPPM=10:INTENSITYPERCENT=0.002754 AND MS2PROD=formula(C3H8N):TOLERANCEPPM=10:INTENSITYPERCENT=0.000233:EXCLUDED</t>
+  </si>
+  <si>
+    <t>*[NH][CH]([CH2]c1[cH][cH][cH][cH][cH]1)C(*)=O</t>
+  </si>
+  <si>
+    <t>1,5-Anhydro-l-rhamnitol substructure (ML-generated using ChemEcho) [ionization mode: positive]</t>
+  </si>
+  <si>
+    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C4H5O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.004677:EXCLUDED AND MS2NL=formula(C6H10O5):TOLERANCEPPM=10:INTENSITYPERCENT=0.052214:EXCLUDED AND MS2PROD=formula(C6H9O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.000123 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C4H5O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.004677:EXCLUDED AND MS2NL=formula(C6H10O5):TOLERANCEPPM=10:INTENSITYPERCENT=0.052214 AND MS2NL=formula(C5H10O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.002833:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C4H5O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.004677 AND MS2PROD=formula(C6H9O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.000020:EXCLUDED AND MS2PROD=formula(C4H6NO):TOLERANCEPPM=10:INTENSITYPERCENT=0.000065:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C4H5O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.004677 AND MS2PROD=formula(C6H9O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.000020 AND MS2NL=formula(CH6O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.000441:EXCLUDED</t>
+  </si>
+  <si>
+    <t>Fucitol-like substructure (ML-generated using ChemEcho) [ionization mode: positive]</t>
+  </si>
+  <si>
+    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C4H5O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.004665:EXCLUDED AND MS2NL=formula(C6H10O5):TOLERANCEPPM=10:INTENSITYPERCENT=0.039612:EXCLUDED AND MS2PROD=formula(C6H12NaO6):TOLERANCEPPM=10:INTENSITYPERCENT=0.001040 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C4H5O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.004665:EXCLUDED AND MS2NL=formula(C6H10O5):TOLERANCEPPM=10:INTENSITYPERCENT=0.039612 AND MS2NL=formula(C5H10O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.002833:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C4H5O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.004665 AND MS2PROD=formula(C4H6NO):TOLERANCEPPM=10:INTENSITYPERCENT=0.000487:EXCLUDED AND MS2PROD=formula(C6H9O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.000004:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C4H5O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.004665 AND MS2PROD=formula(C4H6NO):TOLERANCEPPM=10:INTENSITYPERCENT=0.000487:EXCLUDED AND MS2PROD=formula(C6H9O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.000004 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C4H5O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.004665 AND MS2PROD=formula(C4H6NO):TOLERANCEPPM=10:INTENSITYPERCENT=0.000487 AND MS2PROD=formula(C10H7NO6):TOLERANCEPPM=10:INTENSITYPERCENT=0.000009</t>
+  </si>
+  <si>
+    <t>Purine nucleoside (ML-generated using ChemEcho) [ionization mode: positive]</t>
+  </si>
+  <si>
+    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C5H6N5):TOLERANCEPPM=10:INTENSITYPERCENT=0.717742:EXCLUDED AND MS2PROD=formula(C10H13N5O6P):TOLERANCEPPM=10:INTENSITYPERCENT=0.000400 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C5H6N5):TOLERANCEPPM=10:INTENSITYPERCENT=0.717742 AND MS2PROD=formula(C5H9):TOLERANCEPPM=10:INTENSITYPERCENT=0.008881:EXCLUDED AND MS2NL=formula(C3H4N3O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.398980:EXCLUDED</t>
+  </si>
+  <si>
+    <t>C1:N:C:C2:N:C:N(C3CCCO3):C:2:N:1</t>
+  </si>
+  <si>
+    <t>Fluorobenzene substructure (ML-generated using ChemEcho) [ionization mode: positive]</t>
+  </si>
+  <si>
+    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C7H6F):TOLERANCEPPM=10:INTENSITYPERCENT=0.000017:EXCLUDED AND MS2PROD=formula(C2H6FN3):TOLERANCEPPM=10:INTENSITYPERCENT=0.000116 AND MS2PROD=formula(C9H8F3N2):TOLERANCEPPM=10:INTENSITYPERCENT=0.000079:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C7H6F):TOLERANCEPPM=10:INTENSITYPERCENT=0.000017 AND MS2PROD=formula(C8H6F3):TOLERANCEPPM=10:INTENSITYPERCENT=0.012087:EXCLUDED AND MS2NL=formula(N6O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.000287:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C7H6F):TOLERANCEPPM=10:INTENSITYPERCENT=0.000017 AND MS2PROD=formula(C8H6F3):TOLERANCEPPM=10:INTENSITYPERCENT=0.012087 AND MS2NL=formula(C19H20F4NO4P):TOLERANCEPPM=10:INTENSITYPERCENT=0.001574</t>
+  </si>
+  <si>
+    <t>Fc1ccccc1</t>
+  </si>
+  <si>
+    <t>Butylamine-like (ML-generated using ChemEcho) [ionization mode: positive]</t>
+  </si>
+  <si>
+    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C5H10N3):TOLERANCEPPM=10:INTENSITYPERCENT=0.314554:EXCLUDED AND MS2PROD=formula(C5H7N3Na):TOLERANCEPPM=10:INTENSITYPERCENT=0.072079:EXCLUDED AND MS2NL=formula(C23H40O5):TOLERANCEPPM=10:INTENSITYPERCENT=0.351204 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C5H10N3):TOLERANCEPPM=10:INTENSITYPERCENT=0.314554:EXCLUDED AND MS2PROD=formula(C5H7N3Na):TOLERANCEPPM=10:INTENSITYPERCENT=0.072079 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C5H10N3):TOLERANCEPPM=10:INTENSITYPERCENT=0.314554 AND MS2PROD=formula(C5H7N2):TOLERANCEPPM=10:INTENSITYPERCENT=0.389185</t>
+  </si>
+  <si>
+    <t>C:CCCN</t>
+  </si>
+  <si>
+    <t>Hexyl group  (ML-generated using ChemEcho) [ionization mode: positive]</t>
+  </si>
+  <si>
+    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C3H8O5P):TOLERANCEPPM=10:INTENSITYPERCENT=0.022662:EXCLUDED AND MS2PROD=formula(C3H7NaO5P):TOLERANCEPPM=10:INTENSITYPERCENT=0.001964:EXCLUDED AND MS2PROD=formula(C8H11O11P2):TOLERANCEPPM=10:INTENSITYPERCENT=0.001107 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C3H8O5P):TOLERANCEPPM=10:INTENSITYPERCENT=0.022662:EXCLUDED AND MS2PROD=formula(C3H7NaO5P):TOLERANCEPPM=10:INTENSITYPERCENT=0.001964 AND MS2NL=formula(C6H6NO3P):TOLERANCEPPM=10:INTENSITYPERCENT=0.033988:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C3H8O5P):TOLERANCEPPM=10:INTENSITYPERCENT=0.022662 AND MS2NL=formula(C10H7O6P):TOLERANCEPPM=10:INTENSITYPERCENT=0.001754:EXCLUDED AND MS2NL=formula(C28H34O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.389993:EXCLUDED</t>
+  </si>
+  <si>
+    <t>CCCCCC</t>
+  </si>
+  <si>
+    <t>Benzenesulfonamide group (ML-generated using ChemEcho) [ionization mode: positive]</t>
+  </si>
+  <si>
+    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C6H6NO2S):TOLERANCEPPM=10:INTENSITYPERCENT=0.000207:EXCLUDED AND MS2PROD=formula(C8H13):TOLERANCEPPM=10:INTENSITYPERCENT=0.000001:EXCLUDED AND MS2PROD=formula(C7H7O2S):TOLERANCEPPM=10:INTENSITYPERCENT=0.000037 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C6H6NO2S):TOLERANCEPPM=10:INTENSITYPERCENT=0.000207:EXCLUDED AND MS2PROD=formula(C8H13):TOLERANCEPPM=10:INTENSITYPERCENT=0.000001 AND MS2PROD=formula(C7H7N2):TOLERANCEPPM=10:INTENSITYPERCENT=0.001758 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C6H6NO2S):TOLERANCEPPM=10:INTENSITYPERCENT=0.000207 AND MS2PROD=formula(C5H6NO2):TOLERANCEPPM=10:INTENSITYPERCENT=0.000021:EXCLUDED AND MS2NL=formula(H2O3S):TOLERANCEPPM=10:INTENSITYPERCENT=0.001198:EXCLUDED</t>
+  </si>
+  <si>
+    <t>NS(=O)(=O)c1ccccc1</t>
+  </si>
+  <si>
+    <t>Anhydrohexitol substructure (ML-generated using ChemEcho) [ionization mode: positive]</t>
+  </si>
+  <si>
+    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C4H5O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.004448:EXCLUDED AND MS2NL=formula(C6H10O5):TOLERANCEPPM=10:INTENSITYPERCENT=0.039780:EXCLUDED AND MS2PROD=formula(C6H12NaO6):TOLERANCEPPM=10:INTENSITYPERCENT=0.000726 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C4H5O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.004448:EXCLUDED AND MS2NL=formula(C6H10O5):TOLERANCEPPM=10:INTENSITYPERCENT=0.039780 AND MS2NL=formula(C5H10O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.002833:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C4H5O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.004448 AND MS2PROD=formula(C6H9O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.000020:EXCLUDED AND MS2PROD=formula(C5H5O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.001706 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C4H5O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.004448 AND MS2PROD=formula(C6H9O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.000020 AND MS2NL=formula(CH6O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.000441:EXCLUDED</t>
+  </si>
+  <si>
+    <t>Fluorine containing (ML-generated using ChemEcho) [ionization mode: positive]</t>
+  </si>
+  <si>
+    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C7H6F):TOLERANCEPPM=10:INTENSITYPERCENT=0.000025:EXCLUDED AND MS2PROD=formula(H4FN3):TOLERANCEPPM=10:INTENSITYPERCENT=0.000046 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C7H6F):TOLERANCEPPM=10:INTENSITYPERCENT=0.000025</t>
+  </si>
+  <si>
+    <t>*F</t>
+  </si>
+  <si>
+    <t>1-deoxy-ribitol substructure (ML-generated using ChemEcho) [ionization mode: positive]</t>
+  </si>
+  <si>
+    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C4H5O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.003711:EXCLUDED AND MS2NL=formula(C6H10O5):TOLERANCEPPM=10:INTENSITYPERCENT=0.039554:EXCLUDED AND MS2PROD=formula(C6H12NaO6):TOLERANCEPPM=10:INTENSITYPERCENT=0.000469 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C4H5O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.003711:EXCLUDED AND MS2NL=formula(C6H10O5):TOLERANCEPPM=10:INTENSITYPERCENT=0.039554 AND MS2NL=formula(C5H10O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.002833:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C4H5O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.003711 AND MS2PROD=formula(C5H5O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.002344:EXCLUDED AND MS2PROD=formula(C6H9O3):TOLERANCEPPM=10:INTENSITYPERCENT=0.002869 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C4H5O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.003711 AND MS2PROD=formula(C5H5O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.002344 AND MS2PROD=formula(C13H13O):TOLERANCEPPM=10:INTENSITYPERCENT=0.001033:EXCLUDED</t>
+  </si>
+  <si>
+    <t>Chlorine containing (ML-generated using ChemEcho) [ionization mode: positive]</t>
+  </si>
+  <si>
+    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C7H6Cl):TOLERANCEPPM=10:INTENSITYPERCENT=0.000027:EXCLUDED AND MS2PROD=formula(C5H4Cl):TOLERANCEPPM=10:INTENSITYPERCENT=0.000036 AND MS2NL=formula(C10H11N7O3S2):TOLERANCEPPM=10:INTENSITYPERCENT=0.000231:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C7H6Cl):TOLERANCEPPM=10:INTENSITYPERCENT=0.000027:EXCLUDED AND MS2PROD=formula(C5H4Cl):TOLERANCEPPM=10:INTENSITYPERCENT=0.000036 AND MS2NL=formula(C10H11N7O3S2):TOLERANCEPPM=10:INTENSITYPERCENT=0.000231 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C7H6Cl):TOLERANCEPPM=10:INTENSITYPERCENT=0.000027 AND MS2NL=formula(C19H10F2N2O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.000446:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C7H6Cl):TOLERANCEPPM=10:INTENSITYPERCENT=0.000027 AND MS2NL=formula(C19H10F2N2O4):TOLERANCEPPM=10:INTENSITYPERCENT=0.000446</t>
+  </si>
+  <si>
+    <t>*Cl</t>
+  </si>
+  <si>
+    <t>Indole substructure (C1=CC=C2C(=C1)NC=C2*1) (ML-generated using ChemEcho) [ionization mode: positive]</t>
+  </si>
+  <si>
+    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C9H8N):TOLERANCEPPM=10:INTENSITYPERCENT=0.705920:EXCLUDED AND MS2PROD=formula(C10H11N2):TOLERANCEPPM=10:INTENSITYPERCENT=0.018431 AND MS2PROD=formula(C11H10NO2):TOLERANCEPPM=10:INTENSITYPERCENT=0.000206 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C9H8N):TOLERANCEPPM=10:INTENSITYPERCENT=0.705920 AND MS2NL=formula(C2H7N):TOLERANCEPPM=10:INTENSITYPERCENT=0.391152:EXCLUDED AND MS2PROD=formula(C8H7):TOLERANCEPPM=10:INTENSITYPERCENT=0.015723 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C9H8N):TOLERANCEPPM=10:INTENSITYPERCENT=0.705920 AND MS2NL=formula(C2H7N):TOLERANCEPPM=10:INTENSITYPERCENT=0.391152</t>
+  </si>
+  <si>
+    <t>Steranes ([#6]1-[#6]-[#6]-[#6]2-[#6](-[#6]-1)-[#6]-[#6]-[#6]1-[#6]3-[#6]-[#6]-[#6]-[#6]-3-[#6]-[#6]-[#6]-2-1) (ML-generated using ChemEcho) [ionization mode: positive]</t>
+  </si>
+  <si>
+    <t>QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C24H33):TOLERANCEPPM=10:INTENSITYPERCENT=0.005570:EXCLUDED AND MS2PROD=formula(C24H33O):TOLERANCEPPM=10:INTENSITYPERCENT=0.014301:EXCLUDED AND MS2PROD=formula(C8H7O7):TOLERANCEPPM=10:INTENSITYPERCENT=0.162655 ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C24H33):TOLERANCEPPM=10:INTENSITYPERCENT=0.005570:EXCLUDED AND MS2PROD=formula(C24H33O):TOLERANCEPPM=10:INTENSITYPERCENT=0.014301 AND MS2PROD=formula(C10H13O):TOLERANCEPPM=10:INTENSITYPERCENT=0.008067:EXCLUDED ||| QUERY scaninfo(MS2DATA) WHERE MS2PROD=formula(C24H33):TOLERANCEPPM=10:INTENSITYPERCENT=0.005570 AND MS2NL=formula(C7H12O2):TOLERANCEPPM=10:INTENSITYPERCENT=0.002961:EXCLUDED AND MS2PROD=formula(C10H13):TOLERANCEPPM=10:INTENSITYPERCENT=0.045014:EXCLUDED</t>
   </si>
 </sst>
 </file>
@@ -908,7 +908,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
@@ -917,6 +917,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1137,9 +1138,9 @@
   </sheetPr>
   <dimension ref="A1:F88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C88" sqref="C88"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A60" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F38" sqref="A38:F87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1167,7 +1168,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>166</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -1685,16 +1686,16 @@
         <v>13</v>
       </c>
       <c r="B38" t="s">
-        <v>114</v>
+        <v>123</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>203</v>
+        <v>124</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="F38" t="s">
-        <v>167</v>
+        <v>114</v>
+      </c>
+      <c r="F38" s="8" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1702,16 +1703,16 @@
         <v>13</v>
       </c>
       <c r="B39" t="s">
-        <v>115</v>
+        <v>126</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>204</v>
+        <v>127</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="F39" t="s">
-        <v>168</v>
+        <v>114</v>
+      </c>
+      <c r="F39" s="8" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1719,16 +1720,16 @@
         <v>13</v>
       </c>
       <c r="B40" t="s">
-        <v>116</v>
+        <v>129</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>205</v>
+        <v>130</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="F40" t="s">
-        <v>169</v>
+        <v>114</v>
+      </c>
+      <c r="F40" s="8" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1736,16 +1737,16 @@
         <v>13</v>
       </c>
       <c r="B41" t="s">
-        <v>117</v>
+        <v>132</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>206</v>
+        <v>133</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="F41" t="s">
-        <v>170</v>
+        <v>114</v>
+      </c>
+      <c r="F41" s="8" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1753,16 +1754,16 @@
         <v>13</v>
       </c>
       <c r="B42" t="s">
-        <v>118</v>
+        <v>135</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>207</v>
+        <v>136</v>
       </c>
       <c r="D42" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="F42" t="s">
-        <v>171</v>
+        <v>114</v>
+      </c>
+      <c r="F42" s="8" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1770,16 +1771,16 @@
         <v>13</v>
       </c>
       <c r="B43" t="s">
-        <v>119</v>
+        <v>138</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>208</v>
+        <v>139</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="F43" t="s">
-        <v>172</v>
+        <v>114</v>
+      </c>
+      <c r="F43" s="8" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1787,16 +1788,16 @@
         <v>13</v>
       </c>
       <c r="B44" t="s">
-        <v>120</v>
+        <v>138</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>209</v>
+        <v>139</v>
       </c>
       <c r="D44" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="F44" t="s">
-        <v>173</v>
+        <v>114</v>
+      </c>
+      <c r="F44" s="8" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1804,16 +1805,16 @@
         <v>13</v>
       </c>
       <c r="B45" t="s">
-        <v>121</v>
+        <v>140</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>210</v>
+        <v>141</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="F45" t="s">
-        <v>174</v>
+        <v>114</v>
+      </c>
+      <c r="F45" s="8" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1821,16 +1822,16 @@
         <v>13</v>
       </c>
       <c r="B46" t="s">
-        <v>122</v>
+        <v>143</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>211</v>
+        <v>144</v>
       </c>
       <c r="D46" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="F46" t="s">
-        <v>175</v>
+        <v>114</v>
+      </c>
+      <c r="F46" s="8" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1838,16 +1839,16 @@
         <v>13</v>
       </c>
       <c r="B47" t="s">
-        <v>123</v>
+        <v>146</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>212</v>
+        <v>147</v>
       </c>
       <c r="D47" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="F47" t="s">
-        <v>176</v>
+        <v>114</v>
+      </c>
+      <c r="F47" s="8" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1855,16 +1856,16 @@
         <v>13</v>
       </c>
       <c r="B48" t="s">
-        <v>124</v>
+        <v>149</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>213</v>
+        <v>150</v>
       </c>
       <c r="D48" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="F48" t="s">
-        <v>177</v>
+        <v>114</v>
+      </c>
+      <c r="F48" s="8" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1872,16 +1873,16 @@
         <v>13</v>
       </c>
       <c r="B49" t="s">
-        <v>125</v>
+        <v>152</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>214</v>
+        <v>153</v>
       </c>
       <c r="D49" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="F49" t="s">
-        <v>173</v>
+        <v>114</v>
+      </c>
+      <c r="F49" s="8" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1889,16 +1890,16 @@
         <v>13</v>
       </c>
       <c r="B50" t="s">
-        <v>126</v>
+        <v>154</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>215</v>
+        <v>153</v>
       </c>
       <c r="D50" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="F50" t="s">
-        <v>175</v>
+        <v>114</v>
+      </c>
+      <c r="F50" s="8" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1906,16 +1907,16 @@
         <v>13</v>
       </c>
       <c r="B51" t="s">
-        <v>127</v>
+        <v>155</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>216</v>
+        <v>156</v>
       </c>
       <c r="D51" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="F51" t="s">
-        <v>172</v>
+        <v>114</v>
+      </c>
+      <c r="F51" s="8" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1923,16 +1924,16 @@
         <v>13</v>
       </c>
       <c r="B52" t="s">
-        <v>128</v>
+        <v>158</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>217</v>
+        <v>159</v>
       </c>
       <c r="D52" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="F52" t="s">
-        <v>167</v>
+        <v>114</v>
+      </c>
+      <c r="F52" s="8" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1940,16 +1941,16 @@
         <v>13</v>
       </c>
       <c r="B53" t="s">
-        <v>129</v>
+        <v>161</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>218</v>
+        <v>162</v>
       </c>
       <c r="D53" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="F53" t="s">
-        <v>167</v>
+        <v>114</v>
+      </c>
+      <c r="F53" s="8" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1957,16 +1958,16 @@
         <v>13</v>
       </c>
       <c r="B54" t="s">
-        <v>130</v>
+        <v>164</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>219</v>
+        <v>165</v>
       </c>
       <c r="D54" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="F54" t="s">
-        <v>178</v>
+        <v>114</v>
+      </c>
+      <c r="F54" s="8" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1974,16 +1975,16 @@
         <v>13</v>
       </c>
       <c r="B55" t="s">
-        <v>131</v>
+        <v>167</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>220</v>
+        <v>168</v>
       </c>
       <c r="D55" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="F55" t="s">
-        <v>179</v>
+        <v>114</v>
+      </c>
+      <c r="F55" s="8" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1991,16 +1992,16 @@
         <v>13</v>
       </c>
       <c r="B56" t="s">
-        <v>132</v>
+        <v>170</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>221</v>
+        <v>171</v>
       </c>
       <c r="D56" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="F56" t="s">
-        <v>180</v>
+        <v>114</v>
+      </c>
+      <c r="F56" s="8" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2008,16 +2009,16 @@
         <v>13</v>
       </c>
       <c r="B57" t="s">
-        <v>133</v>
+        <v>173</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>222</v>
+        <v>171</v>
       </c>
       <c r="D57" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="F57" t="s">
-        <v>181</v>
+        <v>114</v>
+      </c>
+      <c r="F57" s="8" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2025,16 +2026,16 @@
         <v>13</v>
       </c>
       <c r="B58" t="s">
-        <v>134</v>
+        <v>175</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>223</v>
+        <v>176</v>
       </c>
       <c r="D58" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="F58" t="s">
-        <v>178</v>
+        <v>114</v>
+      </c>
+      <c r="F58" s="8" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2042,16 +2043,16 @@
         <v>13</v>
       </c>
       <c r="B59" t="s">
-        <v>135</v>
+        <v>178</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>224</v>
+        <v>179</v>
       </c>
       <c r="D59" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="F59" t="s">
-        <v>182</v>
+        <v>114</v>
+      </c>
+      <c r="F59" s="8" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="60" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2059,16 +2060,16 @@
         <v>13</v>
       </c>
       <c r="B60" t="s">
-        <v>136</v>
+        <v>180</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>225</v>
+        <v>181</v>
       </c>
       <c r="D60" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="F60" t="s">
-        <v>170</v>
+        <v>114</v>
+      </c>
+      <c r="F60" s="8" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="61" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2076,16 +2077,16 @@
         <v>13</v>
       </c>
       <c r="B61" t="s">
-        <v>137</v>
+        <v>182</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>226</v>
+        <v>183</v>
       </c>
       <c r="D61" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="F61" t="s">
-        <v>183</v>
+        <v>114</v>
+      </c>
+      <c r="F61" s="8" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="62" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2093,16 +2094,16 @@
         <v>13</v>
       </c>
       <c r="B62" t="s">
-        <v>138</v>
+        <v>185</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>227</v>
+        <v>186</v>
       </c>
       <c r="D62" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="F62" t="s">
-        <v>170</v>
+        <v>114</v>
+      </c>
+      <c r="F62" s="8" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2110,16 +2111,16 @@
         <v>13</v>
       </c>
       <c r="B63" t="s">
-        <v>139</v>
+        <v>188</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>228</v>
+        <v>189</v>
       </c>
       <c r="D63" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="F63" t="s">
-        <v>184</v>
+        <v>114</v>
+      </c>
+      <c r="F63" s="8" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="64" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2127,16 +2128,16 @@
         <v>13</v>
       </c>
       <c r="B64" t="s">
-        <v>140</v>
+        <v>191</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>229</v>
+        <v>192</v>
       </c>
       <c r="D64" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="F64" t="s">
-        <v>185</v>
+        <v>114</v>
+      </c>
+      <c r="F64" s="8" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="65" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2144,16 +2145,16 @@
         <v>13</v>
       </c>
       <c r="B65" t="s">
-        <v>141</v>
+        <v>193</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>230</v>
+        <v>194</v>
       </c>
       <c r="D65" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="F65" t="s">
-        <v>179</v>
+        <v>114</v>
+      </c>
+      <c r="F65" s="8" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="66" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2161,16 +2162,16 @@
         <v>13</v>
       </c>
       <c r="B66" t="s">
-        <v>142</v>
+        <v>196</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>231</v>
+        <v>197</v>
       </c>
       <c r="D66" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="F66" t="s">
-        <v>186</v>
+        <v>114</v>
+      </c>
+      <c r="F66" s="8" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="67" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2178,16 +2179,16 @@
         <v>13</v>
       </c>
       <c r="B67" t="s">
-        <v>143</v>
+        <v>199</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>232</v>
+        <v>200</v>
       </c>
       <c r="D67" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="F67" t="s">
-        <v>187</v>
+        <v>114</v>
+      </c>
+      <c r="F67" s="8" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="68" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2195,16 +2196,16 @@
         <v>13</v>
       </c>
       <c r="B68" t="s">
-        <v>144</v>
+        <v>201</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>233</v>
+        <v>202</v>
       </c>
       <c r="D68" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="F68" t="s">
-        <v>181</v>
+        <v>114</v>
+      </c>
+      <c r="F68" s="8" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2212,16 +2213,16 @@
         <v>13</v>
       </c>
       <c r="B69" t="s">
-        <v>145</v>
+        <v>204</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>234</v>
+        <v>205</v>
       </c>
       <c r="D69" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="F69" t="s">
-        <v>188</v>
+        <v>114</v>
+      </c>
+      <c r="F69" s="8" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="70" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2229,16 +2230,16 @@
         <v>13</v>
       </c>
       <c r="B70" t="s">
-        <v>146</v>
+        <v>206</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>235</v>
+        <v>207</v>
       </c>
       <c r="D70" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="F70" t="s">
-        <v>170</v>
+        <v>114</v>
+      </c>
+      <c r="F70" s="8" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="71" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2246,16 +2247,16 @@
         <v>13</v>
       </c>
       <c r="B71" t="s">
-        <v>147</v>
+        <v>209</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>236</v>
+        <v>210</v>
       </c>
       <c r="D71" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="F71" t="s">
-        <v>189</v>
+        <v>114</v>
+      </c>
+      <c r="F71" s="8" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="72" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2263,16 +2264,16 @@
         <v>13</v>
       </c>
       <c r="B72" t="s">
-        <v>148</v>
+        <v>212</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>237</v>
+        <v>213</v>
       </c>
       <c r="D72" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="F72" t="s">
-        <v>186</v>
+        <v>114</v>
+      </c>
+      <c r="F72" s="8" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="73" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2280,16 +2281,16 @@
         <v>13</v>
       </c>
       <c r="B73" t="s">
-        <v>149</v>
+        <v>214</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>238</v>
+        <v>215</v>
       </c>
       <c r="D73" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="F73" t="s">
-        <v>190</v>
+        <v>114</v>
+      </c>
+      <c r="F73" s="8" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="74" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2297,16 +2298,16 @@
         <v>13</v>
       </c>
       <c r="B74" t="s">
-        <v>150</v>
+        <v>217</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>239</v>
+        <v>218</v>
       </c>
       <c r="D74" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="F74" t="s">
-        <v>188</v>
+        <v>114</v>
+      </c>
+      <c r="F74" s="8" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="75" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2314,16 +2315,16 @@
         <v>13</v>
       </c>
       <c r="B75" t="s">
+        <v>220</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="D75" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="F75" s="8" t="s">
         <v>151</v>
-      </c>
-      <c r="C75" s="3" t="s">
-        <v>240</v>
-      </c>
-      <c r="D75" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="F75" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="76" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2331,16 +2332,16 @@
         <v>13</v>
       </c>
       <c r="B76" t="s">
-        <v>152</v>
+        <v>222</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>241</v>
+        <v>223</v>
       </c>
       <c r="D76" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="F76" t="s">
-        <v>192</v>
+        <v>114</v>
+      </c>
+      <c r="F76" s="8" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="77" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2348,16 +2349,16 @@
         <v>13</v>
       </c>
       <c r="B77" t="s">
-        <v>153</v>
+        <v>224</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>242</v>
+        <v>225</v>
       </c>
       <c r="D77" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="F77" t="s">
-        <v>193</v>
+        <v>114</v>
+      </c>
+      <c r="F77" s="8" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="78" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2365,16 +2366,16 @@
         <v>13</v>
       </c>
       <c r="B78" t="s">
-        <v>154</v>
+        <v>227</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>243</v>
+        <v>228</v>
       </c>
       <c r="D78" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="F78" t="s">
-        <v>177</v>
+        <v>114</v>
+      </c>
+      <c r="F78" s="8" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="79" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2382,16 +2383,16 @@
         <v>13</v>
       </c>
       <c r="B79" t="s">
-        <v>155</v>
+        <v>230</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>244</v>
+        <v>231</v>
       </c>
       <c r="D79" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="F79" t="s">
-        <v>194</v>
+        <v>114</v>
+      </c>
+      <c r="F79" s="8" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="80" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2399,16 +2400,16 @@
         <v>13</v>
       </c>
       <c r="B80" t="s">
-        <v>156</v>
+        <v>233</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>245</v>
+        <v>234</v>
       </c>
       <c r="D80" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="F80" t="s">
-        <v>195</v>
+        <v>114</v>
+      </c>
+      <c r="F80" s="8" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="81" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2416,16 +2417,16 @@
         <v>13</v>
       </c>
       <c r="B81" t="s">
-        <v>157</v>
+        <v>236</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>246</v>
+        <v>237</v>
       </c>
       <c r="D81" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="F81" t="s">
-        <v>196</v>
+        <v>114</v>
+      </c>
+      <c r="F81" s="8" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="82" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2433,16 +2434,16 @@
         <v>13</v>
       </c>
       <c r="B82" t="s">
-        <v>158</v>
+        <v>239</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="D82" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="F82" t="s">
-        <v>197</v>
+        <v>114</v>
+      </c>
+      <c r="F82" s="8" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="83" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2450,16 +2451,16 @@
         <v>13</v>
       </c>
       <c r="B83" t="s">
-        <v>159</v>
+        <v>241</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="D83" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="F83" t="s">
-        <v>198</v>
+        <v>114</v>
+      </c>
+      <c r="F83" s="8" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="84" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2467,16 +2468,16 @@
         <v>13</v>
       </c>
       <c r="B84" t="s">
+        <v>244</v>
+      </c>
+      <c r="C84" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="D84" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="F84" s="8" t="s">
         <v>160</v>
-      </c>
-      <c r="C84" s="3" t="s">
-        <v>249</v>
-      </c>
-      <c r="D84" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="F84" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="85" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2484,16 +2485,16 @@
         <v>13</v>
       </c>
       <c r="B85" t="s">
-        <v>161</v>
+        <v>246</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="D85" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="F85" t="s">
-        <v>183</v>
+        <v>114</v>
+      </c>
+      <c r="F85" s="8" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="86" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2501,16 +2502,16 @@
         <v>13</v>
       </c>
       <c r="B86" t="s">
-        <v>162</v>
+        <v>249</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D86" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="F86" t="s">
-        <v>200</v>
+        <v>114</v>
+      </c>
+      <c r="F86" s="8" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="87" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2518,34 +2519,23 @@
         <v>13</v>
       </c>
       <c r="B87" t="s">
-        <v>163</v>
+        <v>251</v>
       </c>
       <c r="C87" s="3" t="s">
         <v>252</v>
       </c>
       <c r="D87" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="F87" t="s">
-        <v>190</v>
+        <v>114</v>
+      </c>
+      <c r="F87" s="8" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="88" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B88" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="C88" s="3" t="s">
-        <v>202</v>
-      </c>
-      <c r="D88" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="F88" t="s">
-        <v>201</v>
-      </c>
+      <c r="A88" s="7"/>
+      <c r="B88" s="6"/>
+      <c r="C88" s="3"/>
+      <c r="D88" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>